<commit_message>
Fixes for issues caused by best fit. PostRaceEvents now passed around using PostRaceEventState objects (currently untested).
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="251">
   <si>
     <t>Key</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Age:</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>AMPERSAND</t>
@@ -621,6 +618,12 @@
     <t>Unideal Placements</t>
   </si>
   <si>
+    <t>REPEAT_CONFIRM</t>
+  </si>
+  <si>
+    <t>Are you sure you want to use the same crew line-up as the previous race?</t>
+  </si>
+  <si>
     <t>REQUIRED</t>
   </si>
   <si>
@@ -765,12 +768,6 @@
   <si>
     <t>Yes</t>
   </si>
-  <si>
-    <t>REPEAT_CONFIRM</t>
-  </si>
-  <si>
-    <t>Are you sure you want to use the same crew line-up as the previous race?</t>
-  </si>
 </sst>
 </file>
 
@@ -918,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -939,13 +936,13 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -966,10 +963,10 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -993,10 +990,10 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -1020,10 +1017,10 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1047,10 +1044,10 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1074,10 +1071,10 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1101,10 +1098,10 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1128,10 +1125,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1155,10 +1152,10 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
@@ -1182,7 +1179,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
@@ -1209,13 +1206,13 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1236,10 +1233,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
@@ -1263,10 +1260,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
@@ -1290,10 +1287,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
@@ -1317,10 +1314,10 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
@@ -1344,10 +1341,10 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
@@ -1371,10 +1368,10 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
@@ -1398,10 +1395,10 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -1425,10 +1422,10 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
@@ -1452,10 +1449,10 @@
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
@@ -1479,10 +1476,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -1506,10 +1503,10 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -1533,10 +1530,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
@@ -1560,10 +1557,10 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -1587,10 +1584,10 @@
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>5</v>
@@ -1614,10 +1611,10 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>5</v>
@@ -1641,10 +1638,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1668,10 +1665,10 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1695,13 +1692,13 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1722,13 +1719,13 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -1749,10 +1746,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1776,10 +1773,10 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1803,10 +1800,10 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1830,10 +1827,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
@@ -1843,24 +1840,24 @@
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
@@ -1884,10 +1881,10 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>5</v>
@@ -1897,24 +1894,24 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>5</v>
@@ -1938,10 +1935,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>5</v>
@@ -1965,10 +1962,10 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
@@ -1992,10 +1989,10 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>5</v>
@@ -2019,10 +2016,10 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>5</v>
@@ -2046,10 +2043,10 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>5</v>
@@ -2059,24 +2056,24 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>5</v>
@@ -2086,24 +2083,24 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>5</v>
@@ -2113,24 +2110,24 @@
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>5</v>
@@ -2154,10 +2151,10 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>5</v>
@@ -2167,24 +2164,24 @@
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>5</v>
@@ -2208,10 +2205,10 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>5</v>
@@ -2235,10 +2232,10 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>5</v>
@@ -2262,10 +2259,10 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -2289,10 +2286,10 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>5</v>
@@ -2316,10 +2313,10 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>5</v>
@@ -2329,24 +2326,24 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
@@ -2370,10 +2367,10 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
@@ -2383,24 +2380,24 @@
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>114</v>
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>5</v>
@@ -2410,24 +2407,24 @@
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
-      <c r="U58" s="4"/>
-      <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>5</v>
@@ -2450,11 +2447,11 @@
       <c r="W59" s="4"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" t="s">
-        <v>117</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>118</v>
+      <c r="A60" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -2464,24 +2461,24 @@
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -2491,24 +2488,24 @@
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
-      <c r="V61" s="4"/>
-      <c r="W61" s="4"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -2532,10 +2529,10 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>5</v>
@@ -2559,10 +2556,10 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
@@ -2586,10 +2583,10 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>5</v>
@@ -2613,10 +2610,10 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>5</v>
@@ -2640,10 +2637,10 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>5</v>
@@ -2653,27 +2650,27 @@
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
-      <c r="R67" s="3"/>
-      <c r="S67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1.0</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -2694,13 +2691,13 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>5</v>
+        <v>138</v>
+      </c>
+      <c r="C69" s="1">
+        <v>10.0</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -2721,13 +2718,13 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C70" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -2748,13 +2745,13 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C71" s="1">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -2775,13 +2772,13 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C72" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -2802,13 +2799,13 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C73" s="1">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -2829,13 +2826,13 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C74" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -2856,13 +2853,13 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C75" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -2883,13 +2880,13 @@
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C76" s="1">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -2910,13 +2907,13 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C77" s="1">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -2937,64 +2934,64 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="1">
-        <v>8.0</v>
+        <v>156</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4"/>
-      <c r="S78" s="4"/>
-      <c r="T78" s="4"/>
-      <c r="U78" s="4"/>
-      <c r="V78" s="4"/>
-      <c r="W78" s="4"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C79" s="1">
-        <v>9.0</v>
+        <v>158</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
-      <c r="S79" s="4"/>
-      <c r="T79" s="4"/>
-      <c r="U79" s="4"/>
-      <c r="V79" s="4"/>
-      <c r="W79" s="4"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>5</v>
@@ -3004,24 +3001,24 @@
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
-      <c r="Q80" s="3"/>
-      <c r="R80" s="3"/>
-      <c r="S80" s="3"/>
-      <c r="T80" s="3"/>
-      <c r="U80" s="3"/>
-      <c r="V80" s="3"/>
-      <c r="W80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>5</v>
@@ -3031,24 +3028,24 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="3"/>
-      <c r="P81" s="3"/>
-      <c r="Q81" s="3"/>
-      <c r="R81" s="3"/>
-      <c r="S81" s="3"/>
-      <c r="T81" s="3"/>
-      <c r="U81" s="3"/>
-      <c r="V81" s="3"/>
-      <c r="W81" s="3"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+      <c r="U81" s="4"/>
+      <c r="V81" s="4"/>
+      <c r="W81" s="4"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>5</v>
@@ -3072,10 +3069,10 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>5</v>
@@ -3085,27 +3082,27 @@
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-      <c r="R83" s="4"/>
-      <c r="S83" s="4"/>
-      <c r="T83" s="4"/>
-      <c r="U83" s="4"/>
-      <c r="V83" s="4"/>
-      <c r="W83" s="4"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3126,10 +3123,10 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>5</v>
@@ -3139,27 +3136,27 @@
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
-      <c r="N85" s="3"/>
-      <c r="O85" s="3"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
-      <c r="R85" s="3"/>
-      <c r="S85" s="3"/>
-      <c r="T85" s="3"/>
-      <c r="U85" s="3"/>
-      <c r="V85" s="3"/>
-      <c r="W85" s="3"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="4"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="4"/>
+      <c r="U85" s="4"/>
+      <c r="V85" s="4"/>
+      <c r="W85" s="4"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>170</v>
+        <v>65</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3180,10 +3177,10 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>5</v>
@@ -3207,13 +3204,13 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3234,13 +3231,13 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3261,10 +3258,10 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>5</v>
@@ -3274,27 +3271,27 @@
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
-      <c r="M90" s="4"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
-      <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-      <c r="S90" s="4"/>
-      <c r="T90" s="4"/>
-      <c r="U90" s="4"/>
-      <c r="V90" s="4"/>
-      <c r="W90" s="4"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>181</v>
+        <v>5</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3315,10 +3312,10 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>5</v>
@@ -3328,24 +3325,24 @@
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
-      <c r="Q92" s="3"/>
-      <c r="R92" s="3"/>
-      <c r="S92" s="3"/>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-      <c r="W92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="4"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+      <c r="U92" s="4"/>
+      <c r="V92" s="4"/>
+      <c r="W92" s="4"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>5</v>
@@ -3368,11 +3365,11 @@
       <c r="W93" s="4"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="1" t="s">
-        <v>186</v>
+      <c r="A94" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>5</v>
@@ -3395,11 +3392,11 @@
       <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="1" t="s">
-        <v>188</v>
+      <c r="A95" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>5</v>
@@ -3423,10 +3420,10 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="5" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>5</v>
@@ -3449,11 +3446,11 @@
       <c r="W96" s="4"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="5" t="s">
-        <v>192</v>
+      <c r="A97" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>5</v>
@@ -3463,24 +3460,24 @@
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
-      <c r="M97" s="4"/>
-      <c r="N97" s="4"/>
-      <c r="O97" s="4"/>
-      <c r="P97" s="4"/>
-      <c r="Q97" s="4"/>
-      <c r="R97" s="4"/>
-      <c r="S97" s="4"/>
-      <c r="T97" s="4"/>
-      <c r="U97" s="4"/>
-      <c r="V97" s="4"/>
-      <c r="W97" s="4"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
+      <c r="P97" s="3"/>
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="U97" s="3"/>
+      <c r="V97" s="3"/>
+      <c r="W97" s="3"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="5" t="s">
-        <v>194</v>
+      <c r="A98" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>5</v>
@@ -3504,10 +3501,10 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>5</v>
@@ -3517,24 +3514,24 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="T99" s="3"/>
-      <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
-      <c r="W99" s="3"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="4"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+      <c r="U99" s="4"/>
+      <c r="V99" s="4"/>
+      <c r="W99" s="4"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>5</v>
@@ -3558,10 +3555,10 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>5</v>
@@ -3571,24 +3568,24 @@
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="4"/>
-      <c r="R101" s="4"/>
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
-      <c r="U101" s="4"/>
-      <c r="V101" s="4"/>
-      <c r="W101" s="4"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>5</v>
@@ -3612,10 +3609,10 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>5</v>
@@ -3639,10 +3636,10 @@
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>5</v>
@@ -3666,10 +3663,10 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>5</v>
@@ -3692,11 +3689,11 @@
       <c r="W105" s="3"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>211</v>
+      <c r="A106" t="s">
+        <v>213</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -3719,11 +3716,11 @@
       <c r="W106" s="3"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" t="s">
-        <v>212</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>213</v>
+      <c r="A107" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -3733,24 +3730,24 @@
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+      <c r="V107" s="4"/>
+      <c r="W107" s="4"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>5</v>
@@ -3774,10 +3771,10 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>5</v>
@@ -3787,24 +3784,24 @@
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
-      <c r="M109" s="4"/>
-      <c r="N109" s="4"/>
-      <c r="O109" s="4"/>
-      <c r="P109" s="4"/>
-      <c r="Q109" s="4"/>
-      <c r="R109" s="4"/>
-      <c r="S109" s="4"/>
-      <c r="T109" s="4"/>
-      <c r="U109" s="4"/>
-      <c r="V109" s="4"/>
-      <c r="W109" s="4"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3"/>
+      <c r="T109" s="3"/>
+      <c r="U109" s="3"/>
+      <c r="V109" s="3"/>
+      <c r="W109" s="3"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>5</v>
@@ -3828,10 +3825,10 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>5</v>
@@ -3841,24 +3838,24 @@
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-      <c r="Q111" s="3"/>
-      <c r="R111" s="3"/>
-      <c r="S111" s="3"/>
-      <c r="T111" s="3"/>
-      <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
-      <c r="W111" s="3"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4"/>
+      <c r="V111" s="4"/>
+      <c r="W111" s="4"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
@@ -3882,10 +3879,10 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
@@ -3909,10 +3906,10 @@
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
@@ -3922,24 +3919,24 @@
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
-      <c r="R114" s="4"/>
-      <c r="S114" s="4"/>
-      <c r="T114" s="4"/>
-      <c r="U114" s="4"/>
-      <c r="V114" s="4"/>
-      <c r="W114" s="4"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="3"/>
+      <c r="T114" s="3"/>
+      <c r="U114" s="3"/>
+      <c r="V114" s="3"/>
+      <c r="W114" s="3"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>5</v>
@@ -3949,24 +3946,24 @@
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
-      <c r="M115" s="4"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
-      <c r="Q115" s="4"/>
-      <c r="R115" s="4"/>
-      <c r="S115" s="4"/>
-      <c r="T115" s="4"/>
-      <c r="U115" s="4"/>
-      <c r="V115" s="4"/>
-      <c r="W115" s="4"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="3"/>
+      <c r="T115" s="3"/>
+      <c r="U115" s="3"/>
+      <c r="V115" s="3"/>
+      <c r="W115" s="3"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>5</v>
@@ -3989,11 +3986,11 @@
       <c r="W116" s="3"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" s="1" t="s">
-        <v>230</v>
+      <c r="A117" t="s">
+        <v>235</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>5</v>
@@ -4017,10 +4014,10 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>5</v>
@@ -4030,24 +4027,24 @@
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3"/>
-      <c r="Q118" s="3"/>
-      <c r="R118" s="3"/>
-      <c r="S118" s="3"/>
-      <c r="T118" s="3"/>
-      <c r="U118" s="3"/>
-      <c r="V118" s="3"/>
-      <c r="W118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" t="s">
-        <v>234</v>
+      <c r="A119" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>5</v>
@@ -4057,24 +4054,24 @@
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
-      <c r="M119" s="3"/>
-      <c r="N119" s="3"/>
-      <c r="O119" s="3"/>
-      <c r="P119" s="3"/>
-      <c r="Q119" s="3"/>
-      <c r="R119" s="3"/>
-      <c r="S119" s="3"/>
-      <c r="T119" s="3"/>
-      <c r="U119" s="3"/>
-      <c r="V119" s="3"/>
-      <c r="W119" s="3"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="4"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+      <c r="U119" s="4"/>
+      <c r="V119" s="4"/>
+      <c r="W119" s="4"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>5</v>
@@ -4098,10 +4095,10 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>5</v>
@@ -4111,24 +4108,24 @@
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-      <c r="S121" s="4"/>
-      <c r="T121" s="4"/>
-      <c r="U121" s="4"/>
-      <c r="V121" s="4"/>
-      <c r="W121" s="4"/>
+      <c r="M121" s="3"/>
+      <c r="N121" s="3"/>
+      <c r="O121" s="3"/>
+      <c r="P121" s="3"/>
+      <c r="Q121" s="3"/>
+      <c r="R121" s="3"/>
+      <c r="S121" s="3"/>
+      <c r="T121" s="3"/>
+      <c r="U121" s="3"/>
+      <c r="V121" s="3"/>
+      <c r="W121" s="3"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>5</v>
@@ -4138,24 +4135,24 @@
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
-      <c r="M122" s="4"/>
-      <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
-      <c r="Q122" s="4"/>
-      <c r="R122" s="4"/>
-      <c r="S122" s="4"/>
-      <c r="T122" s="4"/>
-      <c r="U122" s="4"/>
-      <c r="V122" s="4"/>
-      <c r="W122" s="4"/>
+      <c r="M122" s="3"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="3"/>
+      <c r="P122" s="3"/>
+      <c r="Q122" s="3"/>
+      <c r="R122" s="3"/>
+      <c r="S122" s="3"/>
+      <c r="T122" s="3"/>
+      <c r="U122" s="3"/>
+      <c r="V122" s="3"/>
+      <c r="W122" s="3"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>5</v>
@@ -4165,24 +4162,24 @@
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
-      <c r="O123" s="3"/>
-      <c r="P123" s="3"/>
-      <c r="Q123" s="3"/>
-      <c r="R123" s="3"/>
-      <c r="S123" s="3"/>
-      <c r="T123" s="3"/>
-      <c r="U123" s="3"/>
-      <c r="V123" s="3"/>
-      <c r="W123" s="3"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="4"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+      <c r="U123" s="4"/>
+      <c r="V123" s="4"/>
+      <c r="W123" s="4"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>5</v>
@@ -4205,15 +4202,7 @@
       <c r="W124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B125" s="4"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
@@ -4232,42 +4221,26 @@
       <c r="W125" s="4"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B126" s="4"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
-      <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="3"/>
-      <c r="R126" s="3"/>
-      <c r="S126" s="3"/>
-      <c r="T126" s="3"/>
-      <c r="U126" s="3"/>
-      <c r="V126" s="3"/>
-      <c r="W126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="4"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+      <c r="U126" s="4"/>
+      <c r="V126" s="4"/>
+      <c r="W126" s="4"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="A127" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B127" s="4"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
@@ -4401,11 +4374,11 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="B134" s="4"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="3"/>
-      <c r="L134" s="3"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
       <c r="O134" s="4"/>
@@ -4420,11 +4393,11 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="B135" s="4"/>
-      <c r="H135" s="3"/>
-      <c r="I135" s="3"/>
-      <c r="J135" s="3"/>
-      <c r="K135" s="3"/>
-      <c r="L135" s="3"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
       <c r="O135" s="4"/>
@@ -4439,11 +4412,11 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="B136" s="4"/>
-      <c r="H136" s="3"/>
-      <c r="I136" s="3"/>
-      <c r="J136" s="3"/>
-      <c r="K136" s="3"/>
-      <c r="L136" s="3"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
       <c r="M136" s="4"/>
       <c r="N136" s="4"/>
       <c r="O136" s="4"/>
@@ -4742,7 +4715,13 @@
       <c r="W151" s="4"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="B152" s="4"/>
+      <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -4761,7 +4740,13 @@
       <c r="W152" s="4"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="B153" s="4"/>
+      <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
@@ -4780,7 +4765,13 @@
       <c r="W153" s="4"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="B154" s="4"/>
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -25898,81 +25889,6 @@
       <c r="V998" s="4"/>
       <c r="W998" s="4"/>
     </row>
-    <row r="999" ht="14.25" customHeight="1">
-      <c r="A999" s="3"/>
-      <c r="B999" s="3"/>
-      <c r="C999" s="4"/>
-      <c r="D999" s="4"/>
-      <c r="E999" s="4"/>
-      <c r="F999" s="4"/>
-      <c r="G999" s="4"/>
-      <c r="H999" s="4"/>
-      <c r="I999" s="4"/>
-      <c r="J999" s="4"/>
-      <c r="K999" s="4"/>
-      <c r="L999" s="4"/>
-      <c r="M999" s="4"/>
-      <c r="N999" s="4"/>
-      <c r="O999" s="4"/>
-      <c r="P999" s="4"/>
-      <c r="Q999" s="4"/>
-      <c r="R999" s="4"/>
-      <c r="S999" s="4"/>
-      <c r="T999" s="4"/>
-      <c r="U999" s="4"/>
-      <c r="V999" s="4"/>
-      <c r="W999" s="4"/>
-    </row>
-    <row r="1000" ht="14.25" customHeight="1">
-      <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="4"/>
-      <c r="D1000" s="4"/>
-      <c r="E1000" s="4"/>
-      <c r="F1000" s="4"/>
-      <c r="G1000" s="4"/>
-      <c r="H1000" s="4"/>
-      <c r="I1000" s="4"/>
-      <c r="J1000" s="4"/>
-      <c r="K1000" s="4"/>
-      <c r="L1000" s="4"/>
-      <c r="M1000" s="4"/>
-      <c r="N1000" s="4"/>
-      <c r="O1000" s="4"/>
-      <c r="P1000" s="4"/>
-      <c r="Q1000" s="4"/>
-      <c r="R1000" s="4"/>
-      <c r="S1000" s="4"/>
-      <c r="T1000" s="4"/>
-      <c r="U1000" s="4"/>
-      <c r="V1000" s="4"/>
-      <c r="W1000" s="4"/>
-    </row>
-    <row r="1001" ht="14.25" customHeight="1">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="4"/>
-      <c r="D1001" s="4"/>
-      <c r="E1001" s="4"/>
-      <c r="F1001" s="4"/>
-      <c r="G1001" s="4"/>
-      <c r="H1001" s="4"/>
-      <c r="I1001" s="4"/>
-      <c r="J1001" s="4"/>
-      <c r="K1001" s="4"/>
-      <c r="L1001" s="4"/>
-      <c r="M1001" s="4"/>
-      <c r="N1001" s="4"/>
-      <c r="O1001" s="4"/>
-      <c r="P1001" s="4"/>
-      <c r="Q1001" s="4"/>
-      <c r="R1001" s="4"/>
-      <c r="S1001" s="4"/>
-      <c r="T1001" s="4"/>
-      <c r="U1001" s="4"/>
-      <c r="V1001" s="4"/>
-      <c r="W1001" s="4"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Code tidy related to events. GetName and names removed for Positions. ToString now used instead as Unity side now handles names.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="253">
   <si>
     <t>Key</t>
   </si>
@@ -768,6 +768,12 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>YOU</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
 </sst>
 </file>
 
@@ -4202,7 +4208,15 @@
       <c r="W124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="B125" s="4"/>
+      <c r="A125" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>

</xml_diff>

<commit_message>
Updated installer, Italian translations for UI and tutorial implemented (Italian tutorial doesn't currently work)
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -10,8 +10,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="C65">
+      <text>
+        <t xml:space="preserve">?????Avere una visione d'insieme, attenzione, percezione sensoriale
+	-Ellis Spice</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="363">
   <si>
     <t>Key</t>
   </si>
@@ -28,7 +44,7 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>XXXX</t>
+    <t>Risultati</t>
   </si>
   <si>
     <t>AGE</t>
@@ -37,60 +53,90 @@
     <t>Age:</t>
   </si>
   <si>
+    <t>Età</t>
+  </si>
+  <si>
     <t>AMPERSAND</t>
   </si>
   <si>
     <t xml:space="preserve"> &amp; </t>
   </si>
   <si>
+    <t xml:space="preserve"> e </t>
+  </si>
+  <si>
     <t>BODY</t>
   </si>
   <si>
     <t>Strength</t>
   </si>
   <si>
+    <t>Forza</t>
+  </si>
+  <si>
     <t>BOWMAN</t>
   </si>
   <si>
     <t>Bowman</t>
   </si>
   <si>
+    <t>Prodiere</t>
+  </si>
+  <si>
     <t>BOWMAN_DESCRIPTION</t>
   </si>
   <si>
     <t>Awareness, fast reactions and being able to handle fear is required here, as those in this position will need to climb the maist/bow to help chnage the sails.</t>
   </si>
   <si>
+    <t>Consapevolezza, capacità di reagire rapidamente e di gestire la paura sono richiesti per questa posizione. Chi ricoprirà questo ruolo dovrà salire sull'albero per aiutare a cambiare le vele.</t>
+  </si>
+  <si>
     <t>CANCEL</t>
   </si>
   <si>
     <t>Cancel</t>
   </si>
   <si>
+    <t>Cancella</t>
+  </si>
+  <si>
     <t>CHARISMA</t>
   </si>
   <si>
     <t>Charisma</t>
   </si>
   <si>
+    <t>Carisma</t>
+  </si>
+  <si>
     <t>CORRECT</t>
   </si>
   <si>
     <t>Correct</t>
   </si>
   <si>
+    <t>Corretto</t>
+  </si>
+  <si>
     <t>CREATE_GAME</t>
   </si>
   <si>
     <t>Create Game</t>
   </si>
   <si>
+    <t>Crea il gioco</t>
+  </si>
+  <si>
     <t>CREW_OPINION</t>
   </si>
   <si>
     <t>Crew Opinion</t>
   </si>
   <si>
+    <t>Opinione dell'equipaggio</t>
+  </si>
+  <si>
     <t>ENGLISH</t>
   </si>
   <si>
@@ -106,6 +152,9 @@
     <t>Exit</t>
   </si>
   <si>
+    <t>Esci</t>
+  </si>
+  <si>
     <t>FEEDBACK</t>
   </si>
   <si>
@@ -118,48 +167,72 @@
     <t>Female</t>
   </si>
   <si>
+    <t>Donna</t>
+  </si>
+  <si>
     <t>FIRE</t>
   </si>
   <si>
     <t>Dismiss</t>
   </si>
   <si>
+    <t>Congeda</t>
+  </si>
+  <si>
     <t>FIRE_BUTTON_HOVER_ALLOWANCE</t>
   </si>
   <si>
     <t>Cannot dismiss crew members due to a lack of talk time.</t>
   </si>
   <si>
+    <t>Non puoi congedare i membri dell'equipaggio perché hai esaurito il tempo di intervista.</t>
+  </si>
+  <si>
     <t>FIRE_BUTTON_HOVER_CREW_LIMIT</t>
   </si>
   <si>
     <t>Cannot dismiss crew members as team is currently at its minimum size.</t>
   </si>
   <si>
+    <t>Non puoi congedare i membri dell'equipaggio perché la squadra ha raggiunto il numero minimo di giocatori.</t>
+  </si>
+  <si>
     <t>FIRE_BUTTON_HOVER_LIMIT</t>
   </si>
   <si>
     <t>Cannot dismiss crew members as crew change limit ({0}) has been reached for this race session.</t>
   </si>
   <si>
+    <t>Non puoi congedare i membri dell'equipaggio perché il limite ({0}) massimo di cambiamenti è stato raggiunto per questa sessione di gioco.</t>
+  </si>
+  <si>
     <t>FIRE_BUTTON_HOVER_TUTORIAL</t>
   </si>
   <si>
     <t>Cannot dismiss crew members during the tutorial.</t>
   </si>
   <si>
+    <t>Non puoi congedare i membri dell'equipaggio durante il tutorial.</t>
+  </si>
+  <si>
     <t>FIRE_WARNING</t>
   </si>
   <si>
     <t>Are you sure you want to remove this person from the team? This action cannot be undone!</t>
   </si>
   <si>
+    <t>Sei sicuro di voler rimuovere questa persona dal team? Questa azione non può essere cancellata.</t>
+  </si>
+  <si>
     <t>GREEN_PLACEMENT</t>
   </si>
   <si>
     <t>Ideal Placements</t>
   </si>
   <si>
+    <t>Collocazioni ideali</t>
+  </si>
+  <si>
     <t>GRINDER</t>
   </si>
   <si>
@@ -172,43 +245,61 @@
     <t>Tasked with hoisting the sails, only the super strong will do well here.</t>
   </si>
   <si>
+    <t>E' impiegato a issare le vele, solo chi è fisicamente molto forte può far bene in questo ruolo.</t>
+  </si>
+  <si>
     <t>HELMSMAN</t>
   </si>
   <si>
     <t>Helmsman</t>
   </si>
   <si>
+    <t>Timoniere</t>
+  </si>
+  <si>
     <t>HELMSMAN_DESCRIPTION</t>
   </si>
   <si>
     <t>Steers the ship. The ability to think ahead and react as soon as possible is needed here.</t>
   </si>
   <si>
+    <t>Guida la barca. La lungimiranza e la capacità di reagire tempestivamente sono necessarie per questo ruolo.</t>
+  </si>
+  <si>
     <t>HELP</t>
   </si>
   <si>
     <t>Help</t>
   </si>
   <si>
+    <t>Aiuto</t>
+  </si>
+  <si>
     <t>HIDDEN</t>
   </si>
   <si>
     <t>Hidden</t>
   </si>
   <si>
+    <t>Nascosto</t>
+  </si>
+  <si>
     <t>HIRE_WARNING_NOT_POSSIBLE</t>
   </si>
   <si>
     <t>You don't have enough time left to hire this person.</t>
   </si>
   <si>
+    <t>Non hai abbastanza tempo a disposizione per assumere questa persona.</t>
+  </si>
+  <si>
     <t>HIRE_WARNING_POSSIBLE</t>
   </si>
   <si>
     <t>Are you sure you want to hire {0}?</t>
   </si>
   <si>
-    <t>{0}</t>
+    <t>Sei sicuro di voler assumere {0}?</t>
   </si>
   <si>
     <t>ITALIAN</t>
@@ -223,154 +314,232 @@
     <t>Language</t>
   </si>
   <si>
+    <t>Lingua</t>
+  </si>
+  <si>
     <t>LEADERBOARDS</t>
   </si>
   <si>
     <t>Leaderboards</t>
   </si>
   <si>
+    <t>Classifiche</t>
+  </si>
+  <si>
     <t>LOAD_GAME</t>
   </si>
   <si>
     <t>Load Game</t>
   </si>
   <si>
+    <t>Carica il gioco</t>
+  </si>
+  <si>
     <t>LOAD_GAME_MISSING_FILES</t>
   </si>
   <si>
     <t>Unable to load game due to missing files. Please try loading a different game.</t>
   </si>
   <si>
+    <t>Il gioco non può essere caricato perché mancano i file. Prova a caricare un gioco diverso.</t>
+  </si>
+  <si>
     <t>LOAD_GAME_NOT_LOADED</t>
   </si>
   <si>
     <t>Game was not loaded. Please try again.</t>
   </si>
   <si>
+    <t>Il gioco non è stato caricato. Prova ancora.</t>
+  </si>
+  <si>
     <t>MAIN_MENU</t>
   </si>
   <si>
     <t>Main Menu</t>
   </si>
   <si>
+    <t>Menù principale</t>
+  </si>
+  <si>
     <t>MALE</t>
   </si>
   <si>
     <t>Male</t>
   </si>
   <si>
+    <t>Uomo</t>
+  </si>
+  <si>
     <t>MANAGER_AGE</t>
   </si>
   <si>
     <t>Manager Age:</t>
   </si>
   <si>
+    <t>Età del coach:</t>
+  </si>
+  <si>
     <t>MANAGER_GENDER</t>
   </si>
   <si>
     <t>Manager Gender:</t>
   </si>
   <si>
+    <t>Sesso del coach:</t>
+  </si>
+  <si>
     <t>MANAGER_NAME</t>
   </si>
   <si>
     <t>Manager Name:</t>
   </si>
   <si>
+    <t>Nome del coach:</t>
+  </si>
+  <si>
     <t>MANAGER_OPINION</t>
   </si>
   <si>
     <t>Manager Opinion</t>
   </si>
   <si>
+    <t>Opinione del coach</t>
+  </si>
+  <si>
     <t>MEETING_EARLY_EXIT</t>
   </si>
   <si>
     <t>Nevermind, goodbye.</t>
   </si>
   <si>
+    <t>Non importa, ciao.</t>
+  </si>
+  <si>
     <t>MEETING_EXIT</t>
   </si>
   <si>
     <t>OK, thank you for telling me that.</t>
   </si>
   <si>
+    <t>OK, grazie per avermelo detto.</t>
+  </si>
+  <si>
     <t>MEETING_HEADER</t>
   </si>
   <si>
     <t>What do you want to ask?</t>
   </si>
   <si>
+    <t>Che cosa vuoi chiedere?</t>
+  </si>
+  <si>
     <t>MEETING_INTRO</t>
   </si>
   <si>
     <t>You wanted to see me?</t>
   </si>
   <si>
+    <t>Volevi vedermi?</t>
+  </si>
+  <si>
     <t>MENU_QUIT_CONFIRM</t>
   </si>
   <si>
     <t>Are you sure you want to quit out to the menu? Unsaved changes will be lost!</t>
   </si>
   <si>
+    <t>Sei sicuro di voler andare al menù? Cambiamenti non salvati andranno perduti.</t>
+  </si>
+  <si>
     <t>MIDBOWMAN</t>
   </si>
   <si>
     <t>Mid-Bowman</t>
   </si>
   <si>
+    <t>Assistente prodiere</t>
+  </si>
+  <si>
     <t>MIDBOWMAN_DESCRIPTION</t>
   </si>
   <si>
     <t>Stows sails below deck and helps with sail changes. Crew positioned here will need to be physically fit, agile and able to deal with being in this hot, dark and wet position.</t>
   </si>
   <si>
+    <t>Ripiega le vele sottocoperta e aiuta nel cambio della vela. Chi e occupa questa posizione deve essere fisicamente prestante, agile ed essere in grado di sopportare il caldo, il buio e l'umidità.</t>
+  </si>
+  <si>
     <t>MOOD</t>
   </si>
   <si>
     <t>Mood</t>
   </si>
   <si>
+    <t>Umore</t>
+  </si>
+  <si>
     <t>MUSIC</t>
   </si>
   <si>
     <t>Music</t>
   </si>
   <si>
+    <t>Musica</t>
+  </si>
+  <si>
     <t>MY_CREW</t>
   </si>
   <si>
     <t>My Crew</t>
   </si>
   <si>
+    <t>Il mio equipaggio</t>
+  </si>
+  <si>
     <t>NAME</t>
   </si>
   <si>
     <t>Name:</t>
   </si>
   <si>
+    <t>Nome:</t>
+  </si>
+  <si>
     <t>NAVIGATOR</t>
   </si>
   <si>
     <t>Navigator</t>
   </si>
   <si>
+    <t>Navigatore</t>
+  </si>
+  <si>
     <t>NAVIGATOR_DESCRIPTION</t>
   </si>
   <si>
     <t>In charge of manoeuvres. Situational awareness and reactions are key to succeed in this position.</t>
   </si>
   <si>
+    <t>Si occupa delle manovre. Consapevolezza situazionale e reattività sono gli aspetti chiave per ricoprire questo ruolo.</t>
+  </si>
+  <si>
     <t>NEW_GAME</t>
   </si>
   <si>
     <t>New Game</t>
   </si>
   <si>
+    <t>Nuovo gioco</t>
+  </si>
+  <si>
     <t>NEW_GAME_CREATION_ERROR</t>
   </si>
   <si>
     <t>Game not created. Please try again.</t>
+  </si>
+  <si>
+    <t>Il gioco non è stato creato. Riprova.</t>
   </si>
   <si>
     <t>NEW_GAME_OVERWRITE</t>
@@ -380,6 +549,9 @@
 Are you sure you want to create a new game and overwrite the existing game?</t>
   </si>
   <si>
+    <t>Un gioco con questo nome esiste già!</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
@@ -392,142 +564,211 @@
     <t>No Role</t>
   </si>
   <si>
+    <t>Nessun ruolo</t>
+  </si>
+  <si>
     <t>OK</t>
   </si>
   <si>
+    <t>Ok</t>
+  </si>
+  <si>
     <t>OVERWRITE</t>
   </si>
   <si>
     <t>Overwrite</t>
   </si>
   <si>
+    <t>Sovrascrivi</t>
+  </si>
+  <si>
     <t>PERCEPTION</t>
   </si>
   <si>
     <t>Perception</t>
   </si>
   <si>
+    <t>Percezione</t>
+  </si>
+  <si>
     <t>PITMAN</t>
   </si>
   <si>
     <t>Pitman</t>
   </si>
   <si>
+    <t>Drizzista</t>
+  </si>
+  <si>
     <t>PITMAN_DESCRIPTION</t>
   </si>
   <si>
     <t>Manages sail changes and can also hoist if needed. Strength, awareness and decent communication skills are required to do well in this role.</t>
   </si>
   <si>
+    <t>Gestisce il cambio delle vele e può anche issarle se necessario. Forza, consapevolezza e buone capacità comunicative sono richieste per una buona riuscita in questo ruolo.</t>
+  </si>
+  <si>
     <t>POSITION_1</t>
   </si>
   <si>
     <t>1st</t>
   </si>
   <si>
+    <t>Primo</t>
+  </si>
+  <si>
     <t>POSITION_10</t>
   </si>
   <si>
     <t>10th</t>
   </si>
   <si>
+    <t>Decimo</t>
+  </si>
+  <si>
     <t>POSITION_2</t>
   </si>
   <si>
     <t>2nd</t>
   </si>
   <si>
+    <t>Secondo</t>
+  </si>
+  <si>
     <t>POSITION_3</t>
   </si>
   <si>
     <t>3rd</t>
   </si>
   <si>
+    <t>Terzo</t>
+  </si>
+  <si>
     <t>POSITION_4</t>
   </si>
   <si>
     <t>4th</t>
   </si>
   <si>
+    <t>Quarto</t>
+  </si>
+  <si>
     <t>POSITION_5</t>
   </si>
   <si>
     <t>5th</t>
   </si>
   <si>
+    <t>Quinto</t>
+  </si>
+  <si>
     <t>POSITION_6</t>
   </si>
   <si>
     <t>6th</t>
   </si>
   <si>
+    <t>Sesto</t>
+  </si>
+  <si>
     <t>POSITION_7</t>
   </si>
   <si>
     <t>7th</t>
   </si>
   <si>
+    <t>Settimo</t>
+  </si>
+  <si>
     <t>POSITION_8</t>
   </si>
   <si>
     <t>8th</t>
   </si>
   <si>
+    <t>Ottavo</t>
+  </si>
+  <si>
     <t>POSITION_9</t>
   </si>
   <si>
     <t>9th</t>
   </si>
   <si>
+    <t>Nono</t>
+  </si>
+  <si>
     <t>POSITION_NAME</t>
   </si>
   <si>
     <t>Position Name</t>
   </si>
   <si>
+    <t>Nome della posizione</t>
+  </si>
+  <si>
     <t>PREVIOUS_MEMBERS</t>
   </si>
   <si>
     <t>Previous Members</t>
   </si>
   <si>
+    <t>Membri precedenti</t>
+  </si>
+  <si>
     <t>PROMOTION_ADDED</t>
   </si>
   <si>
     <t>Added</t>
   </si>
   <si>
+    <t>Aggiunto</t>
+  </si>
+  <si>
     <t>PROMOTION_HEADER</t>
   </si>
   <si>
     <t>Your boat type has changed!</t>
   </si>
   <si>
+    <t>La tua imbarcazione è cambiata!</t>
+  </si>
+  <si>
     <t>PROMOTION_REMOVED</t>
   </si>
   <si>
     <t>Removed</t>
   </si>
   <si>
+    <t>Rimosso</t>
+  </si>
+  <si>
     <t>QUICKNESS</t>
   </si>
   <si>
     <t>Quickness</t>
   </si>
   <si>
+    <t>Velocità</t>
+  </si>
+  <si>
     <t>RACE_BUTTON_PRACTICE</t>
   </si>
   <si>
     <t>Practice {0}/{1}</t>
   </si>
   <si>
-    <t>{0}{1}</t>
+    <t>Prova {0}/{1}</t>
   </si>
   <si>
     <t>RACE_BUTTON_RACE</t>
   </si>
   <si>
     <t>Race!</t>
+  </si>
+  <si>
+    <t>Gara!</t>
   </si>
   <si>
     <t>RACE_CONFIRM_ALLOWANCE_REMAINING</t>
@@ -537,25 +778,34 @@
 Are you sure you want to race with this line-up now?</t>
   </si>
   <si>
+    <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.</t>
+  </si>
+  <si>
     <t>RACE_CONFIRM_NO_ALLOWANCE</t>
   </si>
   <si>
     <t>Are you sure you want to race with this line-up now?</t>
   </si>
   <si>
+    <t>Sei sicuro di voler gareggiare con questa formazione?</t>
+  </si>
+  <si>
     <t>RACE_POSITION</t>
   </si>
   <si>
     <t>Position:</t>
   </si>
   <si>
+    <t>Posizione:</t>
+  </si>
+  <si>
     <t>RACE_RESULT_POSTION</t>
   </si>
   <si>
     <t>{0} finished {1}!</t>
   </si>
   <si>
-    <t>{0}{1}!</t>
+    <t>{0} si classifica {1}!</t>
   </si>
   <si>
     <t>RANDOMISE</t>
@@ -564,24 +814,36 @@
     <t>Randomise</t>
   </si>
   <si>
+    <t>Randomizza</t>
+  </si>
+  <si>
     <t>RECRUIT_BUTTON_HOVER_ALLOWANCE</t>
   </si>
   <si>
     <t>Recruitment unavilable due to lack of talk time.</t>
   </si>
   <si>
+    <t>il reclutamento non è più attivabile a causa della mancanza di tempo di conversazione.</t>
+  </si>
+  <si>
     <t>RECRUIT_BUTTON_HOVER_LIMIT</t>
   </si>
   <si>
     <t>Recruitment unavilable as crew change limit ({0}) has been reached for this race session.</t>
   </si>
   <si>
+    <t>Il reclutamento non è più attivabile. È stato raggiunto il limite ({0}) massimo di cambiamenti per questa sessione di gioco.</t>
+  </si>
+  <si>
     <t>RECRUIT_GREETING_0</t>
   </si>
   <si>
     <t>Hello</t>
   </si>
   <si>
+    <t>Ciao</t>
+  </si>
+  <si>
     <t>RECRUIT_GREETING_1</t>
   </si>
   <si>
@@ -600,84 +862,126 @@
     <t>Hey there</t>
   </si>
   <si>
+    <t>Ehilà</t>
+  </si>
+  <si>
     <t>RECRUIT_LEAVE</t>
   </si>
   <si>
     <t>Leave without recruiting</t>
   </si>
   <si>
+    <t>Lascia senza reclutare nessuno.</t>
+  </si>
+  <si>
     <t>RECRUITMENT_INTRO</t>
   </si>
   <si>
     <t>Your recruits are here. What do you want to ask them all or who do you want to hire?</t>
   </si>
   <si>
+    <t>I tuoi candidati sono qui. Cosa vuoi chiedere loro o chi vorresti reclutare?</t>
+  </si>
+  <si>
     <t>RED_PLACEMENT</t>
   </si>
   <si>
     <t>Unideal Placements</t>
   </si>
   <si>
+    <t>Posizioni non ideali</t>
+  </si>
+  <si>
     <t>REPEAT_CONFIRM</t>
   </si>
   <si>
     <t>Are you sure you want to use the same crew line-up as the previous race?</t>
   </si>
   <si>
+    <t>Sei sicuro di voler utilizzare la stessa formazione anche per la prossima gara?</t>
+  </si>
+  <si>
     <t>REQUIRED</t>
   </si>
   <si>
     <t>Required</t>
   </si>
   <si>
+    <t>Richiesto</t>
+  </si>
+  <si>
     <t>RESULT</t>
   </si>
   <si>
     <t>Result</t>
   </si>
   <si>
+    <t>Risultato</t>
+  </si>
+  <si>
     <t>RESULT_HEADER</t>
   </si>
   <si>
     <t>The race is over and the results are in...</t>
   </si>
   <si>
+    <t>La gara è finita e i risultati sono stati salvati</t>
+  </si>
+  <si>
     <t>ROLE</t>
   </si>
   <si>
     <t>Role:</t>
   </si>
   <si>
+    <t>Ruolo:</t>
+  </si>
+  <si>
     <t>SEASON_RANKING</t>
   </si>
   <si>
     <t>Season Ranking</t>
   </si>
   <si>
+    <t>Classifica del campionato:</t>
+  </si>
+  <si>
     <t>SETTINGS</t>
   </si>
   <si>
     <t>Settings</t>
   </si>
   <si>
+    <t>Impostazioni</t>
+  </si>
+  <si>
     <t>SHOW_TUTORIAL</t>
   </si>
   <si>
     <t>Show Tutorial:</t>
   </si>
   <si>
+    <t>Mostra il tutorial:</t>
+  </si>
+  <si>
     <t>SIGNED_IN_AS</t>
   </si>
   <si>
     <t>Signed in as:</t>
   </si>
   <si>
+    <t>Hai eseguito l'accesso come:</t>
+  </si>
+  <si>
     <t>SKILLS_REQUIRED</t>
   </si>
   <si>
     <t>Skills Required</t>
   </si>
   <si>
+    <t>Competenze richieste</t>
+  </si>
+  <si>
     <t>SKIPPER</t>
   </si>
   <si>
@@ -690,12 +994,18 @@
     <t>The team captain. They'll have to be able to lead the crew and handle the pressure of doing so, all the while knowing how to react in tough situations.</t>
   </si>
   <si>
+    <t>Il capitano della squadra. Dovrà essere in grado di condurre l'equipaggio e gestire la pressione, sapendo come reagire nelle situazioni critiche.</t>
+  </si>
+  <si>
     <t>SOUND</t>
   </si>
   <si>
     <t>Sound FX</t>
   </si>
   <si>
+    <t>Effetti sonori</t>
+  </si>
+  <si>
     <t>SUGAR_SIGN_IN</t>
   </si>
   <si>
@@ -708,34 +1018,52 @@
     <t>Talk Time Remaining</t>
   </si>
   <si>
+    <t>Tempo di conversazione rimanente</t>
+  </si>
+  <si>
     <t>TEAM_COLOURS</t>
   </si>
   <si>
     <t>Team Colours:</t>
   </si>
   <si>
+    <t>Colori della squadra:</t>
+  </si>
+  <si>
     <t>TEAM_MANAGEMENT</t>
   </si>
   <si>
     <t>Team Line-Up</t>
   </si>
   <si>
+    <t>Formazione</t>
+  </si>
+  <si>
     <t>TEAM_NAME</t>
   </si>
   <si>
     <t>Team Name:</t>
   </si>
   <si>
+    <t>Nome della squadra:</t>
+  </si>
+  <si>
     <t>TRIMMER</t>
   </si>
   <si>
     <t>Trimmer</t>
   </si>
   <si>
+    <t>Randista</t>
+  </si>
+  <si>
     <t>TRIMMER_DESCRIPTION</t>
   </si>
   <si>
     <t>Responsible for controlling the shape of the sails. Attention to detail and durability will bring success to those in this position.</t>
+  </si>
+  <si>
+    <t>Responsabile per il controllo delle vele. Attenzione ai dettagli e alla durata sono competenze necessarie per questo ruolo.</t>
   </si>
   <si>
     <t>TUTORIAL_WARNING</t>
@@ -745,34 +1073,52 @@
 If yes, you'll need to start a new game in order to take the tutorial.</t>
   </si>
   <si>
+    <t>Sei sicuro di voler uscire dal tutorial?</t>
+  </si>
+  <si>
     <t>WILLPOWER</t>
   </si>
   <si>
     <t>Willpower</t>
   </si>
   <si>
+    <t>Forza di volontà</t>
+  </si>
+  <si>
     <t>WISDOM</t>
   </si>
   <si>
     <t>Wisdom</t>
   </si>
   <si>
+    <t>Saggezza</t>
+  </si>
+  <si>
     <t>YELLOW_PLACEMENT</t>
   </si>
   <si>
     <t>Ideal In Another Position</t>
   </si>
   <si>
+    <t>Ideale in un'altra posizione</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>Sì</t>
+  </si>
+  <si>
     <t>YOU</t>
   </si>
   <si>
     <t>you</t>
+  </si>
+  <si>
+    <t>tu</t>
   </si>
 </sst>
 </file>
@@ -787,18 +1133,12 @@
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -812,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -827,9 +1167,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,13 +1224,13 @@
       <c r="W1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3"/>
@@ -914,14 +1251,14 @@
       <c r="W2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -941,14 +1278,14 @@
       <c r="W3" s="3"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -968,14 +1305,14 @@
       <c r="W4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -995,14 +1332,14 @@
       <c r="W5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
+      <c r="A6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1022,14 +1359,14 @@
       <c r="W6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
+      <c r="A7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1049,14 +1386,14 @@
       <c r="W7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
+      <c r="A8" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1076,14 +1413,14 @@
       <c r="W8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
+      <c r="A9" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1103,14 +1440,14 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
+      <c r="A10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1130,14 +1467,14 @@
       <c r="W10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
+      <c r="A11" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1157,14 +1494,14 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
+      <c r="A12" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1184,13 +1521,13 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
+      <c r="A13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="3"/>
@@ -1211,14 +1548,14 @@
       <c r="W13" s="4"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
+      <c r="A14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1238,14 +1575,14 @@
       <c r="W14" s="4"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
+      <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1265,14 +1602,14 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
+      <c r="A16" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1292,14 +1629,14 @@
       <c r="W16" s="3"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
+      <c r="A17" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1319,14 +1656,14 @@
       <c r="W17" s="3"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
+      <c r="A18" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1346,14 +1683,14 @@
       <c r="W18" s="3"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
+      <c r="A19" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1373,14 +1710,14 @@
       <c r="W19" s="4"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
+      <c r="A20" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1400,14 +1737,14 @@
       <c r="W20" s="4"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
+      <c r="A21" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1427,14 +1764,14 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
+      <c r="A22" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1454,14 +1791,14 @@
       <c r="W22" s="4"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
+      <c r="A23" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1481,14 +1818,14 @@
       <c r="W23" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
+      <c r="A24" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1508,14 +1845,14 @@
       <c r="W24" s="4"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>49</v>
+      <c r="A25" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1535,14 +1872,14 @@
       <c r="W25" s="4"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
+      <c r="A26" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1562,14 +1899,14 @@
       <c r="W26" s="4"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
+      <c r="A27" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1589,14 +1926,14 @@
       <c r="W27" s="4"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>55</v>
+      <c r="A28" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1616,14 +1953,14 @@
       <c r="W28" s="4"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>57</v>
+      <c r="A29" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1643,14 +1980,14 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
+      <c r="A30" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1670,14 +2007,14 @@
       <c r="W30" s="4"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>61</v>
+      <c r="A31" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>5</v>
+        <v>86</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -1697,14 +2034,14 @@
       <c r="W31" s="4"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
+      <c r="A32" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1724,14 +2061,14 @@
       <c r="W32" s="4"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="1" t="s">
-        <v>66</v>
+      <c r="A33" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>67</v>
+        <v>92</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -1751,14 +2088,14 @@
       <c r="W33" s="4"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>68</v>
+      <c r="A34" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>5</v>
+        <v>94</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -1778,14 +2115,14 @@
       <c r="W34" s="4"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>70</v>
+      <c r="A35" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>5</v>
+        <v>97</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -1805,14 +2142,14 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
+      <c r="A36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -1832,14 +2169,14 @@
       <c r="W36" s="3"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>74</v>
+      <c r="A37" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
+        <v>103</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -1859,14 +2196,14 @@
       <c r="W37" s="4"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>76</v>
+      <c r="A38" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>5</v>
+        <v>106</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -1886,14 +2223,14 @@
       <c r="W38" s="4"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>78</v>
+      <c r="A39" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>5</v>
+        <v>109</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -1913,14 +2250,14 @@
       <c r="W39" s="3"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>80</v>
+      <c r="A40" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>112</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -1940,14 +2277,14 @@
       <c r="W40" s="3"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>82</v>
+      <c r="A41" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>5</v>
+        <v>115</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -1967,14 +2304,14 @@
       <c r="W41" s="3"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>84</v>
+      <c r="A42" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>5</v>
+        <v>118</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -1994,14 +2331,14 @@
       <c r="W42" s="3"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>86</v>
+      <c r="A43" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>5</v>
+        <v>121</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -2021,14 +2358,14 @@
       <c r="W43" s="3"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>88</v>
+      <c r="A44" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>124</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -2048,14 +2385,14 @@
       <c r="W44" s="3"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>90</v>
+      <c r="A45" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>5</v>
+        <v>127</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -2075,14 +2412,14 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>92</v>
+      <c r="A46" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -2102,14 +2439,14 @@
       <c r="W46" s="4"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>94</v>
+      <c r="A47" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>5</v>
+        <v>133</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -2129,14 +2466,14 @@
       <c r="W47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>96</v>
+      <c r="A48" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -2156,14 +2493,14 @@
       <c r="W48" s="4"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>98</v>
+      <c r="A49" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
+        <v>139</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -2183,14 +2520,14 @@
       <c r="W49" s="4"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="1" t="s">
-        <v>100</v>
+      <c r="A50" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>5</v>
+        <v>142</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -2210,14 +2547,14 @@
       <c r="W50" s="4"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="1" t="s">
-        <v>102</v>
+      <c r="A51" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>5</v>
+        <v>145</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -2237,14 +2574,14 @@
       <c r="W51" s="4"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="1" t="s">
-        <v>104</v>
+      <c r="A52" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>5</v>
+        <v>148</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -2264,14 +2601,14 @@
       <c r="W52" s="4"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="1" t="s">
-        <v>106</v>
+      <c r="A53" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>5</v>
+        <v>151</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -2291,14 +2628,14 @@
       <c r="W53" s="4"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="1" t="s">
-        <v>108</v>
+      <c r="A54" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>5</v>
+        <v>154</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -2318,14 +2655,14 @@
       <c r="W54" s="4"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="1" t="s">
-        <v>110</v>
+      <c r="A55" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>5</v>
+        <v>157</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2345,14 +2682,14 @@
       <c r="W55" s="3"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="1" t="s">
-        <v>112</v>
+      <c r="A56" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>5</v>
+        <v>160</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -2372,14 +2709,14 @@
       <c r="W56" s="4"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="1" t="s">
-        <v>114</v>
+      <c r="A57" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>5</v>
+        <v>163</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -2399,14 +2736,14 @@
       <c r="W57" s="4"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>5</v>
+      <c r="A58" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -2426,14 +2763,14 @@
       <c r="W58" s="3"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="1" t="s">
-        <v>118</v>
+      <c r="A59" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>5</v>
+        <v>169</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
@@ -2453,14 +2790,14 @@
       <c r="W59" s="4"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="1" t="s">
-        <v>120</v>
+      <c r="A60" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
+        <v>172</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
@@ -2480,14 +2817,14 @@
       <c r="W60" s="4"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="1" t="s">
-        <v>122</v>
+      <c r="A61" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>5</v>
+        <v>175</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -2507,14 +2844,14 @@
       <c r="W61" s="3"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>124</v>
+      <c r="A62" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>5</v>
+        <v>177</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -2534,14 +2871,14 @@
       <c r="W62" s="4"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="1" t="s">
-        <v>126</v>
+      <c r="A63" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>5</v>
+        <v>179</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -2561,14 +2898,14 @@
       <c r="W63" s="3"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="1" t="s">
-        <v>127</v>
+      <c r="A64" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>5</v>
+        <v>182</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -2588,15 +2925,16 @@
       <c r="W64" s="4"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="1" t="s">
-        <v>129</v>
+      <c r="A65" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D65" s="1"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
@@ -2615,14 +2953,14 @@
       <c r="W65" s="3"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="1" t="s">
-        <v>131</v>
+      <c r="A66" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>5</v>
+        <v>188</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -2642,14 +2980,14 @@
       <c r="W66" s="4"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="1" t="s">
-        <v>133</v>
+      <c r="A67" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>191</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -2669,14 +3007,14 @@
       <c r="W67" s="4"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="1" t="s">
-        <v>135</v>
+      <c r="A68" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1.0</v>
+        <v>194</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -2696,14 +3034,14 @@
       <c r="W68" s="4"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="1" t="s">
-        <v>137</v>
+      <c r="A69" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="1">
-        <v>10.0</v>
+        <v>197</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -2723,14 +3061,14 @@
       <c r="W69" s="4"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="1" t="s">
-        <v>139</v>
+      <c r="A70" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C70" s="1">
-        <v>2.0</v>
+        <v>200</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -2750,14 +3088,14 @@
       <c r="W70" s="4"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="1" t="s">
-        <v>141</v>
+      <c r="A71" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="1">
-        <v>3.0</v>
+        <v>203</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -2777,14 +3115,14 @@
       <c r="W71" s="4"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="1" t="s">
-        <v>143</v>
+      <c r="A72" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C72" s="1">
-        <v>4.0</v>
+        <v>206</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -2804,14 +3142,14 @@
       <c r="W72" s="4"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="1" t="s">
-        <v>145</v>
+      <c r="A73" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C73" s="1">
-        <v>5.0</v>
+        <v>209</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -2831,14 +3169,14 @@
       <c r="W73" s="4"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="1" t="s">
-        <v>147</v>
+      <c r="A74" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" s="1">
-        <v>6.0</v>
+        <v>212</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -2858,14 +3196,14 @@
       <c r="W74" s="4"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="1" t="s">
-        <v>149</v>
+      <c r="A75" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="1">
-        <v>7.0</v>
+        <v>215</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -2885,14 +3223,14 @@
       <c r="W75" s="4"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="1" t="s">
-        <v>151</v>
+      <c r="A76" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" s="1">
-        <v>8.0</v>
+        <v>218</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -2912,14 +3250,14 @@
       <c r="W76" s="4"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="1" t="s">
-        <v>153</v>
+      <c r="A77" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="1">
-        <v>9.0</v>
+        <v>221</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -2939,14 +3277,14 @@
       <c r="W77" s="4"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="1" t="s">
-        <v>155</v>
+      <c r="A78" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>5</v>
+        <v>224</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -2966,14 +3304,14 @@
       <c r="W78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="1" t="s">
-        <v>157</v>
+      <c r="A79" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>5</v>
+        <v>227</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -2993,14 +3331,14 @@
       <c r="W79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="1" t="s">
-        <v>159</v>
+      <c r="A80" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>5</v>
+        <v>230</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3020,14 +3358,14 @@
       <c r="W80" s="4"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="1" t="s">
-        <v>161</v>
+      <c r="A81" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>5</v>
+        <v>233</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -3047,14 +3385,14 @@
       <c r="W81" s="4"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="1" t="s">
-        <v>163</v>
+      <c r="A82" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>5</v>
+        <v>236</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -3074,14 +3412,14 @@
       <c r="W82" s="4"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="1" t="s">
-        <v>165</v>
+      <c r="A83" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>5</v>
+        <v>239</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3101,14 +3439,14 @@
       <c r="W83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="1" t="s">
-        <v>167</v>
+      <c r="A84" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>169</v>
+        <v>242</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3128,14 +3466,14 @@
       <c r="W84" s="4"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="1" t="s">
-        <v>170</v>
+      <c r="A85" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>5</v>
+        <v>245</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -3155,14 +3493,14 @@
       <c r="W85" s="4"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="1" t="s">
-        <v>172</v>
+      <c r="A86" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>65</v>
+        <v>248</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3182,14 +3520,14 @@
       <c r="W86" s="4"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="1" t="s">
-        <v>174</v>
+      <c r="A87" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>5</v>
+        <v>251</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3209,14 +3547,14 @@
       <c r="W87" s="4"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="1" t="s">
-        <v>176</v>
+      <c r="A88" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>5</v>
+        <v>254</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3236,14 +3574,14 @@
       <c r="W88" s="4"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="1" t="s">
-        <v>178</v>
+      <c r="A89" s="2" t="s">
+        <v>256</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>180</v>
+        <v>257</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>258</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3263,14 +3601,14 @@
       <c r="W89" s="4"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="1" t="s">
-        <v>181</v>
+      <c r="A90" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>5</v>
+        <v>260</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -3290,14 +3628,14 @@
       <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="1" t="s">
-        <v>183</v>
+      <c r="A91" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>5</v>
+        <v>263</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3317,14 +3655,14 @@
       <c r="W91" s="4"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="1" t="s">
-        <v>185</v>
+      <c r="A92" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>5</v>
+        <v>266</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -3344,14 +3682,14 @@
       <c r="W92" s="4"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="1" t="s">
-        <v>187</v>
+      <c r="A93" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>5</v>
+        <v>269</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3371,14 +3709,14 @@
       <c r="W93" s="4"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="5" t="s">
-        <v>189</v>
+      <c r="A94" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>5</v>
+        <v>272</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -3398,14 +3736,14 @@
       <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="5" t="s">
-        <v>191</v>
+      <c r="A95" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>5</v>
+        <v>274</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -3425,14 +3763,14 @@
       <c r="W95" s="4"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="5" t="s">
-        <v>193</v>
+      <c r="A96" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>5</v>
+        <v>276</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -3452,14 +3790,14 @@
       <c r="W96" s="4"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="1" t="s">
-        <v>195</v>
+      <c r="A97" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>5</v>
+        <v>279</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -3479,14 +3817,14 @@
       <c r="W97" s="3"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="1" t="s">
-        <v>197</v>
+      <c r="A98" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>5</v>
+        <v>282</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -3506,14 +3844,14 @@
       <c r="W98" s="4"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="1" t="s">
-        <v>199</v>
+      <c r="A99" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>5</v>
+        <v>285</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
@@ -3533,14 +3871,14 @@
       <c r="W99" s="4"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="1" t="s">
-        <v>201</v>
+      <c r="A100" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>5</v>
+        <v>288</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -3560,14 +3898,14 @@
       <c r="W100" s="4"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="1" t="s">
-        <v>203</v>
+      <c r="A101" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>5</v>
+        <v>291</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -3587,14 +3925,14 @@
       <c r="W101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="1" t="s">
-        <v>205</v>
+      <c r="A102" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>5</v>
+        <v>294</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -3614,14 +3952,14 @@
       <c r="W102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="1" t="s">
-        <v>207</v>
+      <c r="A103" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>5</v>
+        <v>297</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -3641,14 +3979,14 @@
       <c r="W103" s="3"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="1" t="s">
-        <v>209</v>
+      <c r="A104" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>5</v>
+        <v>300</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>301</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -3668,14 +4006,14 @@
       <c r="W104" s="3"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="1" t="s">
-        <v>211</v>
+      <c r="A105" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>5</v>
+        <v>303</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -3695,14 +4033,14 @@
       <c r="W105" s="3"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" t="s">
-        <v>213</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>5</v>
+      <c r="A106" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -3722,14 +4060,14 @@
       <c r="W106" s="3"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" s="1" t="s">
-        <v>215</v>
+      <c r="A107" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>5</v>
+        <v>309</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
@@ -3749,14 +4087,14 @@
       <c r="W107" s="4"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="1" t="s">
-        <v>217</v>
+      <c r="A108" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>5</v>
+        <v>312</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -3776,14 +4114,14 @@
       <c r="W108" s="4"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="1" t="s">
-        <v>219</v>
+      <c r="A109" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>5</v>
+        <v>315</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>316</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
@@ -3803,14 +4141,14 @@
       <c r="W109" s="3"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="1" t="s">
-        <v>221</v>
+      <c r="A110" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>5</v>
+        <v>318</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
@@ -3830,14 +4168,14 @@
       <c r="W110" s="4"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>223</v>
+      <c r="A111" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>5</v>
+        <v>320</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>321</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
@@ -3857,14 +4195,14 @@
       <c r="W111" s="4"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="1" t="s">
-        <v>225</v>
+      <c r="A112" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>5</v>
+        <v>323</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -3884,14 +4222,14 @@
       <c r="W112" s="4"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>5</v>
+      <c r="A113" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -3911,14 +4249,14 @@
       <c r="W113" s="4"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="1" t="s">
-        <v>229</v>
+      <c r="A114" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
+        <v>328</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -3938,14 +4276,14 @@
       <c r="W114" s="3"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="1" t="s">
-        <v>231</v>
+      <c r="A115" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>5</v>
+        <v>331</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -3965,14 +4303,14 @@
       <c r="W115" s="3"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" s="1" t="s">
-        <v>233</v>
+      <c r="A116" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>5</v>
+        <v>334</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>335</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -3992,14 +4330,14 @@
       <c r="W116" s="3"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" t="s">
-        <v>235</v>
+      <c r="A117" s="2" t="s">
+        <v>336</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>5</v>
+        <v>337</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -4019,14 +4357,14 @@
       <c r="W117" s="3"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="1" t="s">
-        <v>237</v>
+      <c r="A118" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>5</v>
+        <v>340</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
@@ -4046,14 +4384,14 @@
       <c r="W118" s="4"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" s="1" t="s">
-        <v>239</v>
+      <c r="A119" s="2" t="s">
+        <v>342</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>5</v>
+        <v>343</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>344</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
@@ -4073,14 +4411,14 @@
       <c r="W119" s="4"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" s="1" t="s">
-        <v>241</v>
+      <c r="A120" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>5</v>
+        <v>346</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -4100,14 +4438,14 @@
       <c r="W120" s="4"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" s="1" t="s">
-        <v>243</v>
+      <c r="A121" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>5</v>
+        <v>349</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -4127,14 +4465,14 @@
       <c r="W121" s="3"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" s="1" t="s">
-        <v>245</v>
+      <c r="A122" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>5</v>
+        <v>352</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -4154,14 +4492,14 @@
       <c r="W122" s="3"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="1" t="s">
-        <v>247</v>
+      <c r="A123" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>5</v>
+        <v>355</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>356</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
@@ -4181,14 +4519,14 @@
       <c r="W123" s="4"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" s="1" t="s">
-        <v>249</v>
+      <c r="A124" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>5</v>
+        <v>358</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -4208,14 +4546,14 @@
       <c r="W124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="1" t="s">
-        <v>251</v>
+      <c r="A125" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>5</v>
+        <v>361</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
@@ -25904,6 +26242,7 @@
       <c r="W998" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Players now able to skip to the race session if they select the correct line-up.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="368">
   <si>
     <t>Key</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Age:</t>
   </si>
   <si>
-    <t>Età</t>
+    <t>Età:</t>
   </si>
   <si>
     <t>AMPERSAND</t>
@@ -808,6 +808,22 @@
     <t>{0} si classifica {1}!</t>
   </si>
   <si>
+    <t>RACE_SKIP_CONFIRM_ALLOWANCE_REMAINING</t>
+  </si>
+  <si>
+    <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?
+You also have {0} Talk Time remaining, which will be lost if not used before racing.</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>RACE_SKIP_CONFIRM_NO_ALLOWANCE</t>
+  </si>
+  <si>
+    <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
+  </si>
+  <si>
     <t>RANDOMISE</t>
   </si>
   <si>
@@ -943,7 +959,7 @@
     <t>Season Ranking</t>
   </si>
   <si>
-    <t>Classifica del campionato:</t>
+    <t>Classifica del campionato</t>
   </si>
   <si>
     <t>SETTINGS</t>
@@ -3615,17 +3631,17 @@
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="3"/>
-      <c r="S90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+      <c r="U90" s="4"/>
+      <c r="V90" s="4"/>
+      <c r="W90" s="4"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
@@ -3635,7 +3651,7 @@
         <v>263</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3656,40 +3672,40 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
-      <c r="Q92" s="4"/>
-      <c r="R92" s="4"/>
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
-      <c r="U92" s="4"/>
-      <c r="V92" s="4"/>
-      <c r="W92" s="4"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3710,10 +3726,10 @@
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>272</v>
@@ -3743,7 +3759,7 @@
         <v>274</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -3764,10 +3780,10 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>277</v>
@@ -3797,34 +3813,34 @@
         <v>279</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
-      <c r="R97" s="3"/>
-      <c r="S97" s="3"/>
-      <c r="T97" s="3"/>
-      <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
-      <c r="W97" s="3"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+      <c r="U97" s="4"/>
+      <c r="V97" s="4"/>
+      <c r="W97" s="4"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -3845,40 +3861,40 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="4"/>
-      <c r="T99" s="4"/>
-      <c r="U99" s="4"/>
-      <c r="V99" s="4"/>
-      <c r="W99" s="4"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="3"/>
+      <c r="T99" s="3"/>
+      <c r="U99" s="3"/>
+      <c r="V99" s="3"/>
+      <c r="W99" s="3"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -3899,67 +3915,67 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
-      <c r="S101" s="3"/>
-      <c r="T101" s="3"/>
-      <c r="U101" s="3"/>
-      <c r="V101" s="3"/>
-      <c r="W101" s="3"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="4"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+      <c r="U101" s="4"/>
+      <c r="V101" s="4"/>
+      <c r="W101" s="4"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
-      <c r="M102" s="3"/>
-      <c r="N102" s="3"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
-      <c r="Q102" s="3"/>
-      <c r="R102" s="3"/>
-      <c r="S102" s="3"/>
-      <c r="T102" s="3"/>
-      <c r="U102" s="3"/>
-      <c r="V102" s="3"/>
-      <c r="W102" s="3"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="4"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+      <c r="U102" s="4"/>
+      <c r="V102" s="4"/>
+      <c r="W102" s="4"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -3980,13 +3996,13 @@
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -4007,13 +4023,13 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -4034,13 +4050,13 @@
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -4061,91 +4077,91 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
-      <c r="M107" s="4"/>
-      <c r="N107" s="4"/>
-      <c r="O107" s="4"/>
-      <c r="P107" s="4"/>
-      <c r="Q107" s="4"/>
-      <c r="R107" s="4"/>
-      <c r="S107" s="4"/>
-      <c r="T107" s="4"/>
-      <c r="U107" s="4"/>
-      <c r="V107" s="4"/>
-      <c r="W107" s="4"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="3"/>
+      <c r="T107" s="3"/>
+      <c r="U107" s="3"/>
+      <c r="V107" s="3"/>
+      <c r="W107" s="3"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
-      <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
-      <c r="Q108" s="4"/>
-      <c r="R108" s="4"/>
-      <c r="S108" s="4"/>
-      <c r="T108" s="4"/>
-      <c r="U108" s="4"/>
-      <c r="V108" s="4"/>
-      <c r="W108" s="4"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
-      <c r="N109" s="3"/>
-      <c r="O109" s="3"/>
-      <c r="P109" s="3"/>
-      <c r="Q109" s="3"/>
-      <c r="R109" s="3"/>
-      <c r="S109" s="3"/>
-      <c r="T109" s="3"/>
-      <c r="U109" s="3"/>
-      <c r="V109" s="3"/>
-      <c r="W109" s="3"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="4"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+      <c r="U109" s="4"/>
+      <c r="V109" s="4"/>
+      <c r="W109" s="4"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>318</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>318</v>
@@ -4182,17 +4198,17 @@
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
-      <c r="Q111" s="4"/>
-      <c r="R111" s="4"/>
-      <c r="S111" s="4"/>
-      <c r="T111" s="4"/>
-      <c r="U111" s="4"/>
-      <c r="V111" s="4"/>
-      <c r="W111" s="4"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3"/>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="3"/>
+      <c r="T111" s="3"/>
+      <c r="U111" s="3"/>
+      <c r="V111" s="3"/>
+      <c r="W111" s="3"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="2" t="s">
@@ -4202,7 +4218,7 @@
         <v>323</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -4223,10 +4239,10 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>326</v>
@@ -4263,17 +4279,17 @@
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
-      <c r="O114" s="3"/>
-      <c r="P114" s="3"/>
-      <c r="Q114" s="3"/>
-      <c r="R114" s="3"/>
-      <c r="S114" s="3"/>
-      <c r="T114" s="3"/>
-      <c r="U114" s="3"/>
-      <c r="V114" s="3"/>
-      <c r="W114" s="3"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4"/>
+      <c r="W114" s="4"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="2" t="s">
@@ -4283,34 +4299,34 @@
         <v>331</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
-      <c r="O115" s="3"/>
-      <c r="P115" s="3"/>
-      <c r="Q115" s="3"/>
-      <c r="R115" s="3"/>
-      <c r="S115" s="3"/>
-      <c r="T115" s="3"/>
-      <c r="U115" s="3"/>
-      <c r="V115" s="3"/>
-      <c r="W115" s="3"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="4"/>
+      <c r="W115" s="4"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -4331,13 +4347,13 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -4358,67 +4374,67 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
-      <c r="Q118" s="4"/>
-      <c r="R118" s="4"/>
-      <c r="S118" s="4"/>
-      <c r="T118" s="4"/>
-      <c r="U118" s="4"/>
-      <c r="V118" s="4"/>
-      <c r="W118" s="4"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="3"/>
+      <c r="P118" s="3"/>
+      <c r="Q118" s="3"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="3"/>
+      <c r="T118" s="3"/>
+      <c r="U118" s="3"/>
+      <c r="V118" s="3"/>
+      <c r="W118" s="3"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
-      <c r="M119" s="4"/>
-      <c r="N119" s="4"/>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
-      <c r="Q119" s="4"/>
-      <c r="R119" s="4"/>
-      <c r="S119" s="4"/>
-      <c r="T119" s="4"/>
-      <c r="U119" s="4"/>
-      <c r="V119" s="4"/>
-      <c r="W119" s="4"/>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3"/>
+      <c r="O119" s="3"/>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="3"/>
+      <c r="T119" s="3"/>
+      <c r="U119" s="3"/>
+      <c r="V119" s="3"/>
+      <c r="W119" s="3"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -4439,94 +4455,94 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
-      <c r="M121" s="3"/>
-      <c r="N121" s="3"/>
-      <c r="O121" s="3"/>
-      <c r="P121" s="3"/>
-      <c r="Q121" s="3"/>
-      <c r="R121" s="3"/>
-      <c r="S121" s="3"/>
-      <c r="T121" s="3"/>
-      <c r="U121" s="3"/>
-      <c r="V121" s="3"/>
-      <c r="W121" s="3"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="4"/>
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+      <c r="R121" s="4"/>
+      <c r="S121" s="4"/>
+      <c r="T121" s="4"/>
+      <c r="U121" s="4"/>
+      <c r="V121" s="4"/>
+      <c r="W121" s="4"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3"/>
-      <c r="Q122" s="3"/>
-      <c r="R122" s="3"/>
-      <c r="S122" s="3"/>
-      <c r="T122" s="3"/>
-      <c r="U122" s="3"/>
-      <c r="V122" s="3"/>
-      <c r="W122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="4"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+      <c r="U122" s="4"/>
+      <c r="V122" s="4"/>
+      <c r="W122" s="4"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="4"/>
-      <c r="N123" s="4"/>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
-      <c r="S123" s="4"/>
-      <c r="T123" s="4"/>
-      <c r="U123" s="4"/>
-      <c r="V123" s="4"/>
-      <c r="W123" s="4"/>
+      <c r="M123" s="3"/>
+      <c r="N123" s="3"/>
+      <c r="O123" s="3"/>
+      <c r="P123" s="3"/>
+      <c r="Q123" s="3"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="3"/>
+      <c r="T123" s="3"/>
+      <c r="U123" s="3"/>
+      <c r="V123" s="3"/>
+      <c r="W123" s="3"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>359</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -4547,13 +4563,13 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
@@ -4573,26 +4589,42 @@
       <c r="W125" s="4"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="B126" s="4"/>
+      <c r="A126" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
-      <c r="M126" s="4"/>
-      <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-      <c r="R126" s="4"/>
-      <c r="S126" s="4"/>
-      <c r="T126" s="4"/>
-      <c r="U126" s="4"/>
-      <c r="V126" s="4"/>
-      <c r="W126" s="4"/>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="3"/>
+      <c r="T126" s="3"/>
+      <c r="U126" s="3"/>
+      <c r="V126" s="3"/>
+      <c r="W126" s="3"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="B127" s="4"/>
+      <c r="A127" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>367</v>
+      </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>

</xml_diff>

<commit_message>
Gray icons created for each skill when not known. Hover/rollover descriptions for skills added, descriptions for feedback fleshed out.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C65">
+    <comment authorId="0" ref="C70">
       <text>
         <t xml:space="preserve">?????Avere una visione d'insieme, attenzione, percezione sensoriale
 	-Ellis Spice</t>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="388">
   <si>
     <t>Key</t>
   </si>
@@ -74,6 +74,21 @@
     <t>Forza</t>
   </si>
   <si>
+    <t>BODY_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Strength - physical fitness and endurance</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
+    <t>BODY_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in strength</t>
+  </si>
+  <si>
     <t>BOWMAN</t>
   </si>
   <si>
@@ -110,6 +125,18 @@
     <t>Carisma</t>
   </si>
   <si>
+    <t>CHARISMA_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Charisma - ability to speak and lead</t>
+  </si>
+  <si>
+    <t>CHARISMA_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in charisma</t>
+  </si>
+  <si>
     <t>CORRECT</t>
   </si>
   <si>
@@ -128,13 +155,10 @@
     <t>Crea il gioco</t>
   </si>
   <si>
-    <t>CREW_OPINION</t>
-  </si>
-  <si>
-    <t>Crew Opinion</t>
-  </si>
-  <si>
-    <t>Opinione dell'equipaggio</t>
+    <t>CREW_OPINION_FEEDBACK</t>
+  </si>
+  <si>
+    <t>An effective line-up who like each other more could have been chosen</t>
   </si>
   <si>
     <t>ENGLISH</t>
@@ -227,10 +251,7 @@
     <t>GREEN_PLACEMENT</t>
   </si>
   <si>
-    <t>Ideal Placements</t>
-  </si>
-  <si>
-    <t>Collocazioni ideali</t>
+    <t>Number positioned correctly compared to the best possible line-up</t>
   </si>
   <si>
     <t>GRINDER</t>
@@ -275,13 +296,10 @@
     <t>Aiuto</t>
   </si>
   <si>
-    <t>HIDDEN</t>
-  </si>
-  <si>
-    <t>Hidden</t>
-  </si>
-  <si>
-    <t>Nascosto</t>
+    <t>HIDDEN_FEEDBACK</t>
+  </si>
+  <si>
+    <t>Speak to your team in order to reveal information and avoid hidden feedback</t>
   </si>
   <si>
     <t>HIRE_WARNING_NOT_POSSIBLE</t>
@@ -407,6 +425,12 @@
     <t>Opinione del coach</t>
   </si>
   <si>
+    <t>MANAGER_OPINION_FEEDBACK</t>
+  </si>
+  <si>
+    <t>An effective line-up who like you more could have been chosen</t>
+  </si>
+  <si>
     <t>MEETING_EARLY_EXIT</t>
   </si>
   <si>
@@ -470,13 +494,10 @@
     <t>Ripiega le vele sottocoperta e aiuta nel cambio della vela. Chi e occupa questa posizione deve essere fisicamente prestante, agile ed essere in grado di sopportare il caldo, il buio e l'umidità.</t>
   </si>
   <si>
-    <t>MOOD</t>
-  </si>
-  <si>
-    <t>Mood</t>
-  </si>
-  <si>
-    <t>Umore</t>
+    <t>MOOD_FEEDBACK</t>
+  </si>
+  <si>
+    <t>An effective line-up who are in a better mood could have been chosen</t>
   </si>
   <si>
     <t>MUSIC</t>
@@ -591,6 +612,18 @@
     <t>Percezione</t>
   </si>
   <si>
+    <t>PERCEPTION_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Perception - situational awareness and ability to think outside the box</t>
+  </si>
+  <si>
+    <t>PERCEPTION_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in perception</t>
+  </si>
+  <si>
     <t>PITMAN</t>
   </si>
   <si>
@@ -751,6 +784,18 @@
   </si>
   <si>
     <t>Velocità</t>
+  </si>
+  <si>
+    <t>QUICKNESS_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Quickness - reactions and agility.</t>
+  </si>
+  <si>
+    <t>QUICKNESS_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in quickness</t>
   </si>
   <si>
     <t>RACE_BUTTON_PRACTICE</t>
@@ -815,9 +860,6 @@
 You also have {0} Talk Time remaining, which will be lost if not used before racing.</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
     <t>RACE_SKIP_CONFIRM_NO_ALLOWANCE</t>
   </si>
   <si>
@@ -902,10 +944,7 @@
     <t>RED_PLACEMENT</t>
   </si>
   <si>
-    <t>Unideal Placements</t>
-  </si>
-  <si>
-    <t>Posizioni non ideali</t>
+    <t>Number positioned that are not featured in the best possible line-up</t>
   </si>
   <si>
     <t>REPEAT_CONFIRM</t>
@@ -1101,6 +1140,18 @@
     <t>Forza di volontà</t>
   </si>
   <si>
+    <t>WILLPOWER_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Willpower - ability to keep calm under pressure</t>
+  </si>
+  <si>
+    <t>WILLPOWER_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in willpower</t>
+  </si>
+  <si>
     <t>WISDOM</t>
   </si>
   <si>
@@ -1110,13 +1161,22 @@
     <t>Saggezza</t>
   </si>
   <si>
+    <t>WISDOM_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Wisdom - decision making and judgement</t>
+  </si>
+  <si>
+    <t>WISDOM_FEEDBACK</t>
+  </si>
+  <si>
+    <t>This line-up was lacking in wisdom</t>
+  </si>
+  <si>
     <t>YELLOW_PLACEMENT</t>
   </si>
   <si>
-    <t>Ideal In Another Position</t>
-  </si>
-  <si>
-    <t>Ideale in un'altra posizione</t>
+    <t>Number positioned that feature in the best possible line-up in another position</t>
   </si>
   <si>
     <t>YES</t>
@@ -1141,20 +1201,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1168,7 +1238,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1182,6 +1252,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1362,27 +1438,27 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1403,13 +1479,13 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1430,40 +1506,40 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1484,13 +1560,13 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1510,14 +1586,14 @@
       <c r="W11" s="3"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1537,14 +1613,14 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
+      <c r="A13" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1565,10 +1641,10 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>38</v>
@@ -1618,230 +1694,230 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1862,13 +1938,13 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1889,13 +1965,13 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1916,40 +1992,40 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1970,40 +2046,40 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2024,13 +2100,13 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2051,13 +2127,13 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2078,46 +2154,46 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>93</v>
+      <c r="A34" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -2132,13 +2208,13 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2159,40 +2235,40 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2213,13 +2289,13 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2240,40 +2316,40 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2294,67 +2370,67 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -2375,13 +2451,13 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -2402,67 +2478,67 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
-      <c r="W46" s="4"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -2482,20 +2558,20 @@
       <c r="W47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
+      <c r="A48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -2509,20 +2585,20 @@
       <c r="W48" s="4"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>138</v>
+      <c r="A49" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
@@ -2537,13 +2613,13 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -2564,13 +2640,13 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -2591,40 +2667,40 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
-      <c r="Q52" s="4"/>
-      <c r="R52" s="4"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
-      <c r="U52" s="4"/>
-      <c r="V52" s="4"/>
-      <c r="W52" s="4"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -2645,13 +2721,13 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -2672,40 +2748,40 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -2725,20 +2801,20 @@
       <c r="W56" s="4"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>162</v>
+      <c r="A57" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -2753,40 +2829,40 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
@@ -2807,67 +2883,67 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
-      <c r="V60" s="4"/>
-      <c r="W60" s="4"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -2888,13 +2964,13 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -2915,13 +2991,13 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -2942,68 +3018,67 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="4"/>
+      <c r="W65" s="4"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
-      <c r="V66" s="4"/>
-      <c r="W66" s="4"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -3024,40 +3099,40 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
-      <c r="U68" s="4"/>
-      <c r="V68" s="4"/>
-      <c r="W68" s="4"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -3078,67 +3153,69 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>201</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D70" s="1"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
-      <c r="U70" s="4"/>
-      <c r="V70" s="4"/>
-      <c r="W70" s="4"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>204</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="1"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-      <c r="S71" s="4"/>
-      <c r="T71" s="4"/>
-      <c r="U71" s="4"/>
-      <c r="V71" s="4"/>
-      <c r="W71" s="4"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+      <c r="W71" s="3"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="2" t="s">
-        <v>205</v>
+      <c r="A72" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>207</v>
+        <v>197</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3159,13 +3236,13 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3186,13 +3263,13 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3213,13 +3290,13 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -3240,13 +3317,13 @@
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -3267,13 +3344,13 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3294,67 +3371,67 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-      <c r="Q78" s="3"/>
-      <c r="R78" s="3"/>
-      <c r="S78" s="3"/>
-      <c r="T78" s="3"/>
-      <c r="U78" s="3"/>
-      <c r="V78" s="3"/>
-      <c r="W78" s="3"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="4"/>
+      <c r="W78" s="4"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
-      <c r="Q79" s="3"/>
-      <c r="R79" s="3"/>
-      <c r="S79" s="3"/>
-      <c r="T79" s="3"/>
-      <c r="U79" s="3"/>
-      <c r="V79" s="3"/>
-      <c r="W79" s="3"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="4"/>
+      <c r="V79" s="4"/>
+      <c r="W79" s="4"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3375,13 +3452,13 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -3402,13 +3479,13 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -3429,40 +3506,40 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="3"/>
-      <c r="P83" s="3"/>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="3"/>
-      <c r="S83" s="3"/>
-      <c r="T83" s="3"/>
-      <c r="U83" s="3"/>
-      <c r="V83" s="3"/>
-      <c r="W83" s="3"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="4"/>
+      <c r="S83" s="4"/>
+      <c r="T83" s="4"/>
+      <c r="U83" s="4"/>
+      <c r="V83" s="4"/>
+      <c r="W83" s="4"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3483,67 +3560,67 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="4"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
-      <c r="U86" s="4"/>
-      <c r="V86" s="4"/>
-      <c r="W86" s="4"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3564,13 +3641,13 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3591,13 +3668,13 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3618,94 +3695,94 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
-      <c r="M90" s="4"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
-      <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-      <c r="S90" s="4"/>
-      <c r="T90" s="4"/>
-      <c r="U90" s="4"/>
-      <c r="V90" s="4"/>
-      <c r="W90" s="4"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>261</v>
+        <v>17</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
-      <c r="Q91" s="4"/>
-      <c r="R91" s="4"/>
-      <c r="S91" s="4"/>
-      <c r="T91" s="4"/>
-      <c r="U91" s="4"/>
-      <c r="V91" s="4"/>
-      <c r="W91" s="4"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="2" t="s">
-        <v>264</v>
+      <c r="A92" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
-      <c r="Q92" s="3"/>
-      <c r="R92" s="3"/>
-      <c r="S92" s="3"/>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-      <c r="W92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="4"/>
+      <c r="S92" s="4"/>
+      <c r="T92" s="4"/>
+      <c r="U92" s="4"/>
+      <c r="V92" s="4"/>
+      <c r="W92" s="4"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3726,13 +3803,13 @@
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -3753,13 +3830,13 @@
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -3780,13 +3857,13 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -3807,13 +3884,13 @@
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -3834,13 +3911,13 @@
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -3861,40 +3938,40 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>285</v>
+        <v>17</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="T99" s="3"/>
-      <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
-      <c r="W99" s="3"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="4"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+      <c r="U99" s="4"/>
+      <c r="V99" s="4"/>
+      <c r="W99" s="4"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>288</v>
+        <v>17</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -3915,40 +3992,40 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="2" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="4"/>
-      <c r="R101" s="4"/>
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
-      <c r="U101" s="4"/>
-      <c r="V101" s="4"/>
-      <c r="W101" s="4"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="2" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -3969,148 +4046,148 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
-      <c r="M103" s="3"/>
-      <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3"/>
-      <c r="Q103" s="3"/>
-      <c r="R103" s="3"/>
-      <c r="S103" s="3"/>
-      <c r="T103" s="3"/>
-      <c r="U103" s="3"/>
-      <c r="V103" s="3"/>
-      <c r="W103" s="3"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="4"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+      <c r="U103" s="4"/>
+      <c r="V103" s="4"/>
+      <c r="W103" s="4"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="2" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
-      <c r="M104" s="3"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="3"/>
-      <c r="P104" s="3"/>
-      <c r="Q104" s="3"/>
-      <c r="R104" s="3"/>
-      <c r="S104" s="3"/>
-      <c r="T104" s="3"/>
-      <c r="U104" s="3"/>
-      <c r="V104" s="3"/>
-      <c r="W104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+      <c r="U104" s="4"/>
+      <c r="V104" s="4"/>
+      <c r="W104" s="4"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
-      <c r="M105" s="3"/>
-      <c r="N105" s="3"/>
-      <c r="O105" s="3"/>
-      <c r="P105" s="3"/>
-      <c r="Q105" s="3"/>
-      <c r="R105" s="3"/>
-      <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+      <c r="U105" s="4"/>
+      <c r="V105" s="4"/>
+      <c r="W105" s="4"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
-      <c r="M106" s="3"/>
-      <c r="N106" s="3"/>
-      <c r="O106" s="3"/>
-      <c r="P106" s="3"/>
-      <c r="Q106" s="3"/>
-      <c r="R106" s="3"/>
-      <c r="S106" s="3"/>
-      <c r="T106" s="3"/>
-      <c r="U106" s="3"/>
-      <c r="V106" s="3"/>
-      <c r="W106" s="3"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="4"/>
+      <c r="S106" s="4"/>
+      <c r="T106" s="4"/>
+      <c r="U106" s="4"/>
+      <c r="V106" s="4"/>
+      <c r="W106" s="4"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+      <c r="V107" s="4"/>
+      <c r="W107" s="4"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -4131,13 +4208,13 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="2" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
@@ -4158,13 +4235,13 @@
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>318</v>
+        <v>17</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
@@ -4185,148 +4262,148 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-      <c r="P111" s="3"/>
-      <c r="Q111" s="3"/>
-      <c r="R111" s="3"/>
-      <c r="S111" s="3"/>
-      <c r="T111" s="3"/>
-      <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
-      <c r="W111" s="3"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4"/>
+      <c r="V111" s="4"/>
+      <c r="W111" s="4"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
-      <c r="M112" s="4"/>
-      <c r="N112" s="4"/>
-      <c r="O112" s="4"/>
-      <c r="P112" s="4"/>
-      <c r="Q112" s="4"/>
-      <c r="R112" s="4"/>
-      <c r="S112" s="4"/>
-      <c r="T112" s="4"/>
-      <c r="U112" s="4"/>
-      <c r="V112" s="4"/>
-      <c r="W112" s="4"/>
+      <c r="M112" s="3"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="3"/>
+      <c r="P112" s="3"/>
+      <c r="Q112" s="3"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="3"/>
+      <c r="T112" s="3"/>
+      <c r="U112" s="3"/>
+      <c r="V112" s="3"/>
+      <c r="W112" s="3"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
-      <c r="M113" s="4"/>
-      <c r="N113" s="4"/>
-      <c r="O113" s="4"/>
-      <c r="P113" s="4"/>
-      <c r="Q113" s="4"/>
-      <c r="R113" s="4"/>
-      <c r="S113" s="4"/>
-      <c r="T113" s="4"/>
-      <c r="U113" s="4"/>
-      <c r="V113" s="4"/>
-      <c r="W113" s="4"/>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3"/>
+      <c r="O113" s="3"/>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="3"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="3"/>
+      <c r="T113" s="3"/>
+      <c r="U113" s="3"/>
+      <c r="V113" s="3"/>
+      <c r="W113" s="3"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
-      <c r="R114" s="4"/>
-      <c r="S114" s="4"/>
-      <c r="T114" s="4"/>
-      <c r="U114" s="4"/>
-      <c r="V114" s="4"/>
-      <c r="W114" s="4"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="3"/>
+      <c r="T114" s="3"/>
+      <c r="U114" s="3"/>
+      <c r="V114" s="3"/>
+      <c r="W114" s="3"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
-      <c r="M115" s="4"/>
-      <c r="N115" s="4"/>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
-      <c r="Q115" s="4"/>
-      <c r="R115" s="4"/>
-      <c r="S115" s="4"/>
-      <c r="T115" s="4"/>
-      <c r="U115" s="4"/>
-      <c r="V115" s="4"/>
-      <c r="W115" s="4"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="3"/>
+      <c r="T115" s="3"/>
+      <c r="U115" s="3"/>
+      <c r="V115" s="3"/>
+      <c r="W115" s="3"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -4347,13 +4424,13 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -4374,94 +4451,94 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3"/>
-      <c r="Q118" s="3"/>
-      <c r="R118" s="3"/>
-      <c r="S118" s="3"/>
-      <c r="T118" s="3"/>
-      <c r="U118" s="3"/>
-      <c r="V118" s="3"/>
-      <c r="W118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
-      <c r="M119" s="3"/>
-      <c r="N119" s="3"/>
-      <c r="O119" s="3"/>
-      <c r="P119" s="3"/>
-      <c r="Q119" s="3"/>
-      <c r="R119" s="3"/>
-      <c r="S119" s="3"/>
-      <c r="T119" s="3"/>
-      <c r="U119" s="3"/>
-      <c r="V119" s="3"/>
-      <c r="W119" s="3"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="4"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+      <c r="U119" s="4"/>
+      <c r="V119" s="4"/>
+      <c r="W119" s="4"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-      <c r="S120" s="4"/>
-      <c r="T120" s="4"/>
-      <c r="U120" s="4"/>
-      <c r="V120" s="4"/>
-      <c r="W120" s="4"/>
+      <c r="M120" s="3"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="3"/>
+      <c r="P120" s="3"/>
+      <c r="Q120" s="3"/>
+      <c r="R120" s="3"/>
+      <c r="S120" s="3"/>
+      <c r="T120" s="3"/>
+      <c r="U120" s="3"/>
+      <c r="V120" s="3"/>
+      <c r="W120" s="3"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -4482,13 +4559,13 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -4509,94 +4586,94 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
-      <c r="O123" s="3"/>
-      <c r="P123" s="3"/>
-      <c r="Q123" s="3"/>
-      <c r="R123" s="3"/>
-      <c r="S123" s="3"/>
-      <c r="T123" s="3"/>
-      <c r="U123" s="3"/>
-      <c r="V123" s="3"/>
-      <c r="W123" s="3"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="4"/>
+      <c r="S123" s="4"/>
+      <c r="T123" s="4"/>
+      <c r="U123" s="4"/>
+      <c r="V123" s="4"/>
+      <c r="W123" s="4"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
-      <c r="O124" s="3"/>
-      <c r="P124" s="3"/>
-      <c r="Q124" s="3"/>
-      <c r="R124" s="3"/>
-      <c r="S124" s="3"/>
-      <c r="T124" s="3"/>
-      <c r="U124" s="3"/>
-      <c r="V124" s="3"/>
-      <c r="W124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="4"/>
+      <c r="S124" s="4"/>
+      <c r="T124" s="4"/>
+      <c r="U124" s="4"/>
+      <c r="V124" s="4"/>
+      <c r="W124" s="4"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
-      <c r="M125" s="4"/>
-      <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
-      <c r="Q125" s="4"/>
-      <c r="R125" s="4"/>
-      <c r="S125" s="4"/>
-      <c r="T125" s="4"/>
-      <c r="U125" s="4"/>
-      <c r="V125" s="4"/>
-      <c r="W125" s="4"/>
+      <c r="M125" s="3"/>
+      <c r="N125" s="3"/>
+      <c r="O125" s="3"/>
+      <c r="P125" s="3"/>
+      <c r="Q125" s="3"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="3"/>
+      <c r="T125" s="3"/>
+      <c r="U125" s="3"/>
+      <c r="V125" s="3"/>
+      <c r="W125" s="3"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -4617,52 +4694,68 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
-      <c r="M127" s="4"/>
-      <c r="N127" s="4"/>
-      <c r="O127" s="4"/>
-      <c r="P127" s="4"/>
-      <c r="Q127" s="4"/>
-      <c r="R127" s="4"/>
-      <c r="S127" s="4"/>
-      <c r="T127" s="4"/>
-      <c r="U127" s="4"/>
-      <c r="V127" s="4"/>
-      <c r="W127" s="4"/>
+      <c r="M127" s="3"/>
+      <c r="N127" s="3"/>
+      <c r="O127" s="3"/>
+      <c r="P127" s="3"/>
+      <c r="Q127" s="3"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="3"/>
+      <c r="T127" s="3"/>
+      <c r="U127" s="3"/>
+      <c r="V127" s="3"/>
+      <c r="W127" s="3"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
-      <c r="B128" s="4"/>
+      <c r="A128" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
-      <c r="M128" s="4"/>
-      <c r="N128" s="4"/>
-      <c r="O128" s="4"/>
-      <c r="P128" s="4"/>
-      <c r="Q128" s="4"/>
-      <c r="R128" s="4"/>
-      <c r="S128" s="4"/>
-      <c r="T128" s="4"/>
-      <c r="U128" s="4"/>
-      <c r="V128" s="4"/>
-      <c r="W128" s="4"/>
+      <c r="M128" s="3"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="3"/>
+      <c r="P128" s="3"/>
+      <c r="Q128" s="3"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="3"/>
+      <c r="T128" s="3"/>
+      <c r="U128" s="3"/>
+      <c r="V128" s="3"/>
+      <c r="W128" s="3"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="B129" s="4"/>
+      <c r="A129" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>359</v>
+      </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
@@ -4681,7 +4774,15 @@
       <c r="W129" s="4"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="B130" s="4"/>
+      <c r="A130" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
@@ -4700,7 +4801,15 @@
       <c r="W130" s="4"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="B131" s="4"/>
+      <c r="A131" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
@@ -4719,50 +4828,74 @@
       <c r="W131" s="4"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="B132" s="4"/>
+      <c r="A132" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>368</v>
+      </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
-      <c r="Q132" s="4"/>
-      <c r="R132" s="4"/>
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
-      <c r="U132" s="4"/>
-      <c r="V132" s="4"/>
-      <c r="W132" s="4"/>
+      <c r="M132" s="3"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="3"/>
+      <c r="P132" s="3"/>
+      <c r="Q132" s="3"/>
+      <c r="R132" s="3"/>
+      <c r="S132" s="3"/>
+      <c r="T132" s="3"/>
+      <c r="U132" s="3"/>
+      <c r="V132" s="3"/>
+      <c r="W132" s="3"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="B133" s="4"/>
+      <c r="A133" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
-      <c r="M133" s="4"/>
-      <c r="N133" s="4"/>
-      <c r="O133" s="4"/>
-      <c r="P133" s="4"/>
-      <c r="Q133" s="4"/>
-      <c r="R133" s="4"/>
-      <c r="S133" s="4"/>
-      <c r="T133" s="4"/>
-      <c r="U133" s="4"/>
-      <c r="V133" s="4"/>
-      <c r="W133" s="4"/>
+      <c r="M133" s="3"/>
+      <c r="N133" s="3"/>
+      <c r="O133" s="3"/>
+      <c r="P133" s="3"/>
+      <c r="Q133" s="3"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="3"/>
+      <c r="T133" s="3"/>
+      <c r="U133" s="3"/>
+      <c r="V133" s="3"/>
+      <c r="W133" s="3"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="B134" s="4"/>
-      <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-      <c r="L134" s="4"/>
+      <c r="A134" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
       <c r="O134" s="4"/>
@@ -4776,50 +4909,74 @@
       <c r="W134" s="4"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="B135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-      <c r="L135" s="4"/>
-      <c r="M135" s="4"/>
-      <c r="N135" s="4"/>
-      <c r="O135" s="4"/>
-      <c r="P135" s="4"/>
-      <c r="Q135" s="4"/>
-      <c r="R135" s="4"/>
-      <c r="S135" s="4"/>
-      <c r="T135" s="4"/>
-      <c r="U135" s="4"/>
-      <c r="V135" s="4"/>
-      <c r="W135" s="4"/>
+      <c r="A135" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+      <c r="M135" s="3"/>
+      <c r="N135" s="3"/>
+      <c r="O135" s="3"/>
+      <c r="P135" s="3"/>
+      <c r="Q135" s="3"/>
+      <c r="R135" s="3"/>
+      <c r="S135" s="3"/>
+      <c r="T135" s="3"/>
+      <c r="U135" s="3"/>
+      <c r="V135" s="3"/>
+      <c r="W135" s="3"/>
     </row>
     <row r="136" ht="14.25" customHeight="1">
-      <c r="B136" s="4"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="4"/>
-      <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
-      <c r="N136" s="4"/>
-      <c r="O136" s="4"/>
-      <c r="P136" s="4"/>
-      <c r="Q136" s="4"/>
-      <c r="R136" s="4"/>
-      <c r="S136" s="4"/>
-      <c r="T136" s="4"/>
-      <c r="U136" s="4"/>
-      <c r="V136" s="4"/>
-      <c r="W136" s="4"/>
+      <c r="A136" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+      <c r="M136" s="3"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="3"/>
+      <c r="P136" s="3"/>
+      <c r="Q136" s="3"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="3"/>
+      <c r="T136" s="3"/>
+      <c r="U136" s="3"/>
+      <c r="V136" s="3"/>
+      <c r="W136" s="3"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="B137" s="4"/>
-      <c r="H137" s="4"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="4"/>
+      <c r="A137" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
       <c r="M137" s="4"/>
       <c r="N137" s="4"/>
       <c r="O137" s="4"/>
@@ -4833,12 +4990,20 @@
       <c r="W137" s="4"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="B138" s="4"/>
-      <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
+      <c r="A138" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
       <c r="M138" s="4"/>
       <c r="N138" s="4"/>
       <c r="O138" s="4"/>
@@ -4852,31 +5017,47 @@
       <c r="W138" s="4"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="B139" s="4"/>
-      <c r="H139" s="4"/>
-      <c r="I139" s="4"/>
-      <c r="J139" s="4"/>
-      <c r="K139" s="4"/>
-      <c r="L139" s="4"/>
-      <c r="M139" s="4"/>
-      <c r="N139" s="4"/>
-      <c r="O139" s="4"/>
-      <c r="P139" s="4"/>
-      <c r="Q139" s="4"/>
-      <c r="R139" s="4"/>
-      <c r="S139" s="4"/>
-      <c r="T139" s="4"/>
-      <c r="U139" s="4"/>
-      <c r="V139" s="4"/>
-      <c r="W139" s="4"/>
+      <c r="A139" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="3"/>
+      <c r="M139" s="3"/>
+      <c r="N139" s="3"/>
+      <c r="O139" s="3"/>
+      <c r="P139" s="3"/>
+      <c r="Q139" s="3"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="3"/>
+      <c r="T139" s="3"/>
+      <c r="U139" s="3"/>
+      <c r="V139" s="3"/>
+      <c r="W139" s="3"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="B140" s="4"/>
-      <c r="H140" s="4"/>
-      <c r="I140" s="4"/>
-      <c r="J140" s="4"/>
-      <c r="K140" s="4"/>
-      <c r="L140" s="4"/>
+      <c r="A140" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
       <c r="M140" s="4"/>
       <c r="N140" s="4"/>
       <c r="O140" s="4"/>
@@ -5099,13 +5280,7 @@
       <c r="W151" s="4"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" s="3"/>
-      <c r="B152" s="3"/>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="4"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="4"/>
+      <c r="B152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -5124,13 +5299,7 @@
       <c r="W152" s="4"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" s="3"/>
-      <c r="B153" s="3"/>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="4"/>
-      <c r="F153" s="4"/>
-      <c r="G153" s="4"/>
+      <c r="B153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
@@ -5149,13 +5318,7 @@
       <c r="W153" s="4"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" s="3"/>
-      <c r="B154" s="3"/>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4"/>
-      <c r="E154" s="4"/>
-      <c r="F154" s="4"/>
-      <c r="G154" s="4"/>
+      <c r="B154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -26273,6 +26436,81 @@
       <c r="V998" s="4"/>
       <c r="W998" s="4"/>
     </row>
+    <row r="999" ht="14.25" customHeight="1">
+      <c r="A999" s="3"/>
+      <c r="B999" s="3"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
+      <c r="L999" s="4"/>
+      <c r="M999" s="4"/>
+      <c r="N999" s="4"/>
+      <c r="O999" s="4"/>
+      <c r="P999" s="4"/>
+      <c r="Q999" s="4"/>
+      <c r="R999" s="4"/>
+      <c r="S999" s="4"/>
+      <c r="T999" s="4"/>
+      <c r="U999" s="4"/>
+      <c r="V999" s="4"/>
+      <c r="W999" s="4"/>
+    </row>
+    <row r="1000" ht="14.25" customHeight="1">
+      <c r="A1000" s="3"/>
+      <c r="B1000" s="3"/>
+      <c r="C1000" s="4"/>
+      <c r="D1000" s="4"/>
+      <c r="E1000" s="4"/>
+      <c r="F1000" s="4"/>
+      <c r="G1000" s="4"/>
+      <c r="H1000" s="4"/>
+      <c r="I1000" s="4"/>
+      <c r="J1000" s="4"/>
+      <c r="K1000" s="4"/>
+      <c r="L1000" s="4"/>
+      <c r="M1000" s="4"/>
+      <c r="N1000" s="4"/>
+      <c r="O1000" s="4"/>
+      <c r="P1000" s="4"/>
+      <c r="Q1000" s="4"/>
+      <c r="R1000" s="4"/>
+      <c r="S1000" s="4"/>
+      <c r="T1000" s="4"/>
+      <c r="U1000" s="4"/>
+      <c r="V1000" s="4"/>
+      <c r="W1000" s="4"/>
+    </row>
+    <row r="1001" ht="14.25" customHeight="1">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="4"/>
+      <c r="D1001" s="4"/>
+      <c r="E1001" s="4"/>
+      <c r="F1001" s="4"/>
+      <c r="G1001" s="4"/>
+      <c r="H1001" s="4"/>
+      <c r="I1001" s="4"/>
+      <c r="J1001" s="4"/>
+      <c r="K1001" s="4"/>
+      <c r="L1001" s="4"/>
+      <c r="M1001" s="4"/>
+      <c r="N1001" s="4"/>
+      <c r="O1001" s="4"/>
+      <c r="P1001" s="4"/>
+      <c r="Q1001" s="4"/>
+      <c r="R1001" s="4"/>
+      <c r="S1001" s="4"/>
+      <c r="T1001" s="4"/>
+      <c r="U1001" s="4"/>
+      <c r="V1001" s="4"/>
+      <c r="W1001" s="4"/>
+    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Final result screen created.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C107">
+    <comment authorId="0" ref="C109">
       <text>
         <t xml:space="preserve">?????Avere una visione d'insieme, attenzione, percezione sensoriale
 	-Ellis Spice</t>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="517">
   <si>
     <t>Key</t>
   </si>
@@ -476,6 +476,12 @@
     <t>Esci</t>
   </si>
   <si>
+    <t>EXIT_GAME</t>
+  </si>
+  <si>
+    <t>Exit Game</t>
+  </si>
+  <si>
     <t>FEEDBACK</t>
   </si>
   <si>
@@ -507,6 +513,15 @@
   </si>
   <si>
     <t>Final Result</t>
+  </si>
+  <si>
+    <t>FINAL_RESULT_TEXT</t>
+  </si>
+  <si>
+    <t>In this game we found that your prevailing style is:</t>
+  </si>
+  <si>
+    <t>Nel gioco è emerso che il tuo stile prevalente è:</t>
   </si>
   <si>
     <t>FIRE</t>
@@ -3081,113 +3096,117 @@
       <c r="A47" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
-      <c r="V50" s="4"/>
-      <c r="W50" s="4"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1" t="s">
@@ -3217,47 +3236,51 @@
       <c r="W51" s="4"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
@@ -3272,40 +3295,40 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
-      <c r="Q54" s="4"/>
-      <c r="R54" s="4"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="4"/>
-      <c r="V54" s="4"/>
-      <c r="W54" s="4"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -3326,13 +3349,13 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -3353,40 +3376,40 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -3413,34 +3436,34 @@
         <v>161</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
@@ -3467,7 +3490,7 @@
         <v>166</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -3488,13 +3511,13 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -3515,46 +3538,46 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-      <c r="Q63" s="3"/>
-      <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
@@ -3568,51 +3591,47 @@
       <c r="W64" s="4"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-      <c r="U65" s="4"/>
-      <c r="V65" s="4"/>
-      <c r="W65" s="4"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
+      <c r="C66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
@@ -3626,20 +3645,24 @@
       <c r="W66" s="4"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
@@ -3654,10 +3677,10 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>186</v>
@@ -3680,20 +3703,20 @@
       <c r="W68" s="4"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
+        <v>189</v>
+      </c>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
@@ -3707,24 +3730,20 @@
       <c r="W69" s="4"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B70" s="5" t="s">
+      <c r="A70" s="2" t="s">
         <v>190</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
@@ -3738,20 +3757,20 @@
       <c r="W70" s="4"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
@@ -3765,20 +3784,24 @@
       <c r="W71" s="4"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
@@ -3792,20 +3815,20 @@
       <c r="W72" s="4"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
@@ -3819,24 +3842,20 @@
       <c r="W73" s="4"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
       <c r="O74" s="4"/>
@@ -3850,47 +3869,51 @@
       <c r="W74" s="4"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="4"/>
+      <c r="U75" s="4"/>
+      <c r="V75" s="4"/>
+      <c r="W75" s="4"/>
+    </row>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
-      <c r="R75" s="3"/>
-      <c r="S75" s="3"/>
-      <c r="T75" s="3"/>
-      <c r="U75" s="3"/>
-      <c r="V75" s="3"/>
-      <c r="W75" s="3"/>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="2" t="s">
+      <c r="B76" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
@@ -3905,50 +3928,46 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
-      <c r="S77" s="4"/>
-      <c r="T77" s="4"/>
-      <c r="U77" s="4"/>
-      <c r="V77" s="4"/>
-      <c r="W77" s="4"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="C78" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
       <c r="O78" s="4"/>
@@ -3963,67 +3982,71 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
-      <c r="Q79" s="3"/>
-      <c r="R79" s="3"/>
-      <c r="S79" s="3"/>
-      <c r="T79" s="3"/>
-      <c r="U79" s="3"/>
-      <c r="V79" s="3"/>
-      <c r="W79" s="3"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="4"/>
+      <c r="V79" s="4"/>
+      <c r="W79" s="4"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
-      <c r="Q80" s="3"/>
-      <c r="R80" s="3"/>
-      <c r="S80" s="3"/>
-      <c r="T80" s="3"/>
-      <c r="U80" s="3"/>
-      <c r="V80" s="3"/>
-      <c r="W80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -4044,13 +4067,13 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -4071,13 +4094,13 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -4097,74 +4120,74 @@
       <c r="W83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="C84" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="3"/>
+      <c r="T84" s="3"/>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+      <c r="W84" s="3"/>
+    </row>
+    <row r="85" ht="14.25" customHeight="1">
+      <c r="A85" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="4"/>
-      <c r="R84" s="4"/>
-      <c r="S84" s="4"/>
-      <c r="T84" s="4"/>
-      <c r="U84" s="4"/>
-      <c r="V84" s="4"/>
-      <c r="W84" s="4"/>
-    </row>
-    <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="4"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
       <c r="O86" s="4"/>
@@ -4178,20 +4201,20 @@
       <c r="W86" s="4"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
+      <c r="C87" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
       <c r="O87" s="4"/>
@@ -4206,40 +4229,40 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="3"/>
-      <c r="P88" s="3"/>
-      <c r="Q88" s="3"/>
-      <c r="R88" s="3"/>
-      <c r="S88" s="3"/>
-      <c r="T88" s="3"/>
-      <c r="U88" s="3"/>
-      <c r="V88" s="3"/>
-      <c r="W88" s="3"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+      <c r="U88" s="4"/>
+      <c r="V88" s="4"/>
+      <c r="W88" s="4"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -4260,40 +4283,40 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
-      <c r="M90" s="4"/>
-      <c r="N90" s="4"/>
-      <c r="O90" s="4"/>
-      <c r="P90" s="4"/>
-      <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-      <c r="S90" s="4"/>
-      <c r="T90" s="4"/>
-      <c r="U90" s="4"/>
-      <c r="V90" s="4"/>
-      <c r="W90" s="4"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -4314,13 +4337,13 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -4340,20 +4363,20 @@
       <c r="W92" s="4"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
       <c r="O93" s="4"/>
@@ -4394,20 +4417,20 @@
       <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="1" t="s">
         <v>261</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
+      <c r="C95" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
@@ -4422,40 +4445,40 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
-      <c r="S96" s="3"/>
-      <c r="T96" s="3"/>
-      <c r="U96" s="3"/>
-      <c r="V96" s="3"/>
-      <c r="W96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+      <c r="U96" s="4"/>
+      <c r="V96" s="4"/>
+      <c r="W96" s="4"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4476,67 +4499,67 @@
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
-      <c r="M98" s="4"/>
-      <c r="N98" s="4"/>
-      <c r="O98" s="4"/>
-      <c r="P98" s="4"/>
-      <c r="Q98" s="4"/>
-      <c r="R98" s="4"/>
-      <c r="S98" s="4"/>
-      <c r="T98" s="4"/>
-      <c r="U98" s="4"/>
-      <c r="V98" s="4"/>
-      <c r="W98" s="4"/>
+      <c r="M98" s="3"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="3"/>
+      <c r="P98" s="3"/>
+      <c r="Q98" s="3"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="3"/>
+      <c r="T98" s="3"/>
+      <c r="U98" s="3"/>
+      <c r="V98" s="3"/>
+      <c r="W98" s="3"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="T99" s="3"/>
-      <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
-      <c r="W99" s="3"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="4"/>
+      <c r="S99" s="4"/>
+      <c r="T99" s="4"/>
+      <c r="U99" s="4"/>
+      <c r="V99" s="4"/>
+      <c r="W99" s="4"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -4557,46 +4580,46 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
-      <c r="M101" s="4"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="4"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="4"/>
-      <c r="R101" s="4"/>
-      <c r="S101" s="4"/>
-      <c r="T101" s="4"/>
-      <c r="U101" s="4"/>
-      <c r="V101" s="4"/>
-      <c r="W101" s="4"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="H102" s="4"/>
-      <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
-      <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
@@ -4611,10 +4634,10 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>286</v>
@@ -4624,33 +4647,33 @@
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
-      <c r="M103" s="3"/>
-      <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
-      <c r="P103" s="3"/>
-      <c r="Q103" s="3"/>
-      <c r="R103" s="3"/>
-      <c r="S103" s="3"/>
-      <c r="T103" s="3"/>
-      <c r="U103" s="3"/>
-      <c r="V103" s="3"/>
-      <c r="W103" s="3"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="4"/>
+      <c r="S103" s="4"/>
+      <c r="T103" s="4"/>
+      <c r="U103" s="4"/>
+      <c r="V103" s="4"/>
+      <c r="W103" s="4"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="H104" s="3"/>
-      <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="4"/>
@@ -4668,7 +4691,7 @@
         <v>290</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>291</v>
@@ -4722,12 +4745,11 @@
         <v>295</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D107" s="1"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
@@ -4747,95 +4769,96 @@
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D108" s="1"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
-      <c r="N108" s="3"/>
-      <c r="O108" s="3"/>
-      <c r="P108" s="3"/>
-      <c r="Q108" s="3"/>
-      <c r="R108" s="3"/>
-      <c r="S108" s="3"/>
-      <c r="T108" s="3"/>
-      <c r="U108" s="3"/>
-      <c r="V108" s="3"/>
-      <c r="W108" s="3"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="4"/>
+      <c r="S108" s="4"/>
+      <c r="T108" s="4"/>
+      <c r="U108" s="4"/>
+      <c r="V108" s="4"/>
+      <c r="W108" s="4"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="2" t="s">
         <v>300</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>301</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="D109" s="1"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
-      <c r="M109" s="4"/>
-      <c r="N109" s="4"/>
-      <c r="O109" s="4"/>
-      <c r="P109" s="4"/>
-      <c r="Q109" s="4"/>
-      <c r="R109" s="4"/>
-      <c r="S109" s="4"/>
-      <c r="T109" s="4"/>
-      <c r="U109" s="4"/>
-      <c r="V109" s="4"/>
-      <c r="W109" s="4"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3"/>
+      <c r="T109" s="3"/>
+      <c r="U109" s="3"/>
+      <c r="V109" s="3"/>
+      <c r="W109" s="3"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C110" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="C110" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D110" s="1"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
-      <c r="M110" s="4"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="4"/>
-      <c r="P110" s="4"/>
-      <c r="Q110" s="4"/>
-      <c r="R110" s="4"/>
-      <c r="S110" s="4"/>
-      <c r="T110" s="4"/>
-      <c r="U110" s="4"/>
-      <c r="V110" s="4"/>
-      <c r="W110" s="4"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="3"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="3"/>
+      <c r="T110" s="3"/>
+      <c r="U110" s="3"/>
+      <c r="V110" s="3"/>
+      <c r="W110" s="3"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>307</v>
+      <c r="C111" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
@@ -4856,13 +4879,13 @@
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -4883,13 +4906,13 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -4910,13 +4933,13 @@
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -4937,13 +4960,13 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -4964,13 +4987,13 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>322</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -4991,13 +5014,13 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -5018,13 +5041,13 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
@@ -5045,13 +5068,13 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
@@ -5072,13 +5095,13 @@
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>334</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -5099,13 +5122,13 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -5126,50 +5149,46 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3"/>
-      <c r="Q122" s="3"/>
-      <c r="R122" s="3"/>
-      <c r="S122" s="3"/>
-      <c r="T122" s="3"/>
-      <c r="U122" s="3"/>
-      <c r="V122" s="3"/>
-      <c r="W122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="4"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+      <c r="U122" s="4"/>
+      <c r="V122" s="4"/>
+      <c r="W122" s="4"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="C123" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
-      <c r="I123" s="4"/>
-      <c r="J123" s="4"/>
-      <c r="K123" s="4"/>
-      <c r="L123" s="4"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="3"/>
       <c r="M123" s="4"/>
       <c r="N123" s="4"/>
       <c r="O123" s="4"/>
@@ -5210,20 +5229,24 @@
       <c r="W124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="5" t="s">
         <v>347</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="3"/>
-      <c r="K125" s="3"/>
-      <c r="L125" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="4"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
       <c r="M125" s="4"/>
       <c r="N125" s="4"/>
       <c r="O125" s="4"/>
@@ -5238,40 +5261,40 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
-      <c r="M126" s="4"/>
-      <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-      <c r="R126" s="4"/>
-      <c r="S126" s="4"/>
-      <c r="T126" s="4"/>
-      <c r="U126" s="4"/>
-      <c r="V126" s="4"/>
-      <c r="W126" s="4"/>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="3"/>
+      <c r="T126" s="3"/>
+      <c r="U126" s="3"/>
+      <c r="V126" s="3"/>
+      <c r="W126" s="3"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -5292,121 +5315,121 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
-      <c r="M128" s="3"/>
-      <c r="N128" s="3"/>
-      <c r="O128" s="3"/>
-      <c r="P128" s="3"/>
-      <c r="Q128" s="3"/>
-      <c r="R128" s="3"/>
-      <c r="S128" s="3"/>
-      <c r="T128" s="3"/>
-      <c r="U128" s="3"/>
-      <c r="V128" s="3"/>
-      <c r="W128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="4"/>
+      <c r="S128" s="4"/>
+      <c r="T128" s="4"/>
+      <c r="U128" s="4"/>
+      <c r="V128" s="4"/>
+      <c r="W128" s="4"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
-      <c r="M129" s="3"/>
-      <c r="N129" s="3"/>
-      <c r="O129" s="3"/>
-      <c r="P129" s="3"/>
-      <c r="Q129" s="3"/>
-      <c r="R129" s="3"/>
-      <c r="S129" s="3"/>
-      <c r="T129" s="3"/>
-      <c r="U129" s="3"/>
-      <c r="V129" s="3"/>
-      <c r="W129" s="3"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="4"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+      <c r="U129" s="4"/>
+      <c r="V129" s="4"/>
+      <c r="W129" s="4"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="2" t="s">
         <v>360</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>47</v>
+      <c r="C130" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
-      <c r="M130" s="4"/>
-      <c r="N130" s="4"/>
-      <c r="O130" s="4"/>
-      <c r="P130" s="4"/>
-      <c r="Q130" s="4"/>
-      <c r="R130" s="4"/>
-      <c r="S130" s="4"/>
-      <c r="T130" s="4"/>
-      <c r="U130" s="4"/>
-      <c r="V130" s="4"/>
-      <c r="W130" s="4"/>
+      <c r="M130" s="3"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="3"/>
+      <c r="P130" s="3"/>
+      <c r="Q130" s="3"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="3"/>
+      <c r="T130" s="3"/>
+      <c r="U130" s="3"/>
+      <c r="V130" s="3"/>
+      <c r="W130" s="3"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>364</v>
+        <v>47</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
-      <c r="M131" s="4"/>
-      <c r="N131" s="4"/>
-      <c r="O131" s="4"/>
-      <c r="P131" s="4"/>
-      <c r="Q131" s="4"/>
-      <c r="R131" s="4"/>
-      <c r="S131" s="4"/>
-      <c r="T131" s="4"/>
-      <c r="U131" s="4"/>
-      <c r="V131" s="4"/>
-      <c r="W131" s="4"/>
+      <c r="M131" s="3"/>
+      <c r="N131" s="3"/>
+      <c r="O131" s="3"/>
+      <c r="P131" s="3"/>
+      <c r="Q131" s="3"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="3"/>
+      <c r="T131" s="3"/>
+      <c r="U131" s="3"/>
+      <c r="V131" s="3"/>
+      <c r="W131" s="3"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="1" t="s">
         <v>365</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>367</v>
+      <c r="C132" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -5427,13 +5450,13 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>370</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
@@ -5454,13 +5477,13 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
@@ -5481,13 +5504,13 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
@@ -5508,13 +5531,13 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -5535,13 +5558,13 @@
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
@@ -5568,7 +5591,7 @@
         <v>383</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>47</v>
+        <v>384</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -5589,30 +5612,30 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>386</v>
+        <v>47</v>
       </c>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
       <c r="L139" s="3"/>
-      <c r="M139" s="3"/>
-      <c r="N139" s="3"/>
-      <c r="O139" s="3"/>
-      <c r="P139" s="3"/>
-      <c r="Q139" s="3"/>
-      <c r="R139" s="3"/>
-      <c r="S139" s="3"/>
-      <c r="T139" s="3"/>
-      <c r="U139" s="3"/>
-      <c r="V139" s="3"/>
-      <c r="W139" s="3"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="4"/>
+      <c r="S139" s="4"/>
+      <c r="T139" s="4"/>
+      <c r="U139" s="4"/>
+      <c r="V139" s="4"/>
+      <c r="W139" s="4"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="2" t="s">
@@ -5622,7 +5645,7 @@
         <v>388</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>389</v>
+        <v>47</v>
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
@@ -5643,40 +5666,40 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
       <c r="L141" s="3"/>
-      <c r="M141" s="4"/>
-      <c r="N141" s="4"/>
-      <c r="O141" s="4"/>
-      <c r="P141" s="4"/>
-      <c r="Q141" s="4"/>
-      <c r="R141" s="4"/>
-      <c r="S141" s="4"/>
-      <c r="T141" s="4"/>
-      <c r="U141" s="4"/>
-      <c r="V141" s="4"/>
-      <c r="W141" s="4"/>
+      <c r="M141" s="3"/>
+      <c r="N141" s="3"/>
+      <c r="O141" s="3"/>
+      <c r="P141" s="3"/>
+      <c r="Q141" s="3"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="3"/>
+      <c r="T141" s="3"/>
+      <c r="U141" s="3"/>
+      <c r="V141" s="3"/>
+      <c r="W141" s="3"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
@@ -5697,10 +5720,10 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>397</v>
@@ -5730,7 +5753,7 @@
         <v>399</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
@@ -5751,10 +5774,10 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>402</v>
@@ -5784,34 +5807,34 @@
         <v>404</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
-      <c r="N146" s="3"/>
-      <c r="O146" s="3"/>
-      <c r="P146" s="3"/>
-      <c r="Q146" s="3"/>
-      <c r="R146" s="3"/>
-      <c r="S146" s="3"/>
-      <c r="T146" s="3"/>
-      <c r="U146" s="3"/>
-      <c r="V146" s="3"/>
-      <c r="W146" s="3"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="4"/>
+      <c r="S146" s="4"/>
+      <c r="T146" s="4"/>
+      <c r="U146" s="4"/>
+      <c r="V146" s="4"/>
+      <c r="W146" s="4"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
@@ -5832,30 +5855,30 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
       <c r="L148" s="3"/>
-      <c r="M148" s="4"/>
-      <c r="N148" s="4"/>
-      <c r="O148" s="4"/>
-      <c r="P148" s="4"/>
-      <c r="Q148" s="4"/>
-      <c r="R148" s="4"/>
-      <c r="S148" s="4"/>
-      <c r="T148" s="4"/>
-      <c r="U148" s="4"/>
-      <c r="V148" s="4"/>
-      <c r="W148" s="4"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="3"/>
+      <c r="P148" s="3"/>
+      <c r="Q148" s="3"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="3"/>
+      <c r="T148" s="3"/>
+      <c r="U148" s="3"/>
+      <c r="V148" s="3"/>
+      <c r="W148" s="3"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
@@ -5892,61 +5915,61 @@
         <v>415</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>416</v>
+        <v>47</v>
       </c>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
       <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
-      <c r="N150" s="3"/>
-      <c r="O150" s="3"/>
-      <c r="P150" s="3"/>
-      <c r="Q150" s="3"/>
-      <c r="R150" s="3"/>
-      <c r="S150" s="3"/>
-      <c r="T150" s="3"/>
-      <c r="U150" s="3"/>
-      <c r="V150" s="3"/>
-      <c r="W150" s="3"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4"/>
+      <c r="R150" s="4"/>
+      <c r="S150" s="4"/>
+      <c r="T150" s="4"/>
+      <c r="U150" s="4"/>
+      <c r="V150" s="4"/>
+      <c r="W150" s="4"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
-      <c r="O151" s="3"/>
-      <c r="P151" s="3"/>
-      <c r="Q151" s="3"/>
-      <c r="R151" s="3"/>
-      <c r="S151" s="3"/>
-      <c r="T151" s="3"/>
-      <c r="U151" s="3"/>
-      <c r="V151" s="3"/>
-      <c r="W151" s="3"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="4"/>
+      <c r="S151" s="4"/>
+      <c r="T151" s="4"/>
+      <c r="U151" s="4"/>
+      <c r="V151" s="4"/>
+      <c r="W151" s="4"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>422</v>
       </c>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
@@ -5967,13 +5990,13 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
@@ -5994,13 +6017,13 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="C154" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>428</v>
       </c>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
@@ -6021,13 +6044,13 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
@@ -6048,91 +6071,91 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>434</v>
       </c>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
-      <c r="M156" s="4"/>
-      <c r="N156" s="4"/>
-      <c r="O156" s="4"/>
-      <c r="P156" s="4"/>
-      <c r="Q156" s="4"/>
-      <c r="R156" s="4"/>
-      <c r="S156" s="4"/>
-      <c r="T156" s="4"/>
-      <c r="U156" s="4"/>
-      <c r="V156" s="4"/>
-      <c r="W156" s="4"/>
+      <c r="M156" s="3"/>
+      <c r="N156" s="3"/>
+      <c r="O156" s="3"/>
+      <c r="P156" s="3"/>
+      <c r="Q156" s="3"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="3"/>
+      <c r="T156" s="3"/>
+      <c r="U156" s="3"/>
+      <c r="V156" s="3"/>
+      <c r="W156" s="3"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
-      <c r="M157" s="4"/>
-      <c r="N157" s="4"/>
-      <c r="O157" s="4"/>
-      <c r="P157" s="4"/>
-      <c r="Q157" s="4"/>
-      <c r="R157" s="4"/>
-      <c r="S157" s="4"/>
-      <c r="T157" s="4"/>
-      <c r="U157" s="4"/>
-      <c r="V157" s="4"/>
-      <c r="W157" s="4"/>
+      <c r="M157" s="3"/>
+      <c r="N157" s="3"/>
+      <c r="O157" s="3"/>
+      <c r="P157" s="3"/>
+      <c r="Q157" s="3"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="3"/>
+      <c r="T157" s="3"/>
+      <c r="U157" s="3"/>
+      <c r="V157" s="3"/>
+      <c r="W157" s="3"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
-      <c r="M158" s="3"/>
-      <c r="N158" s="3"/>
-      <c r="O158" s="3"/>
-      <c r="P158" s="3"/>
-      <c r="Q158" s="3"/>
-      <c r="R158" s="3"/>
-      <c r="S158" s="3"/>
-      <c r="T158" s="3"/>
-      <c r="U158" s="3"/>
-      <c r="V158" s="3"/>
-      <c r="W158" s="3"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+      <c r="R158" s="4"/>
+      <c r="S158" s="4"/>
+      <c r="T158" s="4"/>
+      <c r="U158" s="4"/>
+      <c r="V158" s="4"/>
+      <c r="W158" s="4"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>442</v>
@@ -6169,17 +6192,17 @@
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
       <c r="L160" s="3"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="4"/>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
-      <c r="Q160" s="4"/>
-      <c r="R160" s="4"/>
-      <c r="S160" s="4"/>
-      <c r="T160" s="4"/>
-      <c r="U160" s="4"/>
-      <c r="V160" s="4"/>
-      <c r="W160" s="4"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="3"/>
+      <c r="T160" s="3"/>
+      <c r="U160" s="3"/>
+      <c r="V160" s="3"/>
+      <c r="W160" s="3"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
@@ -6189,7 +6212,7 @@
         <v>447</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
@@ -6210,10 +6233,10 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>450</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>450</v>
@@ -6250,17 +6273,17 @@
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
-      <c r="M163" s="3"/>
-      <c r="N163" s="3"/>
-      <c r="O163" s="3"/>
-      <c r="P163" s="3"/>
-      <c r="Q163" s="3"/>
-      <c r="R163" s="3"/>
-      <c r="S163" s="3"/>
-      <c r="T163" s="3"/>
-      <c r="U163" s="3"/>
-      <c r="V163" s="3"/>
-      <c r="W163" s="3"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="4"/>
+      <c r="O163" s="4"/>
+      <c r="P163" s="4"/>
+      <c r="Q163" s="4"/>
+      <c r="R163" s="4"/>
+      <c r="S163" s="4"/>
+      <c r="T163" s="4"/>
+      <c r="U163" s="4"/>
+      <c r="V163" s="4"/>
+      <c r="W163" s="4"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
@@ -6270,34 +6293,34 @@
         <v>455</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
-      <c r="M164" s="3"/>
-      <c r="N164" s="3"/>
-      <c r="O164" s="3"/>
-      <c r="P164" s="3"/>
-      <c r="Q164" s="3"/>
-      <c r="R164" s="3"/>
-      <c r="S164" s="3"/>
-      <c r="T164" s="3"/>
-      <c r="U164" s="3"/>
-      <c r="V164" s="3"/>
-      <c r="W164" s="3"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="4"/>
+      <c r="S164" s="4"/>
+      <c r="T164" s="4"/>
+      <c r="U164" s="4"/>
+      <c r="V164" s="4"/>
+      <c r="W164" s="4"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
@@ -6318,13 +6341,13 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>462</v>
       </c>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
@@ -6344,72 +6367,68 @@
       <c r="W166" s="3"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="A167" s="1" t="s">
+      <c r="A167" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="H167" s="3"/>
+      <c r="I167" s="3"/>
+      <c r="J167" s="3"/>
+      <c r="K167" s="3"/>
+      <c r="L167" s="3"/>
+      <c r="M167" s="3"/>
+      <c r="N167" s="3"/>
+      <c r="O167" s="3"/>
+      <c r="P167" s="3"/>
+      <c r="Q167" s="3"/>
+      <c r="R167" s="3"/>
+      <c r="S167" s="3"/>
+      <c r="T167" s="3"/>
+      <c r="U167" s="3"/>
+      <c r="V167" s="3"/>
+      <c r="W167" s="3"/>
+    </row>
+    <row r="168" ht="14.25" customHeight="1">
+      <c r="A168" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="H167" s="4"/>
-      <c r="I167" s="4"/>
-      <c r="J167" s="4"/>
-      <c r="K167" s="4"/>
-      <c r="L167" s="4"/>
-      <c r="M167" s="4"/>
-      <c r="N167" s="4"/>
-      <c r="O167" s="4"/>
-      <c r="P167" s="4"/>
-      <c r="Q167" s="4"/>
-      <c r="R167" s="4"/>
-      <c r="S167" s="4"/>
-      <c r="T167" s="4"/>
-      <c r="U167" s="4"/>
-      <c r="V167" s="4"/>
-      <c r="W167" s="4"/>
-    </row>
-    <row r="168" ht="14.25" customHeight="1">
-      <c r="A168" s="1" t="s">
+      <c r="B168" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="C168" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="D168" s="4"/>
-      <c r="E168" s="4"/>
-      <c r="F168" s="4"/>
-      <c r="G168" s="4"/>
-      <c r="H168" s="4"/>
-      <c r="I168" s="4"/>
-      <c r="J168" s="4"/>
-      <c r="K168" s="4"/>
-      <c r="L168" s="4"/>
-      <c r="M168" s="4"/>
-      <c r="N168" s="4"/>
-      <c r="O168" s="4"/>
-      <c r="P168" s="4"/>
-      <c r="Q168" s="4"/>
-      <c r="R168" s="4"/>
-      <c r="S168" s="4"/>
-      <c r="T168" s="4"/>
-      <c r="U168" s="4"/>
-      <c r="V168" s="4"/>
-      <c r="W168" s="4"/>
+      <c r="H168" s="3"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="3"/>
+      <c r="K168" s="3"/>
+      <c r="L168" s="3"/>
+      <c r="M168" s="3"/>
+      <c r="N168" s="3"/>
+      <c r="O168" s="3"/>
+      <c r="P168" s="3"/>
+      <c r="Q168" s="3"/>
+      <c r="R168" s="3"/>
+      <c r="S168" s="3"/>
+      <c r="T168" s="3"/>
+      <c r="U168" s="3"/>
+      <c r="V168" s="3"/>
+      <c r="W168" s="3"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="C169" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6430,13 +6449,13 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B170" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="C170" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -6460,20 +6479,20 @@
       <c r="W170" s="4"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C171" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="H171" s="3"/>
-      <c r="I171" s="3"/>
-      <c r="J171" s="3"/>
-      <c r="K171" s="3"/>
-      <c r="L171" s="3"/>
+      <c r="H171" s="4"/>
+      <c r="I171" s="4"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="4"/>
       <c r="M171" s="4"/>
       <c r="N171" s="4"/>
       <c r="O171" s="4"/>
@@ -6487,20 +6506,24 @@
       <c r="W171" s="4"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="2" t="s">
+      <c r="A172" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B172" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="H172" s="3"/>
-      <c r="I172" s="3"/>
-      <c r="J172" s="3"/>
-      <c r="K172" s="3"/>
-      <c r="L172" s="3"/>
+      <c r="D172" s="4"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="4"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="4"/>
+      <c r="I172" s="4"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="4"/>
+      <c r="L172" s="4"/>
       <c r="M172" s="4"/>
       <c r="N172" s="4"/>
       <c r="O172" s="4"/>
@@ -6515,13 +6538,13 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
@@ -6541,24 +6564,20 @@
       <c r="W173" s="4"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="5" t="s">
+      <c r="A174" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B174" s="5" t="s">
+      <c r="C174" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="C174" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D174" s="4"/>
-      <c r="E174" s="4"/>
-      <c r="F174" s="4"/>
-      <c r="G174" s="4"/>
-      <c r="H174" s="4"/>
-      <c r="I174" s="4"/>
-      <c r="J174" s="4"/>
-      <c r="K174" s="4"/>
-      <c r="L174" s="4"/>
+      <c r="H174" s="3"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+      <c r="L174" s="3"/>
       <c r="M174" s="4"/>
       <c r="N174" s="4"/>
       <c r="O174" s="4"/>
@@ -6572,24 +6591,20 @@
       <c r="W174" s="4"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" s="5" t="s">
+      <c r="A175" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B175" s="5" t="s">
+      <c r="C175" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="C175" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
-      <c r="L175" s="4"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="3"/>
+      <c r="K175" s="3"/>
+      <c r="L175" s="3"/>
       <c r="M175" s="4"/>
       <c r="N175" s="4"/>
       <c r="O175" s="4"/>
@@ -6603,95 +6618,103 @@
       <c r="W175" s="4"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B176" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="C176" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="4"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+      <c r="U176" s="4"/>
+      <c r="V176" s="4"/>
+      <c r="W176" s="4"/>
+    </row>
+    <row r="177" ht="14.25" customHeight="1">
+      <c r="A177" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="H176" s="3"/>
-      <c r="I176" s="3"/>
-      <c r="J176" s="3"/>
-      <c r="K176" s="3"/>
-      <c r="L176" s="3"/>
-      <c r="M176" s="3"/>
-      <c r="N176" s="3"/>
-      <c r="O176" s="3"/>
-      <c r="P176" s="3"/>
-      <c r="Q176" s="3"/>
-      <c r="R176" s="3"/>
-      <c r="S176" s="3"/>
-      <c r="T176" s="3"/>
-      <c r="U176" s="3"/>
-      <c r="V176" s="3"/>
-      <c r="W176" s="3"/>
-    </row>
-    <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="2" t="s">
+      <c r="B177" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="C177" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H177" s="3"/>
-      <c r="I177" s="3"/>
-      <c r="J177" s="3"/>
-      <c r="K177" s="3"/>
-      <c r="L177" s="3"/>
-      <c r="M177" s="3"/>
-      <c r="N177" s="3"/>
-      <c r="O177" s="3"/>
-      <c r="P177" s="3"/>
-      <c r="Q177" s="3"/>
-      <c r="R177" s="3"/>
-      <c r="S177" s="3"/>
-      <c r="T177" s="3"/>
-      <c r="U177" s="3"/>
-      <c r="V177" s="3"/>
-      <c r="W177" s="3"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="4"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+      <c r="U177" s="4"/>
+      <c r="V177" s="4"/>
+      <c r="W177" s="4"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="2" t="s">
         <v>495</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>47</v>
+      <c r="C178" s="2" t="s">
+        <v>497</v>
       </c>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
       <c r="L178" s="3"/>
-      <c r="M178" s="4"/>
-      <c r="N178" s="4"/>
-      <c r="O178" s="4"/>
-      <c r="P178" s="4"/>
-      <c r="Q178" s="4"/>
-      <c r="R178" s="4"/>
-      <c r="S178" s="4"/>
-      <c r="T178" s="4"/>
-      <c r="U178" s="4"/>
-      <c r="V178" s="4"/>
-      <c r="W178" s="4"/>
+      <c r="M178" s="3"/>
+      <c r="N178" s="3"/>
+      <c r="O178" s="3"/>
+      <c r="P178" s="3"/>
+      <c r="Q178" s="3"/>
+      <c r="R178" s="3"/>
+      <c r="S178" s="3"/>
+      <c r="T178" s="3"/>
+      <c r="U178" s="3"/>
+      <c r="V178" s="3"/>
+      <c r="W178" s="3"/>
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>499</v>
+        <v>47</v>
       </c>
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
@@ -6711,13 +6734,13 @@
       <c r="W179" s="3"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="2" t="s">
+      <c r="A180" s="1" t="s">
         <v>500</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C180" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H180" s="3"/>
@@ -6725,51 +6748,51 @@
       <c r="J180" s="3"/>
       <c r="K180" s="3"/>
       <c r="L180" s="3"/>
-      <c r="M180" s="3"/>
-      <c r="N180" s="3"/>
-      <c r="O180" s="3"/>
-      <c r="P180" s="3"/>
-      <c r="Q180" s="3"/>
-      <c r="R180" s="3"/>
-      <c r="S180" s="3"/>
-      <c r="T180" s="3"/>
-      <c r="U180" s="3"/>
-      <c r="V180" s="3"/>
-      <c r="W180" s="3"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="4"/>
+      <c r="S180" s="4"/>
+      <c r="T180" s="4"/>
+      <c r="U180" s="4"/>
+      <c r="V180" s="4"/>
+      <c r="W180" s="4"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="1" t="s">
+      <c r="A181" s="2" t="s">
         <v>502</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="C181" s="1" t="s">
-        <v>47</v>
+      <c r="C181" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3"/>
       <c r="L181" s="3"/>
-      <c r="M181" s="4"/>
-      <c r="N181" s="4"/>
-      <c r="O181" s="4"/>
-      <c r="P181" s="4"/>
-      <c r="Q181" s="4"/>
-      <c r="R181" s="4"/>
-      <c r="S181" s="4"/>
-      <c r="T181" s="4"/>
-      <c r="U181" s="4"/>
-      <c r="V181" s="4"/>
-      <c r="W181" s="4"/>
+      <c r="M181" s="3"/>
+      <c r="N181" s="3"/>
+      <c r="O181" s="3"/>
+      <c r="P181" s="3"/>
+      <c r="Q181" s="3"/>
+      <c r="R181" s="3"/>
+      <c r="S181" s="3"/>
+      <c r="T181" s="3"/>
+      <c r="U181" s="3"/>
+      <c r="V181" s="3"/>
+      <c r="W181" s="3"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>47</v>
@@ -6779,44 +6802,44 @@
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
       <c r="L182" s="3"/>
-      <c r="M182" s="4"/>
-      <c r="N182" s="4"/>
-      <c r="O182" s="4"/>
-      <c r="P182" s="4"/>
-      <c r="Q182" s="4"/>
-      <c r="R182" s="4"/>
-      <c r="S182" s="4"/>
-      <c r="T182" s="4"/>
-      <c r="U182" s="4"/>
-      <c r="V182" s="4"/>
-      <c r="W182" s="4"/>
+      <c r="M182" s="3"/>
+      <c r="N182" s="3"/>
+      <c r="O182" s="3"/>
+      <c r="P182" s="3"/>
+      <c r="Q182" s="3"/>
+      <c r="R182" s="3"/>
+      <c r="S182" s="3"/>
+      <c r="T182" s="3"/>
+      <c r="U182" s="3"/>
+      <c r="V182" s="3"/>
+      <c r="W182" s="3"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="A183" s="2" t="s">
-        <v>506</v>
+      <c r="A183" s="1" t="s">
+        <v>507</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="C183" s="2" t="s">
         <v>508</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
       <c r="K183" s="3"/>
       <c r="L183" s="3"/>
-      <c r="M183" s="3"/>
-      <c r="N183" s="3"/>
-      <c r="O183" s="3"/>
-      <c r="P183" s="3"/>
-      <c r="Q183" s="3"/>
-      <c r="R183" s="3"/>
-      <c r="S183" s="3"/>
-      <c r="T183" s="3"/>
-      <c r="U183" s="3"/>
-      <c r="V183" s="3"/>
-      <c r="W183" s="3"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="4"/>
+      <c r="S183" s="4"/>
+      <c r="T183" s="4"/>
+      <c r="U183" s="4"/>
+      <c r="V183" s="4"/>
+      <c r="W183" s="4"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="2" t="s">
@@ -6826,7 +6849,7 @@
         <v>510</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>511</v>
+        <v>47</v>
       </c>
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
@@ -6846,43 +6869,47 @@
       <c r="W184" s="4"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="A185" s="3"/>
-      <c r="B185" s="3"/>
-      <c r="C185" s="4"/>
-      <c r="D185" s="4"/>
-      <c r="E185" s="4"/>
-      <c r="F185" s="4"/>
-      <c r="G185" s="4"/>
-      <c r="H185" s="4"/>
-      <c r="I185" s="4"/>
-      <c r="J185" s="4"/>
-      <c r="K185" s="4"/>
-      <c r="L185" s="4"/>
-      <c r="M185" s="4"/>
-      <c r="N185" s="4"/>
-      <c r="O185" s="4"/>
-      <c r="P185" s="4"/>
-      <c r="Q185" s="4"/>
-      <c r="R185" s="4"/>
-      <c r="S185" s="4"/>
-      <c r="T185" s="4"/>
-      <c r="U185" s="4"/>
-      <c r="V185" s="4"/>
-      <c r="W185" s="4"/>
+      <c r="A185" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="3"/>
+      <c r="K185" s="3"/>
+      <c r="L185" s="3"/>
+      <c r="M185" s="3"/>
+      <c r="N185" s="3"/>
+      <c r="O185" s="3"/>
+      <c r="P185" s="3"/>
+      <c r="Q185" s="3"/>
+      <c r="R185" s="3"/>
+      <c r="S185" s="3"/>
+      <c r="T185" s="3"/>
+      <c r="U185" s="3"/>
+      <c r="V185" s="3"/>
+      <c r="W185" s="3"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="A186" s="3"/>
-      <c r="B186" s="3"/>
-      <c r="C186" s="4"/>
-      <c r="D186" s="4"/>
-      <c r="E186" s="4"/>
-      <c r="F186" s="4"/>
-      <c r="G186" s="4"/>
-      <c r="H186" s="4"/>
-      <c r="I186" s="4"/>
-      <c r="J186" s="4"/>
-      <c r="K186" s="4"/>
-      <c r="L186" s="4"/>
+      <c r="A186" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3"/>
       <c r="M186" s="4"/>
       <c r="N186" s="4"/>
       <c r="O186" s="4"/>

</xml_diff>

<commit_message>
Latest version of SUGAR Unity asset now in use. Utilities contained within now in use instead of separate scripts
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
@@ -27,15 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="518">
   <si>
     <t>Key</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Italian</t>
+    <t>en-gb</t>
+  </si>
+  <si>
+    <t>it</t>
   </si>
   <si>
     <t>ACCOMMODATING</t>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
   <si>
     <t>EXCLAIMATION_MARK</t>
@@ -1750,7 +1753,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -3016,10 +3019,10 @@
         <v>123</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -3040,13 +3043,13 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3067,13 +3070,13 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -3094,10 +3097,10 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>47</v>
@@ -3125,13 +3128,13 @@
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -3152,10 +3155,10 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>47</v>
@@ -3183,13 +3186,13 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -3210,10 +3213,10 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>47</v>
@@ -3237,10 +3240,10 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>47</v>
@@ -3264,13 +3267,13 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -3295,13 +3298,13 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -3322,13 +3325,13 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -3349,13 +3352,13 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -3376,13 +3379,13 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -3403,13 +3406,13 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -3430,13 +3433,13 @@
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
@@ -3457,10 +3460,10 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>47</v>
@@ -3484,13 +3487,13 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -3511,13 +3514,13 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -3538,13 +3541,13 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -3565,13 +3568,13 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -3592,13 +3595,13 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -3619,10 +3622,10 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>47</v>
@@ -3646,13 +3649,13 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3677,13 +3680,13 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3704,13 +3707,13 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -3731,13 +3734,13 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3758,13 +3761,13 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -3785,13 +3788,13 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3816,13 +3819,13 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3843,13 +3846,13 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3870,10 +3873,10 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>47</v>
@@ -3897,13 +3900,13 @@
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3928,13 +3931,13 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3955,13 +3958,13 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -3982,13 +3985,13 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -4009,13 +4012,13 @@
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -4040,13 +4043,13 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -4067,13 +4070,13 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -4094,13 +4097,13 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -4121,13 +4124,13 @@
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -4148,13 +4151,13 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -4175,13 +4178,13 @@
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -4202,10 +4205,10 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>47</v>
@@ -4229,13 +4232,13 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -4256,13 +4259,13 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -4283,13 +4286,13 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -4310,13 +4313,13 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -4337,13 +4340,13 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -4364,13 +4367,13 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -4391,13 +4394,13 @@
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -4418,10 +4421,10 @@
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>47</v>
@@ -4445,13 +4448,13 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
@@ -4472,13 +4475,13 @@
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4499,13 +4502,13 @@
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -4526,13 +4529,13 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
@@ -4553,13 +4556,13 @@
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -4580,13 +4583,13 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -4607,13 +4610,13 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -4634,13 +4637,13 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -4661,13 +4664,13 @@
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -4688,13 +4691,13 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -4715,13 +4718,13 @@
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -4742,13 +4745,13 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
@@ -4769,13 +4772,13 @@
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -4796,13 +4799,13 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D109" s="1"/>
       <c r="H109" s="3"/>
@@ -4824,10 +4827,10 @@
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>47</v>
@@ -4852,10 +4855,10 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>47</v>
@@ -4879,13 +4882,13 @@
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -4906,13 +4909,13 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -4933,13 +4936,13 @@
     </row>
     <row r="114" ht="14.25" customHeight="1">
       <c r="A114" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -4960,13 +4963,13 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -4987,13 +4990,13 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -5014,13 +5017,13 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -5041,13 +5044,13 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
@@ -5068,13 +5071,13 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
@@ -5095,13 +5098,13 @@
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -5122,13 +5125,13 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -5149,13 +5152,13 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -5176,13 +5179,13 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
@@ -5203,13 +5206,13 @@
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -5230,10 +5233,10 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="5" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>47</v>
@@ -5261,13 +5264,13 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -5288,13 +5291,13 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -5315,13 +5318,13 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
@@ -5342,13 +5345,13 @@
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
@@ -5369,13 +5372,13 @@
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
@@ -5396,10 +5399,10 @@
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>47</v>
@@ -5423,10 +5426,10 @@
     </row>
     <row r="132" ht="14.25" customHeight="1">
       <c r="A132" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>47</v>
@@ -5450,13 +5453,13 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
@@ -5477,13 +5480,13 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
@@ -5504,13 +5507,13 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
@@ -5531,13 +5534,13 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -5558,13 +5561,13 @@
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
@@ -5585,13 +5588,13 @@
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -5612,10 +5615,10 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>47</v>
@@ -5639,10 +5642,10 @@
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>47</v>
@@ -5666,13 +5669,13 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
@@ -5693,13 +5696,13 @@
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
@@ -5720,13 +5723,13 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
@@ -5747,13 +5750,13 @@
     </row>
     <row r="144" ht="14.25" customHeight="1">
       <c r="A144" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
@@ -5774,13 +5777,13 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
@@ -5801,13 +5804,13 @@
     </row>
     <row r="146" ht="14.25" customHeight="1">
       <c r="A146" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
@@ -5828,13 +5831,13 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
@@ -5855,13 +5858,13 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
@@ -5882,13 +5885,13 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
@@ -5909,10 +5912,10 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>47</v>
@@ -5936,13 +5939,13 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
@@ -5963,13 +5966,13 @@
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
@@ -5990,13 +5993,13 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
@@ -6017,13 +6020,13 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
@@ -6044,13 +6047,13 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
@@ -6071,13 +6074,13 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
@@ -6098,13 +6101,13 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
@@ -6125,13 +6128,13 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
@@ -6152,13 +6155,13 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
@@ -6179,13 +6182,13 @@
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
@@ -6206,13 +6209,13 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
@@ -6233,13 +6236,13 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
@@ -6260,13 +6263,13 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
@@ -6287,13 +6290,13 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
@@ -6314,13 +6317,13 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
@@ -6341,13 +6344,13 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
@@ -6368,13 +6371,13 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H167" s="3"/>
       <c r="I167" s="3"/>
@@ -6395,13 +6398,13 @@
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="H168" s="3"/>
       <c r="I168" s="3"/>
@@ -6422,13 +6425,13 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6449,13 +6452,13 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -6480,13 +6483,13 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -6507,13 +6510,13 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -6538,13 +6541,13 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H173" s="3"/>
       <c r="I173" s="3"/>
@@ -6565,13 +6568,13 @@
     </row>
     <row r="174" ht="14.25" customHeight="1">
       <c r="A174" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
@@ -6592,13 +6595,13 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H175" s="3"/>
       <c r="I175" s="3"/>
@@ -6619,13 +6622,13 @@
     </row>
     <row r="176" ht="14.25" customHeight="1">
       <c r="A176" s="5" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -6650,13 +6653,13 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="5" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -6681,13 +6684,13 @@
     </row>
     <row r="178" ht="14.25" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
@@ -6708,10 +6711,10 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>47</v>
@@ -6735,10 +6738,10 @@
     </row>
     <row r="180" ht="14.25" customHeight="1">
       <c r="A180" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>47</v>
@@ -6762,13 +6765,13 @@
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
@@ -6789,10 +6792,10 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>47</v>
@@ -6816,10 +6819,10 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>47</v>
@@ -6843,10 +6846,10 @@
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>47</v>
@@ -6870,13 +6873,13 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
@@ -6897,13 +6900,13 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>

</xml_diff>

<commit_message>
Bug fixes, questionnaire introduction added
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="529">
   <si>
     <t>Key</t>
   </si>
@@ -1698,6 +1698,17 @@
   </si>
   <si>
     <t>Questionario Conflitto</t>
+  </si>
+  <si>
+    <t>QUESTIONNAIRE_INTRO</t>
+  </si>
+  <si>
+    <t>Picture yourself in a situation where your wishes differ from that of another person.
+For each of the following 30 statements, choose either A or B (with a circle) as the one which best describes how you would respond. Sometimes neither the A or B statement is typical of your response but try to choose the one that would seem most likely to be your instinctive response in that situation. Only you will see the finished exercise.</t>
+  </si>
+  <si>
+    <t>Ti verranno proposte 30 coppie di affermazioni, che descrivono possibili risposte comportamentali in situazioni di conflitto. Di volta in volta, scegli l’alternativa più vera per te tra A o B.
+A volte né A né B potrebbero corrispondere al tuo comportamento, scegli comunque l’alternativa che più si avvicina al tuo modo di fare.</t>
   </si>
 </sst>
 </file>
@@ -7043,9 +7054,15 @@
       <c r="W189" s="4"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" s="3"/>
-      <c r="B190" s="3"/>
-      <c r="C190" s="4"/>
+      <c r="A190" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>528</v>
+      </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
       <c r="F190" s="4"/>
@@ -27317,31 +27334,6 @@
       <c r="V1000" s="4"/>
       <c r="W1000" s="4"/>
     </row>
-    <row r="1001" ht="14.25" customHeight="1">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="4"/>
-      <c r="D1001" s="4"/>
-      <c r="E1001" s="4"/>
-      <c r="F1001" s="4"/>
-      <c r="G1001" s="4"/>
-      <c r="H1001" s="4"/>
-      <c r="I1001" s="4"/>
-      <c r="J1001" s="4"/>
-      <c r="K1001" s="4"/>
-      <c r="L1001" s="4"/>
-      <c r="M1001" s="4"/>
-      <c r="N1001" s="4"/>
-      <c r="O1001" s="4"/>
-      <c r="P1001" s="4"/>
-      <c r="Q1001" s="4"/>
-      <c r="R1001" s="4"/>
-      <c r="S1001" s="4"/>
-      <c r="T1001" s="4"/>
-      <c r="U1001" s="4"/>
-      <c r="V1001" s="4"/>
-      <c r="W1001" s="4"/>
-    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Improvements made to English localization of text translated from Italian
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C109">
+    <comment authorId="0" ref="C110">
       <text>
         <t xml:space="preserve">?????Avere una visione d'insieme, attenzione, percezione sensoriale
 	-Ellis Spice</t>
@@ -50,7 +50,7 @@
     <t>ACCOMMODATING_DESCRIPTION</t>
   </si>
   <si>
-    <t>The person neglects their own interests to meet those of others. This implies an aspect of self-sacrifice. The individual who exercises this style can be generous or selfless, obedient to the demands of others even when you disagree, or surrenders to the other's point of view.
+    <t>A person who neglects their own interests to meet those of others, which implies an aspect of self-sacrifice. An individual who exercises this style can be generous or selfless, obedient to the demands of others even when they disagree, or surrenders to the other's point of view.
 Intended use:
 When the other party is the expert or has a better solution. It can also be effective in preserving future relations with the other party.</t>
   </si>
@@ -63,7 +63,7 @@
     <t>ACCOMMODATING_QUESTIONS_HIGH</t>
   </si>
   <si>
-    <t>Do you feel that your ideas and your problems do not receive the proper attention?
+    <t>Do you feel that your ideas and problems do not receive proper attention?
 Do you seem to be too permissive?</t>
   </si>
   <si>
@@ -75,7 +75,7 @@
   </si>
   <si>
     <t>Do you sometimes find it difficult to admit that you are wrong?
-Do you recognize that there are legitimate exceptions to the rules?
+Do you recognize that there are legitimate exceptions to rules?
 Do you know when to admit you were wrong?</t>
   </si>
   <si>
@@ -143,10 +143,10 @@
     <t>AVOIDING_DESCRIPTION</t>
   </si>
   <si>
-    <t>The individual does not immediately pursue their own interests or those of another. Rather, they avoid conflict. Avoidance can take the form of diplomatically ignoring a problem, postponing it until a convenient time or simply withdrawing from a threatening situation.
+    <t>A person who does not immediately pursue their own interests or those of another, instead avoiding conflict. Avoidance can take the form of diplomatically ignoring a problem, postponing it until a convenient time or simply withdrawing from a threatening situation.
 Intended use:
 When the problem is not very important, such as when there are other more important issues to deal with, or when you have no chance of winning;
-It can also be effective when the problem would be very expensive to deal with (the cost is much higher benefits) or when others are emotionally charged and require a certain space;
+It can also be effective when the problem would be very expensive to deal with (the cost is much higher than the benefits) or when others are emotionally charged and require a certain space;
 When others are able to resolve the conflict in a more effective way.
 Sometimes problems will resolve themselves, but hope is not a strategy, and above all avoidance is not a good strategy in the long run.</t>
   </si>
@@ -216,7 +216,7 @@
     <t>BOWMAN_DESCRIPTION</t>
   </si>
   <si>
-    <t>Awareness, fast reactions and being able to handle fear is required here, as those in this position will need to climb the maist/bow to help chnage the sails.</t>
+    <t>Awareness, fast reactions and being able to handle fear is required here, as those in this position will need to climb the maist/bow to help change the sails.</t>
   </si>
   <si>
     <t>Consapevolezza, capacità di reagire rapidamente e di gestire la paura sono richiesti per questa posizione. Chi ricoprirà questo ruolo dovrà salire sull'albero per aiutare a cambiare le vele.</t>
@@ -270,7 +270,7 @@
     <t>COLLABORATING_DESCRIPTION</t>
   </si>
   <si>
-    <t>The individual tries to cooperate with others to find a solution that can meet the needs of both parties. It involves the deepening of the problem in order to identify underlying issues perceived by the parties involved and find an alternative that can satisfy the needs of both.
+    <t>An individual who tries to cooperate with others to find a solution that can meet the needs of both parties. It involves looking deeper into the problem in order to identify underlying issues perceived by the parties involved and find an alternative that can satisfy the needs of both.
 The cooperation between two individuals may take the form of exploring the disagreement in an attempt to learn from each other, for a resolution of a specific condition otherwise likely to cause a competition for resources, or comparison and search for a solution creative of an interpersonal problem.
 Intended use:
 In complex situations when you need to find a new and innovative solution. This may involve a redefinition of the problem bringing out everyone's ideas. It requires a high level of confidence, a lot of time and effort to convince all and synthesize ideas.</t>
@@ -316,7 +316,7 @@
     <t>COMPETING_DESCRIPTION</t>
   </si>
   <si>
-    <t>The person pursues their own interests by using any form of power to get what they want, be it to defend their rights, to defend a position which they believe is correct or to just attempt to win or prevail over others.
+    <t>A person who pursues their own interests by using any form of power to get what they want, be it to defend their rights, to defend a position which they believe is correct or to just attempt to win or prevail over others.
 Intended use:
 In emergency situations when you need to take a decisive decision quickly and other people are aware of this and thus approve the adoption of this style.</t>
   </si>
@@ -360,7 +360,7 @@
     <t>COMPROMISING_DESCRIPTION</t>
   </si>
   <si>
-    <t>The person trying to reach a compromise, the goal is to find an expedient, mutually acceptable solution which partially meets the needs of both parties. The search for a compromise represents a middle ground between the competition and the arrangement in the sense that you give up a little more than when you compete, but less than if you adopt an accommodating behavior. Similarly, the issue is addressed more directly than avoidance, but you do not get to develop it as with the collaboration. The compromise may mean finding an agreement in the middle, make mutual concessions, or look for a solution that represents a middle ground.
+    <t>A person who tries to reach a compromise, a mutually acceptable solution which partially meets the needs of both parties. The search for a compromise represents a middle ground between the competition and the arrangement in the sense that you give up a little more than when you compete, but less than if you adopt an accommodating behavior. Similarly, the issue is addressed more directly than avoidance, but you do not get to develop it as with the collaboration. The compromise may mean finding an agreement in the middle, make mutual concessions, or look for a solution that represents a middle ground.
 Intended use:
 When you need a temporary solution or when both sides have equally important objectives. The trap is easy to fall into the compromise as a way out when in fact the collaboration would produce a better solution.</t>
   </si>
@@ -414,6 +414,15 @@
 </t>
   </si>
   <si>
+    <t>CONFLICT_QUESTIONNAIRE</t>
+  </si>
+  <si>
+    <t>Conflict Questionnaire</t>
+  </si>
+  <si>
+    <t>Questionario Conflitto</t>
+  </si>
+  <si>
     <t>COOPERATIVITY</t>
   </si>
   <si>
@@ -678,7 +687,7 @@
   </si>
   <si>
     <t>This style is characterized by:
-A content exchange with the group and its attention to the growth of the individual;
+An exchange with the group and its attention to the growth of the individual;
 The renunciation of responsibility, postpone the decision, the non-return feedback;
 Operating minimal effort to meet the needs of others.</t>
   </si>
@@ -719,7 +728,7 @@
     <t>The conflict management styles can be matched with three leadership styles. The two main dimensions are:
 1. Watching out for yourself, focusing on your own needs and interests;
 2. Watching out for others, focusing on the needs and interests of others.
-The combination of these results in three leadership styles represented below. If you are curious to find out more you can read a description of each by clicking on the images.</t>
+The combination of these results in three leadership styles is represented below. If you are curious to find out more you can read a description of each by clicking on the images.</t>
   </si>
   <si>
     <t xml:space="preserve">Agli stili di gestione del conflitto sono stati abbinati tre stili di gestione della leadership. Le due dimensioni principali sono:
@@ -1195,6 +1204,17 @@
     <t>Domanda</t>
   </si>
   <si>
+    <t>QUESTIONNAIRE_INTRO</t>
+  </si>
+  <si>
+    <t>Picture yourself in a situation where your wishes differ from that of another person.
+For each of the following 30 statements, choose either A or B (with a circle) as the one which best describes how you would respond. Sometimes neither the A or B statement is typical of your response but try to choose the one that would seem most likely to be your instinctive response in that situation. Only you will see the finished exercise.</t>
+  </si>
+  <si>
+    <t>Ti verranno proposte 30 coppie di affermazioni, che descrivono possibili risposte comportamentali in situazioni di conflitto. Di volta in volta, scegli l’alternativa più vera per te tra A o B.
+A volte né A né B potrebbero corrispondere al tuo comportamento, scegli comunque l’alternativa che più si avvicina al tuo modo di fare.</t>
+  </si>
+  <si>
     <t>QUICKNESS</t>
   </si>
   <si>
@@ -1477,6 +1497,12 @@
   </si>
   <si>
     <t>Effetti sonori</t>
+  </si>
+  <si>
+    <t>SUBMIT</t>
+  </si>
+  <si>
+    <t>Submit</t>
   </si>
   <si>
     <t>SUGAR_SIGN_IN</t>
@@ -1561,8 +1587,8 @@
 The ability to evolve the interests and motivations of people, involving them and getting them to also reach challenging goals.
 Attempting to listen and be interested in emotions, values, morals, individual qualities.
 Pay attention to the growth and needs of others, encouraging them to be creative and innovative.
-It is a reference model and leads by example.
-It has the ability to adapt to situations and contexts.</t>
+Be a role model to others and lead by example.
+The ability to adapt to situations and contexts.</t>
   </si>
   <si>
     <t>Le sue principali caratteristiche sono:
@@ -1683,32 +1709,6 @@
   </si>
   <si>
     <t>tu</t>
-  </si>
-  <si>
-    <t>SUBMIT</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>CONFLICT_QUESTIONNAIRE</t>
-  </si>
-  <si>
-    <t>Conflict Questionnaire</t>
-  </si>
-  <si>
-    <t>Questionario Conflitto</t>
-  </si>
-  <si>
-    <t>QUESTIONNAIRE_INTRO</t>
-  </si>
-  <si>
-    <t>Picture yourself in a situation where your wishes differ from that of another person.
-For each of the following 30 statements, choose either A or B (with a circle) as the one which best describes how you would respond. Sometimes neither the A or B statement is typical of your response but try to choose the one that would seem most likely to be your instinctive response in that situation. Only you will see the finished exercise.</t>
-  </si>
-  <si>
-    <t>Ti verranno proposte 30 coppie di affermazioni, che descrivono possibili risposte comportamentali in situazioni di conflitto. Di volta in volta, scegli l’alternativa più vera per te tra A o B.
-A volte né A né B potrebbero corrispondere al tuo comportamento, scegli comunque l’alternativa che più si avvicina al tuo modo di fare.</t>
   </si>
 </sst>
 </file>
@@ -2913,7 +2913,7 @@
       <c r="B39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>111</v>
       </c>
       <c r="D39" s="4"/>
@@ -2969,20 +2969,24 @@
       <c r="W40" s="4"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
@@ -3010,60 +3014,60 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
@@ -3078,13 +3082,13 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -3105,10 +3109,10 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>129</v>
@@ -3118,167 +3122,167 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
+        <v>132</v>
+      </c>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B48" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="B48" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="C48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
-      <c r="V51" s="4"/>
-      <c r="W51" s="4"/>
+      <c r="C51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>47</v>
@@ -3301,19 +3305,15 @@
       <c r="W52" s="4"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="A53" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="C53" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -3332,31 +3332,35 @@
       <c r="W53" s="4"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="2" t="s">
@@ -3373,17 +3377,17 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -3481,17 +3485,17 @@
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-      <c r="S59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
-      <c r="W59" s="3"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="4"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="2" t="s">
@@ -3501,34 +3505,34 @@
         <v>165</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
-      <c r="V60" s="4"/>
-      <c r="W60" s="4"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>167</v>
+        <v>47</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -3549,10 +3553,10 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>170</v>
@@ -3643,59 +3647,55 @@
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="4"/>
+      <c r="V65" s="4"/>
+      <c r="W65" s="4"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
-      <c r="P66" s="4"/>
-      <c r="Q66" s="4"/>
-      <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4"/>
-      <c r="V66" s="4"/>
-      <c r="W66" s="4"/>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -3714,20 +3714,24 @@
       <c r="W67" s="4"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
@@ -3775,7 +3779,7 @@
         <v>192</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3795,20 +3799,20 @@
       <c r="W70" s="4"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="1" t="s">
-        <v>193</v>
+      <c r="A71" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
+        <v>195</v>
+      </c>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
@@ -3823,18 +3827,14 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B72" s="5" t="s">
         <v>196</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -3853,20 +3853,24 @@
       <c r="W72" s="4"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="5" t="s">
         <v>199</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
@@ -3907,20 +3911,20 @@
       <c r="W74" s="4"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
+      <c r="C75" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
@@ -3934,19 +3938,15 @@
       <c r="W75" s="4"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B76" s="5" t="s">
+      <c r="A76" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
+      <c r="C76" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -3965,31 +3965,35 @@
       <c r="W76" s="4"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="5" t="s">
         <v>210</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="3"/>
-      <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
-      <c r="V77" s="3"/>
-      <c r="W77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="2" t="s">
@@ -4006,17 +4010,17 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4"/>
-      <c r="S78" s="4"/>
-      <c r="T78" s="4"/>
-      <c r="U78" s="4"/>
-      <c r="V78" s="4"/>
-      <c r="W78" s="4"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="2" t="s">
@@ -4046,24 +4050,20 @@
       <c r="W79" s="4"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
       <c r="O80" s="4"/>
@@ -4077,31 +4077,35 @@
       <c r="W80" s="4"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="3"/>
-      <c r="P81" s="3"/>
-      <c r="Q81" s="3"/>
-      <c r="R81" s="3"/>
-      <c r="S81" s="3"/>
-      <c r="T81" s="3"/>
-      <c r="U81" s="3"/>
-      <c r="V81" s="3"/>
-      <c r="W81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+      <c r="U81" s="4"/>
+      <c r="V81" s="4"/>
+      <c r="W81" s="4"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="2" t="s">
@@ -4212,41 +4216,41 @@
       <c r="W85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
-      <c r="U86" s="4"/>
-      <c r="V86" s="4"/>
-      <c r="W86" s="4"/>
+      <c r="H86" s="3"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>47</v>
+      <c r="C87" s="8" t="s">
+        <v>241</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -4266,20 +4270,20 @@
       <c r="W87" s="4"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="2" t="s">
-        <v>241</v>
+      <c r="A88" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C88" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
+      <c r="C88" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
       <c r="O88" s="4"/>
@@ -4334,17 +4338,17 @@
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-      <c r="Q90" s="3"/>
-      <c r="R90" s="3"/>
-      <c r="S90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+      <c r="S90" s="4"/>
+      <c r="T90" s="4"/>
+      <c r="U90" s="4"/>
+      <c r="V90" s="4"/>
+      <c r="W90" s="4"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="2" t="s">
@@ -4361,17 +4365,17 @@
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
-      <c r="M91" s="4"/>
-      <c r="N91" s="4"/>
-      <c r="O91" s="4"/>
-      <c r="P91" s="4"/>
-      <c r="Q91" s="4"/>
-      <c r="R91" s="4"/>
-      <c r="S91" s="4"/>
-      <c r="T91" s="4"/>
-      <c r="U91" s="4"/>
-      <c r="V91" s="4"/>
-      <c r="W91" s="4"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="2" t="s">
@@ -4455,20 +4459,20 @@
       <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
-      <c r="K95" s="4"/>
-      <c r="L95" s="4"/>
+      <c r="C95" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
@@ -4482,20 +4486,20 @@
       <c r="W95" s="4"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="2" t="s">
-        <v>264</v>
+      <c r="A96" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C96" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
+      <c r="C96" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
       <c r="O96" s="4"/>
@@ -4550,17 +4554,17 @@
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
-      <c r="R98" s="3"/>
-      <c r="S98" s="3"/>
-      <c r="T98" s="3"/>
-      <c r="U98" s="3"/>
-      <c r="V98" s="3"/>
-      <c r="W98" s="3"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="4"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+      <c r="U98" s="4"/>
+      <c r="V98" s="4"/>
+      <c r="W98" s="4"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="2" t="s">
@@ -4577,17 +4581,17 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="4"/>
-      <c r="T99" s="4"/>
-      <c r="U99" s="4"/>
-      <c r="V99" s="4"/>
-      <c r="W99" s="4"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="3"/>
+      <c r="T99" s="3"/>
+      <c r="U99" s="3"/>
+      <c r="V99" s="3"/>
+      <c r="W99" s="3"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="2" t="s">
@@ -4631,17 +4635,17 @@
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
-      <c r="S101" s="3"/>
-      <c r="T101" s="3"/>
-      <c r="U101" s="3"/>
-      <c r="V101" s="3"/>
-      <c r="W101" s="3"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="4"/>
+      <c r="S101" s="4"/>
+      <c r="T101" s="4"/>
+      <c r="U101" s="4"/>
+      <c r="V101" s="4"/>
+      <c r="W101" s="4"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="2" t="s">
@@ -4658,17 +4662,17 @@
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="4"/>
-      <c r="R102" s="4"/>
-      <c r="S102" s="4"/>
-      <c r="T102" s="4"/>
-      <c r="U102" s="4"/>
-      <c r="V102" s="4"/>
-      <c r="W102" s="4"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="3"/>
+      <c r="T102" s="3"/>
+      <c r="U102" s="3"/>
+      <c r="V102" s="3"/>
+      <c r="W102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
@@ -4698,20 +4702,20 @@
       <c r="W103" s="4"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
-      <c r="K104" s="4"/>
-      <c r="L104" s="4"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="4"/>
@@ -4725,38 +4729,38 @@
       <c r="W104" s="4"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="1" t="s">
         <v>291</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="H105" s="3"/>
-      <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
-      <c r="M105" s="3"/>
-      <c r="N105" s="3"/>
-      <c r="O105" s="3"/>
-      <c r="P105" s="3"/>
-      <c r="Q105" s="3"/>
-      <c r="R105" s="3"/>
-      <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
+      <c r="C105" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H105" s="4"/>
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4"/>
+      <c r="U105" s="4"/>
+      <c r="V105" s="4"/>
+      <c r="W105" s="4"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>295</v>
@@ -4766,48 +4770,48 @@
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
-      <c r="M106" s="4"/>
-      <c r="N106" s="4"/>
-      <c r="O106" s="4"/>
-      <c r="P106" s="4"/>
-      <c r="Q106" s="4"/>
-      <c r="R106" s="4"/>
-      <c r="S106" s="4"/>
-      <c r="T106" s="4"/>
-      <c r="U106" s="4"/>
-      <c r="V106" s="4"/>
-      <c r="W106" s="4"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="3"/>
+      <c r="T106" s="3"/>
+      <c r="U106" s="3"/>
+      <c r="V106" s="3"/>
+      <c r="W106" s="3"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>296</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+      <c r="V107" s="4"/>
+      <c r="W107" s="4"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>299</v>
@@ -4820,17 +4824,17 @@
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
-      <c r="M108" s="4"/>
-      <c r="N108" s="4"/>
-      <c r="O108" s="4"/>
-      <c r="P108" s="4"/>
-      <c r="Q108" s="4"/>
-      <c r="R108" s="4"/>
-      <c r="S108" s="4"/>
-      <c r="T108" s="4"/>
-      <c r="U108" s="4"/>
-      <c r="V108" s="4"/>
-      <c r="W108" s="4"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="2" t="s">
@@ -4839,26 +4843,25 @@
       <c r="B109" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D109" s="1"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
-      <c r="N109" s="3"/>
-      <c r="O109" s="3"/>
-      <c r="P109" s="3"/>
-      <c r="Q109" s="3"/>
-      <c r="R109" s="3"/>
-      <c r="S109" s="3"/>
-      <c r="T109" s="3"/>
-      <c r="U109" s="3"/>
-      <c r="V109" s="3"/>
-      <c r="W109" s="3"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="4"/>
+      <c r="S109" s="4"/>
+      <c r="T109" s="4"/>
+      <c r="U109" s="4"/>
+      <c r="V109" s="4"/>
+      <c r="W109" s="4"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="2" t="s">
@@ -4868,7 +4871,7 @@
         <v>305</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>47</v>
+        <v>306</v>
       </c>
       <c r="D110" s="1"/>
       <c r="H110" s="3"/>
@@ -4889,41 +4892,42 @@
       <c r="W110" s="3"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" s="1" t="s">
-        <v>306</v>
+      <c r="A111" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D111" s="1"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
-      <c r="M111" s="4"/>
-      <c r="N111" s="4"/>
-      <c r="O111" s="4"/>
-      <c r="P111" s="4"/>
-      <c r="Q111" s="4"/>
-      <c r="R111" s="4"/>
-      <c r="S111" s="4"/>
-      <c r="T111" s="4"/>
-      <c r="U111" s="4"/>
-      <c r="V111" s="4"/>
-      <c r="W111" s="4"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3"/>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="3"/>
+      <c r="T111" s="3"/>
+      <c r="U111" s="3"/>
+      <c r="V111" s="3"/>
+      <c r="W111" s="3"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" s="2" t="s">
-        <v>308</v>
+      <c r="A112" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C112" s="2" t="s">
         <v>310</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
@@ -5254,75 +5258,75 @@
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
-      <c r="O124" s="3"/>
-      <c r="P124" s="3"/>
-      <c r="Q124" s="3"/>
-      <c r="R124" s="3"/>
-      <c r="S124" s="3"/>
-      <c r="T124" s="3"/>
-      <c r="U124" s="3"/>
-      <c r="V124" s="3"/>
-      <c r="W124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="4"/>
+      <c r="S124" s="4"/>
+      <c r="T124" s="4"/>
+      <c r="U124" s="4"/>
+      <c r="V124" s="4"/>
+      <c r="W124" s="4"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="2" t="s">
         <v>348</v>
       </c>
       <c r="C125" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+      <c r="J125" s="3"/>
+      <c r="K125" s="3"/>
+      <c r="L125" s="3"/>
+      <c r="M125" s="3"/>
+      <c r="N125" s="3"/>
+      <c r="O125" s="3"/>
+      <c r="P125" s="3"/>
+      <c r="Q125" s="3"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="3"/>
+      <c r="T125" s="3"/>
+      <c r="U125" s="3"/>
+      <c r="V125" s="3"/>
+      <c r="W125" s="3"/>
+    </row>
+    <row r="126" ht="14.25" customHeight="1">
+      <c r="A126" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D125" s="4"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="4"/>
-      <c r="G125" s="4"/>
-      <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
-      <c r="J125" s="4"/>
-      <c r="K125" s="4"/>
-      <c r="L125" s="4"/>
-      <c r="M125" s="4"/>
-      <c r="N125" s="4"/>
-      <c r="O125" s="4"/>
-      <c r="P125" s="4"/>
-      <c r="Q125" s="4"/>
-      <c r="R125" s="4"/>
-      <c r="S125" s="4"/>
-      <c r="T125" s="4"/>
-      <c r="U125" s="4"/>
-      <c r="V125" s="4"/>
-      <c r="W125" s="4"/>
-    </row>
-    <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="H126" s="3"/>
-      <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
-      <c r="L126" s="3"/>
-      <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="3"/>
-      <c r="R126" s="3"/>
-      <c r="S126" s="3"/>
-      <c r="T126" s="3"/>
-      <c r="U126" s="3"/>
-      <c r="V126" s="3"/>
-      <c r="W126" s="3"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="4"/>
+      <c r="S126" s="4"/>
+      <c r="T126" s="4"/>
+      <c r="U126" s="4"/>
+      <c r="V126" s="4"/>
+      <c r="W126" s="4"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
@@ -5339,17 +5343,17 @@
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
-      <c r="M127" s="4"/>
-      <c r="N127" s="4"/>
-      <c r="O127" s="4"/>
-      <c r="P127" s="4"/>
-      <c r="Q127" s="4"/>
-      <c r="R127" s="4"/>
-      <c r="S127" s="4"/>
-      <c r="T127" s="4"/>
-      <c r="U127" s="4"/>
-      <c r="V127" s="4"/>
-      <c r="W127" s="4"/>
+      <c r="M127" s="3"/>
+      <c r="N127" s="3"/>
+      <c r="O127" s="3"/>
+      <c r="P127" s="3"/>
+      <c r="Q127" s="3"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="3"/>
+      <c r="T127" s="3"/>
+      <c r="U127" s="3"/>
+      <c r="V127" s="3"/>
+      <c r="W127" s="3"/>
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="2" t="s">
@@ -5406,24 +5410,20 @@
       <c r="W129" s="4"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="2" t="s">
         <v>362</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="4"/>
-      <c r="I130" s="4"/>
-      <c r="J130" s="4"/>
-      <c r="K130" s="4"/>
-      <c r="L130" s="4"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
       <c r="M130" s="4"/>
       <c r="N130" s="4"/>
       <c r="O130" s="4"/>
@@ -5437,122 +5437,130 @@
       <c r="W130" s="4"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="5" t="s">
         <v>365</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H131" s="3"/>
-      <c r="I131" s="3"/>
-      <c r="J131" s="3"/>
-      <c r="K131" s="3"/>
-      <c r="L131" s="3"/>
-      <c r="M131" s="3"/>
-      <c r="N131" s="3"/>
-      <c r="O131" s="3"/>
-      <c r="P131" s="3"/>
-      <c r="Q131" s="3"/>
-      <c r="R131" s="3"/>
-      <c r="S131" s="3"/>
-      <c r="T131" s="3"/>
-      <c r="U131" s="3"/>
-      <c r="V131" s="3"/>
-      <c r="W131" s="3"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="4"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+      <c r="U131" s="4"/>
+      <c r="V131" s="4"/>
+      <c r="W131" s="4"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H132" s="3"/>
-      <c r="I132" s="3"/>
-      <c r="J132" s="3"/>
-      <c r="K132" s="3"/>
-      <c r="L132" s="3"/>
-      <c r="M132" s="3"/>
-      <c r="N132" s="3"/>
-      <c r="O132" s="3"/>
-      <c r="P132" s="3"/>
-      <c r="Q132" s="3"/>
-      <c r="R132" s="3"/>
-      <c r="S132" s="3"/>
-      <c r="T132" s="3"/>
-      <c r="U132" s="3"/>
-      <c r="V132" s="3"/>
-      <c r="W132" s="3"/>
+      <c r="C132" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="4"/>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="4"/>
+      <c r="Q132" s="4"/>
+      <c r="R132" s="4"/>
+      <c r="S132" s="4"/>
+      <c r="T132" s="4"/>
+      <c r="U132" s="4"/>
+      <c r="V132" s="4"/>
+      <c r="W132" s="4"/>
     </row>
     <row r="133" ht="14.25" customHeight="1">
-      <c r="A133" s="1" t="s">
-        <v>369</v>
+      <c r="A133" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>47</v>
+        <v>371</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
-      <c r="M133" s="4"/>
-      <c r="N133" s="4"/>
-      <c r="O133" s="4"/>
-      <c r="P133" s="4"/>
-      <c r="Q133" s="4"/>
-      <c r="R133" s="4"/>
-      <c r="S133" s="4"/>
-      <c r="T133" s="4"/>
-      <c r="U133" s="4"/>
-      <c r="V133" s="4"/>
-      <c r="W133" s="4"/>
+      <c r="M133" s="3"/>
+      <c r="N133" s="3"/>
+      <c r="O133" s="3"/>
+      <c r="P133" s="3"/>
+      <c r="Q133" s="3"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="3"/>
+      <c r="T133" s="3"/>
+      <c r="U133" s="3"/>
+      <c r="V133" s="3"/>
+      <c r="W133" s="3"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>373</v>
+        <v>47</v>
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
       <c r="L134" s="3"/>
-      <c r="M134" s="4"/>
-      <c r="N134" s="4"/>
-      <c r="O134" s="4"/>
-      <c r="P134" s="4"/>
-      <c r="Q134" s="4"/>
-      <c r="R134" s="4"/>
-      <c r="S134" s="4"/>
-      <c r="T134" s="4"/>
-      <c r="U134" s="4"/>
-      <c r="V134" s="4"/>
-      <c r="W134" s="4"/>
+      <c r="M134" s="3"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="3"/>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="3"/>
+      <c r="R134" s="3"/>
+      <c r="S134" s="3"/>
+      <c r="T134" s="3"/>
+      <c r="U134" s="3"/>
+      <c r="V134" s="3"/>
+      <c r="W134" s="3"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="2" t="s">
-        <v>374</v>
+      <c r="A135" s="1" t="s">
+        <v>375</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C135" s="2" t="s">
         <v>376</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
@@ -5687,7 +5695,7 @@
         <v>390</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>47</v>
+        <v>391</v>
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
@@ -5708,13 +5716,13 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>47</v>
+        <v>394</v>
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
@@ -5735,40 +5743,40 @@
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="2" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>395</v>
+        <v>47</v>
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
       <c r="L142" s="3"/>
-      <c r="M142" s="3"/>
-      <c r="N142" s="3"/>
-      <c r="O142" s="3"/>
-      <c r="P142" s="3"/>
-      <c r="Q142" s="3"/>
-      <c r="R142" s="3"/>
-      <c r="S142" s="3"/>
-      <c r="T142" s="3"/>
-      <c r="U142" s="3"/>
-      <c r="V142" s="3"/>
-      <c r="W142" s="3"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="4"/>
+      <c r="S142" s="4"/>
+      <c r="T142" s="4"/>
+      <c r="U142" s="4"/>
+      <c r="V142" s="4"/>
+      <c r="W142" s="4"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>398</v>
+        <v>47</v>
       </c>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
@@ -5802,17 +5810,17 @@
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="4"/>
-      <c r="O144" s="4"/>
-      <c r="P144" s="4"/>
-      <c r="Q144" s="4"/>
-      <c r="R144" s="4"/>
-      <c r="S144" s="4"/>
-      <c r="T144" s="4"/>
-      <c r="U144" s="4"/>
-      <c r="V144" s="4"/>
-      <c r="W144" s="4"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3"/>
+      <c r="P144" s="3"/>
+      <c r="Q144" s="3"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="3"/>
+      <c r="T144" s="3"/>
+      <c r="U144" s="3"/>
+      <c r="V144" s="3"/>
+      <c r="W144" s="3"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
@@ -5849,7 +5857,7 @@
         <v>406</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
@@ -5870,13 +5878,13 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
@@ -5897,13 +5905,13 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
@@ -5924,30 +5932,30 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
       <c r="L149" s="3"/>
-      <c r="M149" s="3"/>
-      <c r="N149" s="3"/>
-      <c r="O149" s="3"/>
-      <c r="P149" s="3"/>
-      <c r="Q149" s="3"/>
-      <c r="R149" s="3"/>
-      <c r="S149" s="3"/>
-      <c r="T149" s="3"/>
-      <c r="U149" s="3"/>
-      <c r="V149" s="3"/>
-      <c r="W149" s="3"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="4"/>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4"/>
+      <c r="R149" s="4"/>
+      <c r="S149" s="4"/>
+      <c r="T149" s="4"/>
+      <c r="U149" s="4"/>
+      <c r="V149" s="4"/>
+      <c r="W149" s="4"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
@@ -5984,34 +5992,34 @@
         <v>419</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>47</v>
+        <v>420</v>
       </c>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
-      <c r="M151" s="4"/>
-      <c r="N151" s="4"/>
-      <c r="O151" s="4"/>
-      <c r="P151" s="4"/>
-      <c r="Q151" s="4"/>
-      <c r="R151" s="4"/>
-      <c r="S151" s="4"/>
-      <c r="T151" s="4"/>
-      <c r="U151" s="4"/>
-      <c r="V151" s="4"/>
-      <c r="W151" s="4"/>
+      <c r="M151" s="3"/>
+      <c r="N151" s="3"/>
+      <c r="O151" s="3"/>
+      <c r="P151" s="3"/>
+      <c r="Q151" s="3"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="3"/>
+      <c r="T151" s="3"/>
+      <c r="U151" s="3"/>
+      <c r="V151" s="3"/>
+      <c r="W151" s="3"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
@@ -6032,30 +6040,30 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>425</v>
+        <v>47</v>
       </c>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
       <c r="L153" s="3"/>
-      <c r="M153" s="3"/>
-      <c r="N153" s="3"/>
-      <c r="O153" s="3"/>
-      <c r="P153" s="3"/>
-      <c r="Q153" s="3"/>
-      <c r="R153" s="3"/>
-      <c r="S153" s="3"/>
-      <c r="T153" s="3"/>
-      <c r="U153" s="3"/>
-      <c r="V153" s="3"/>
-      <c r="W153" s="3"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="4"/>
+      <c r="P153" s="4"/>
+      <c r="Q153" s="4"/>
+      <c r="R153" s="4"/>
+      <c r="S153" s="4"/>
+      <c r="T153" s="4"/>
+      <c r="U153" s="4"/>
+      <c r="V153" s="4"/>
+      <c r="W153" s="4"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
@@ -6072,17 +6080,17 @@
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
-      <c r="M154" s="3"/>
-      <c r="N154" s="3"/>
-      <c r="O154" s="3"/>
-      <c r="P154" s="3"/>
-      <c r="Q154" s="3"/>
-      <c r="R154" s="3"/>
-      <c r="S154" s="3"/>
-      <c r="T154" s="3"/>
-      <c r="U154" s="3"/>
-      <c r="V154" s="3"/>
-      <c r="W154" s="3"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+      <c r="Q154" s="4"/>
+      <c r="R154" s="4"/>
+      <c r="S154" s="4"/>
+      <c r="T154" s="4"/>
+      <c r="U154" s="4"/>
+      <c r="V154" s="4"/>
+      <c r="W154" s="4"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
@@ -6207,17 +6215,17 @@
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
       <c r="L159" s="3"/>
-      <c r="M159" s="4"/>
-      <c r="N159" s="4"/>
-      <c r="O159" s="4"/>
-      <c r="P159" s="4"/>
-      <c r="Q159" s="4"/>
-      <c r="R159" s="4"/>
-      <c r="S159" s="4"/>
-      <c r="T159" s="4"/>
-      <c r="U159" s="4"/>
-      <c r="V159" s="4"/>
-      <c r="W159" s="4"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
+      <c r="O159" s="3"/>
+      <c r="P159" s="3"/>
+      <c r="Q159" s="3"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="3"/>
+      <c r="T159" s="3"/>
+      <c r="U159" s="3"/>
+      <c r="V159" s="3"/>
+      <c r="W159" s="3"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
@@ -6234,17 +6242,17 @@
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
       <c r="L160" s="3"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="4"/>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
-      <c r="Q160" s="4"/>
-      <c r="R160" s="4"/>
-      <c r="S160" s="4"/>
-      <c r="T160" s="4"/>
-      <c r="U160" s="4"/>
-      <c r="V160" s="4"/>
-      <c r="W160" s="4"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="3"/>
+      <c r="T160" s="3"/>
+      <c r="U160" s="3"/>
+      <c r="V160" s="3"/>
+      <c r="W160" s="3"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
@@ -6261,17 +6269,17 @@
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
       <c r="L161" s="3"/>
-      <c r="M161" s="3"/>
-      <c r="N161" s="3"/>
-      <c r="O161" s="3"/>
-      <c r="P161" s="3"/>
-      <c r="Q161" s="3"/>
-      <c r="R161" s="3"/>
-      <c r="S161" s="3"/>
-      <c r="T161" s="3"/>
-      <c r="U161" s="3"/>
-      <c r="V161" s="3"/>
-      <c r="W161" s="3"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="4"/>
+      <c r="Q161" s="4"/>
+      <c r="R161" s="4"/>
+      <c r="S161" s="4"/>
+      <c r="T161" s="4"/>
+      <c r="U161" s="4"/>
+      <c r="V161" s="4"/>
+      <c r="W161" s="4"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
@@ -6281,7 +6289,7 @@
         <v>451</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
@@ -6302,37 +6310,37 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
-      <c r="M163" s="4"/>
-      <c r="N163" s="4"/>
-      <c r="O163" s="4"/>
-      <c r="P163" s="4"/>
-      <c r="Q163" s="4"/>
-      <c r="R163" s="4"/>
-      <c r="S163" s="4"/>
-      <c r="T163" s="4"/>
-      <c r="U163" s="4"/>
-      <c r="V163" s="4"/>
-      <c r="W163" s="4"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
+      <c r="O163" s="3"/>
+      <c r="P163" s="3"/>
+      <c r="Q163" s="3"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="3"/>
+      <c r="T163" s="3"/>
+      <c r="U163" s="3"/>
+      <c r="V163" s="3"/>
+      <c r="W163" s="3"/>
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>457</v>
@@ -6362,7 +6370,7 @@
         <v>459</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
@@ -6383,57 +6391,61 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
-      <c r="M166" s="3"/>
-      <c r="N166" s="3"/>
-      <c r="O166" s="3"/>
-      <c r="P166" s="3"/>
-      <c r="Q166" s="3"/>
-      <c r="R166" s="3"/>
-      <c r="S166" s="3"/>
-      <c r="T166" s="3"/>
-      <c r="U166" s="3"/>
-      <c r="V166" s="3"/>
-      <c r="W166" s="3"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="4"/>
+      <c r="Q166" s="4"/>
+      <c r="R166" s="4"/>
+      <c r="S166" s="4"/>
+      <c r="T166" s="4"/>
+      <c r="U166" s="4"/>
+      <c r="V166" s="4"/>
+      <c r="W166" s="4"/>
     </row>
     <row r="167" ht="14.25" customHeight="1">
-      <c r="A167" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="B167" s="2" t="s">
+      <c r="A167" s="5" t="s">
         <v>464</v>
       </c>
+      <c r="B167" s="5" t="s">
+        <v>465</v>
+      </c>
       <c r="C167" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="H167" s="3"/>
-      <c r="I167" s="3"/>
-      <c r="J167" s="3"/>
-      <c r="K167" s="3"/>
-      <c r="L167" s="3"/>
-      <c r="M167" s="3"/>
-      <c r="N167" s="3"/>
-      <c r="O167" s="3"/>
-      <c r="P167" s="3"/>
-      <c r="Q167" s="3"/>
-      <c r="R167" s="3"/>
-      <c r="S167" s="3"/>
-      <c r="T167" s="3"/>
-      <c r="U167" s="3"/>
-      <c r="V167" s="3"/>
-      <c r="W167" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="4"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="4"/>
+      <c r="L167" s="4"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="4"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
+      <c r="U167" s="4"/>
+      <c r="V167" s="4"/>
+      <c r="W167" s="4"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="2" t="s">
@@ -6443,34 +6455,34 @@
         <v>467</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H168" s="3"/>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
-      <c r="M168" s="3"/>
-      <c r="N168" s="3"/>
-      <c r="O168" s="3"/>
-      <c r="P168" s="3"/>
-      <c r="Q168" s="3"/>
-      <c r="R168" s="3"/>
-      <c r="S168" s="3"/>
-      <c r="T168" s="3"/>
-      <c r="U168" s="3"/>
-      <c r="V168" s="3"/>
-      <c r="W168" s="3"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="4"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="4"/>
+      <c r="Q168" s="4"/>
+      <c r="R168" s="4"/>
+      <c r="S168" s="4"/>
+      <c r="T168" s="4"/>
+      <c r="U168" s="4"/>
+      <c r="V168" s="4"/>
+      <c r="W168" s="4"/>
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="H169" s="3"/>
       <c r="I169" s="3"/>
@@ -6490,104 +6502,96 @@
       <c r="W169" s="3"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="1" t="s">
+      <c r="A170" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="H170" s="3"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="3"/>
+      <c r="K170" s="3"/>
+      <c r="L170" s="3"/>
+      <c r="M170" s="3"/>
+      <c r="N170" s="3"/>
+      <c r="O170" s="3"/>
+      <c r="P170" s="3"/>
+      <c r="Q170" s="3"/>
+      <c r="R170" s="3"/>
+      <c r="S170" s="3"/>
+      <c r="T170" s="3"/>
+      <c r="U170" s="3"/>
+      <c r="V170" s="3"/>
+      <c r="W170" s="3"/>
+    </row>
+    <row r="171" ht="14.25" customHeight="1">
+      <c r="A171" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="H170" s="4"/>
-      <c r="I170" s="4"/>
-      <c r="J170" s="4"/>
-      <c r="K170" s="4"/>
-      <c r="L170" s="4"/>
-      <c r="M170" s="4"/>
-      <c r="N170" s="4"/>
-      <c r="O170" s="4"/>
-      <c r="P170" s="4"/>
-      <c r="Q170" s="4"/>
-      <c r="R170" s="4"/>
-      <c r="S170" s="4"/>
-      <c r="T170" s="4"/>
-      <c r="U170" s="4"/>
-      <c r="V170" s="4"/>
-      <c r="W170" s="4"/>
-    </row>
-    <row r="171" ht="14.25" customHeight="1">
-      <c r="A171" s="1" t="s">
+      <c r="B171" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="C171" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="3"/>
+      <c r="K171" s="3"/>
+      <c r="L171" s="3"/>
+      <c r="M171" s="3"/>
+      <c r="N171" s="3"/>
+      <c r="O171" s="3"/>
+      <c r="P171" s="3"/>
+      <c r="Q171" s="3"/>
+      <c r="R171" s="3"/>
+      <c r="S171" s="3"/>
+      <c r="T171" s="3"/>
+      <c r="U171" s="3"/>
+      <c r="V171" s="3"/>
+      <c r="W171" s="3"/>
+    </row>
+    <row r="172" ht="14.25" customHeight="1">
+      <c r="A172" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="D171" s="4"/>
-      <c r="E171" s="4"/>
-      <c r="F171" s="4"/>
-      <c r="G171" s="4"/>
-      <c r="H171" s="4"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="4"/>
-      <c r="K171" s="4"/>
-      <c r="L171" s="4"/>
-      <c r="M171" s="4"/>
-      <c r="N171" s="4"/>
-      <c r="O171" s="4"/>
-      <c r="P171" s="4"/>
-      <c r="Q171" s="4"/>
-      <c r="R171" s="4"/>
-      <c r="S171" s="4"/>
-      <c r="T171" s="4"/>
-      <c r="U171" s="4"/>
-      <c r="V171" s="4"/>
-      <c r="W171" s="4"/>
-    </row>
-    <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" s="1" t="s">
+      <c r="B172" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="H172" s="4"/>
-      <c r="I172" s="4"/>
-      <c r="J172" s="4"/>
-      <c r="K172" s="4"/>
-      <c r="L172" s="4"/>
-      <c r="M172" s="4"/>
-      <c r="N172" s="4"/>
-      <c r="O172" s="4"/>
-      <c r="P172" s="4"/>
-      <c r="Q172" s="4"/>
-      <c r="R172" s="4"/>
-      <c r="S172" s="4"/>
-      <c r="T172" s="4"/>
-      <c r="U172" s="4"/>
-      <c r="V172" s="4"/>
-      <c r="W172" s="4"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="3"/>
+      <c r="K172" s="3"/>
+      <c r="L172" s="3"/>
+      <c r="M172" s="3"/>
+      <c r="N172" s="3"/>
+      <c r="O172" s="3"/>
+      <c r="P172" s="3"/>
+      <c r="Q172" s="3"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="3"/>
+      <c r="T172" s="3"/>
+      <c r="U172" s="3"/>
+      <c r="V172" s="3"/>
+      <c r="W172" s="3"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="C173" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D173" s="4"/>
-      <c r="E173" s="4"/>
-      <c r="F173" s="4"/>
-      <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
@@ -6606,20 +6610,24 @@
       <c r="W173" s="4"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B174" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="H174" s="3"/>
-      <c r="I174" s="3"/>
-      <c r="J174" s="3"/>
-      <c r="K174" s="3"/>
-      <c r="L174" s="3"/>
+      <c r="D174" s="4"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
+      <c r="H174" s="4"/>
+      <c r="I174" s="4"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="4"/>
+      <c r="L174" s="4"/>
       <c r="M174" s="4"/>
       <c r="N174" s="4"/>
       <c r="O174" s="4"/>
@@ -6633,20 +6641,20 @@
       <c r="W174" s="4"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="C175" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="H175" s="3"/>
-      <c r="I175" s="3"/>
-      <c r="J175" s="3"/>
-      <c r="K175" s="3"/>
-      <c r="L175" s="3"/>
+      <c r="H175" s="4"/>
+      <c r="I175" s="4"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="4"/>
+      <c r="L175" s="4"/>
       <c r="M175" s="4"/>
       <c r="N175" s="4"/>
       <c r="O175" s="4"/>
@@ -6660,20 +6668,24 @@
       <c r="W175" s="4"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B176" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="H176" s="3"/>
-      <c r="I176" s="3"/>
-      <c r="J176" s="3"/>
-      <c r="K176" s="3"/>
-      <c r="L176" s="3"/>
+      <c r="D176" s="4"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
       <c r="M176" s="4"/>
       <c r="N176" s="4"/>
       <c r="O176" s="4"/>
@@ -6687,24 +6699,20 @@
       <c r="W176" s="4"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="5" t="s">
+      <c r="A177" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B177" s="5" t="s">
+      <c r="C177" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C177" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="D177" s="4"/>
-      <c r="E177" s="4"/>
-      <c r="F177" s="4"/>
-      <c r="G177" s="4"/>
-      <c r="H177" s="4"/>
-      <c r="I177" s="4"/>
-      <c r="J177" s="4"/>
-      <c r="K177" s="4"/>
-      <c r="L177" s="4"/>
+      <c r="H177" s="3"/>
+      <c r="I177" s="3"/>
+      <c r="J177" s="3"/>
+      <c r="K177" s="3"/>
+      <c r="L177" s="3"/>
       <c r="M177" s="4"/>
       <c r="N177" s="4"/>
       <c r="O177" s="4"/>
@@ -6718,24 +6726,20 @@
       <c r="W177" s="4"/>
     </row>
     <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="5" t="s">
+      <c r="A178" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="B178" s="5" t="s">
+      <c r="C178" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D178" s="4"/>
-      <c r="E178" s="4"/>
-      <c r="F178" s="4"/>
-      <c r="G178" s="4"/>
-      <c r="H178" s="4"/>
-      <c r="I178" s="4"/>
-      <c r="J178" s="4"/>
-      <c r="K178" s="4"/>
-      <c r="L178" s="4"/>
+      <c r="H178" s="3"/>
+      <c r="I178" s="3"/>
+      <c r="J178" s="3"/>
+      <c r="K178" s="3"/>
+      <c r="L178" s="3"/>
       <c r="M178" s="4"/>
       <c r="N178" s="4"/>
       <c r="O178" s="4"/>
@@ -6750,73 +6754,81 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="H179" s="3"/>
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
       <c r="K179" s="3"/>
       <c r="L179" s="3"/>
-      <c r="M179" s="3"/>
-      <c r="N179" s="3"/>
-      <c r="O179" s="3"/>
-      <c r="P179" s="3"/>
-      <c r="Q179" s="3"/>
-      <c r="R179" s="3"/>
-      <c r="S179" s="3"/>
-      <c r="T179" s="3"/>
-      <c r="U179" s="3"/>
-      <c r="V179" s="3"/>
-      <c r="W179" s="3"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="4"/>
+      <c r="S179" s="4"/>
+      <c r="T179" s="4"/>
+      <c r="U179" s="4"/>
+      <c r="V179" s="4"/>
+      <c r="W179" s="4"/>
     </row>
     <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="2" t="s">
+      <c r="A180" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B180" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="C180" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H180" s="3"/>
-      <c r="I180" s="3"/>
-      <c r="J180" s="3"/>
-      <c r="K180" s="3"/>
-      <c r="L180" s="3"/>
-      <c r="M180" s="3"/>
-      <c r="N180" s="3"/>
-      <c r="O180" s="3"/>
-      <c r="P180" s="3"/>
-      <c r="Q180" s="3"/>
-      <c r="R180" s="3"/>
-      <c r="S180" s="3"/>
-      <c r="T180" s="3"/>
-      <c r="U180" s="3"/>
-      <c r="V180" s="3"/>
-      <c r="W180" s="3"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="4"/>
+      <c r="L180" s="4"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="4"/>
+      <c r="S180" s="4"/>
+      <c r="T180" s="4"/>
+      <c r="U180" s="4"/>
+      <c r="V180" s="4"/>
+      <c r="W180" s="4"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="1" t="s">
+      <c r="A181" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" s="5" t="s">
         <v>505</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H181" s="3"/>
-      <c r="I181" s="3"/>
-      <c r="J181" s="3"/>
-      <c r="K181" s="3"/>
-      <c r="L181" s="3"/>
+        <v>506</v>
+      </c>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+      <c r="L181" s="4"/>
       <c r="M181" s="4"/>
       <c r="N181" s="4"/>
       <c r="O181" s="4"/>
@@ -6831,13 +6843,13 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
@@ -6858,10 +6870,10 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>47</v>
@@ -6885,10 +6897,10 @@
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>47</v>
@@ -6912,40 +6924,40 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>47</v>
+        <v>516</v>
       </c>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
       <c r="L185" s="3"/>
-      <c r="M185" s="4"/>
-      <c r="N185" s="4"/>
-      <c r="O185" s="4"/>
-      <c r="P185" s="4"/>
-      <c r="Q185" s="4"/>
-      <c r="R185" s="4"/>
-      <c r="S185" s="4"/>
-      <c r="T185" s="4"/>
-      <c r="U185" s="4"/>
-      <c r="V185" s="4"/>
-      <c r="W185" s="4"/>
+      <c r="M185" s="3"/>
+      <c r="N185" s="3"/>
+      <c r="O185" s="3"/>
+      <c r="P185" s="3"/>
+      <c r="Q185" s="3"/>
+      <c r="R185" s="3"/>
+      <c r="S185" s="3"/>
+      <c r="T185" s="3"/>
+      <c r="U185" s="3"/>
+      <c r="V185" s="3"/>
+      <c r="W185" s="3"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>517</v>
+        <v>47</v>
       </c>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
@@ -6965,14 +6977,14 @@
       <c r="W186" s="3"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
-      <c r="A187" s="2" t="s">
-        <v>518</v>
+      <c r="A187" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="C187" s="2" t="s">
         <v>520</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H187" s="3"/>
       <c r="I187" s="3"/>
@@ -6992,24 +7004,20 @@
       <c r="W187" s="4"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="5" t="s">
+      <c r="A188" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B188" s="5" t="s">
+      <c r="B188" s="2" t="s">
         <v>522</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D188" s="4"/>
-      <c r="E188" s="4"/>
-      <c r="F188" s="4"/>
-      <c r="G188" s="4"/>
-      <c r="H188" s="4"/>
-      <c r="I188" s="4"/>
-      <c r="J188" s="4"/>
-      <c r="K188" s="4"/>
-      <c r="L188" s="4"/>
+      <c r="H188" s="3"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="3"/>
+      <c r="K188" s="3"/>
+      <c r="L188" s="3"/>
       <c r="M188" s="4"/>
       <c r="N188" s="4"/>
       <c r="O188" s="4"/>
@@ -7023,55 +7031,47 @@
       <c r="W188" s="4"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" s="5" t="s">
+      <c r="A189" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B189" s="5" t="s">
+      <c r="B189" s="2" t="s">
         <v>524</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="D189" s="4"/>
-      <c r="E189" s="4"/>
-      <c r="F189" s="4"/>
-      <c r="G189" s="4"/>
-      <c r="H189" s="4"/>
-      <c r="I189" s="4"/>
-      <c r="J189" s="4"/>
-      <c r="K189" s="4"/>
-      <c r="L189" s="4"/>
-      <c r="M189" s="4"/>
-      <c r="N189" s="4"/>
-      <c r="O189" s="4"/>
-      <c r="P189" s="4"/>
-      <c r="Q189" s="4"/>
-      <c r="R189" s="4"/>
-      <c r="S189" s="4"/>
-      <c r="T189" s="4"/>
-      <c r="U189" s="4"/>
-      <c r="V189" s="4"/>
-      <c r="W189" s="4"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="3"/>
+      <c r="K189" s="3"/>
+      <c r="L189" s="3"/>
+      <c r="M189" s="3"/>
+      <c r="N189" s="3"/>
+      <c r="O189" s="3"/>
+      <c r="P189" s="3"/>
+      <c r="Q189" s="3"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="3"/>
+      <c r="T189" s="3"/>
+      <c r="U189" s="3"/>
+      <c r="V189" s="3"/>
+      <c r="W189" s="3"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" s="5" t="s">
+      <c r="A190" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B190" s="5" t="s">
+      <c r="B190" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="C190" s="5" t="s">
+      <c r="C190" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D190" s="4"/>
-      <c r="E190" s="4"/>
-      <c r="F190" s="4"/>
-      <c r="G190" s="4"/>
-      <c r="H190" s="4"/>
-      <c r="I190" s="4"/>
-      <c r="J190" s="4"/>
-      <c r="K190" s="4"/>
-      <c r="L190" s="4"/>
+      <c r="H190" s="3"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="3"/>
+      <c r="K190" s="3"/>
+      <c r="L190" s="3"/>
       <c r="M190" s="4"/>
       <c r="N190" s="4"/>
       <c r="O190" s="4"/>

</xml_diff>

<commit_message>
Further UI improvements. Score values now rounded instead of having fraction removed. As a result, score required to place 1st and score required to complete the race in 30 minutes adjusted to account for slightly higher scores.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="564">
   <si>
     <t>Key</t>
   </si>
@@ -1334,7 +1334,8 @@
 Are you sure you want to race with this line-up now?</t>
   </si>
   <si>
-    <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.</t>
+    <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.
+Sei sicuro di voler gareggiare con questa formazione?</t>
   </si>
   <si>
     <t>RACE_CONFIRM_NO_ALLOWANCE</t>
@@ -1367,17 +1368,21 @@
     <t>RACE_SKIP_CONFIRM_ALLOWANCE_REMAINING</t>
   </si>
   <si>
-    <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?
-You also have {0} Talk Time remaining, which will be lost if not used before racing.</t>
+    <t>You have {0} Talk Time remaining! If you don't use it before the race, they will be lost.
+Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
+  </si>
+  <si>
+    <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.
+Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
+  </si>
+  <si>
+    <t>RACE_SKIP_CONFIRM_NO_ALLOWANCE</t>
+  </si>
+  <si>
+    <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
   </si>
   <si>
     <t>Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
-  </si>
-  <si>
-    <t>RACE_SKIP_CONFIRM_NO_ALLOWANCE</t>
-  </si>
-  <si>
-    <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
   </si>
   <si>
     <t>RANDOMISE</t>
@@ -1699,6 +1704,15 @@
     <t>Responsabile per il controllo delle vele. Attenzione ai dettagli e alla durata sono competenze necessarie per questo ruolo.</t>
   </si>
   <si>
+    <t>TUTORIAL_CLOSE</t>
+  </si>
+  <si>
+    <t>To close, click anywhere on the screen.</t>
+  </si>
+  <si>
+    <t>Per chiudere, clicca in qualunque punto dello schermo.</t>
+  </si>
+  <si>
     <t>TUTORIAL_WARNING</t>
   </si>
   <si>
@@ -1742,7 +1756,7 @@
     <t>Willpower - ability to keep calm under pressure</t>
   </si>
   <si>
-    <t>Fermezza - capacità di rimanere calmi quando si è sotto pressione</t>
+    <t>Forza di volontà - capacità di rimanere calmi quando si è sotto pressione</t>
   </si>
   <si>
     <t>WILLPOWER_FEEDBACK</t>
@@ -1824,7 +1838,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1835,12 +1849,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1855,7 +1863,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1892,9 +1900,6 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -5755,7 +5760,7 @@
       <c r="B139" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C139" s="9" t="s">
         <v>408</v>
       </c>
       <c r="H139" s="4"/>
@@ -5863,7 +5868,7 @@
       <c r="B143" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C143" s="12" t="s">
+      <c r="C143" s="9" t="s">
         <v>420</v>
       </c>
       <c r="H143" s="4"/>
@@ -5891,7 +5896,7 @@
         <v>422</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -5912,13 +5917,13 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -5939,13 +5944,13 @@
     </row>
     <row r="146" ht="14.25" customHeight="1">
       <c r="A146" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -5966,13 +5971,13 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -5993,13 +5998,13 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -6020,13 +6025,13 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -6047,13 +6052,13 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -6074,13 +6079,13 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -6101,13 +6106,13 @@
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -6128,13 +6133,13 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -6155,13 +6160,13 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -6182,13 +6187,13 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -6209,13 +6214,13 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -6236,13 +6241,13 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -6263,13 +6268,13 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -6290,13 +6295,13 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
@@ -6317,13 +6322,13 @@
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -6344,13 +6349,13 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -6371,13 +6376,13 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -6398,13 +6403,13 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -6425,13 +6430,13 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
@@ -6452,13 +6457,13 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
@@ -6479,13 +6484,13 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -6506,13 +6511,13 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
@@ -6533,13 +6538,13 @@
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E168" s="3"/>
       <c r="F168" s="3"/>
@@ -6563,13 +6568,13 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6590,13 +6595,13 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
@@ -6617,13 +6622,13 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -6644,13 +6649,13 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
@@ -6671,13 +6676,13 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
@@ -6698,13 +6703,13 @@
     </row>
     <row r="174" ht="14.25" customHeight="1">
       <c r="A174" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H174" s="3"/>
       <c r="I174" s="3"/>
@@ -6725,13 +6730,13 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B175" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E175" s="3"/>
       <c r="F175" s="3"/>
@@ -6755,13 +6760,13 @@
     </row>
     <row r="176" ht="14.25" customHeight="1">
       <c r="A176" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
@@ -6782,13 +6787,13 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
@@ -6812,13 +6817,13 @@
     </row>
     <row r="178" ht="14.25" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
@@ -6839,13 +6844,13 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
@@ -6866,19 +6871,23 @@
     </row>
     <row r="180" ht="14.25" customHeight="1">
       <c r="A180" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="C180" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="H180" s="4"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="4"/>
-      <c r="K180" s="4"/>
-      <c r="L180" s="4"/>
+      <c r="C180" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="3"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="3"/>
       <c r="M180" s="3"/>
       <c r="N180" s="3"/>
       <c r="O180" s="3"/>
@@ -6892,23 +6901,20 @@
       <c r="W180" s="3"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="B181" s="6" t="s">
+      <c r="A181" s="2" t="s">
         <v>528</v>
       </c>
+      <c r="B181" s="2" t="s">
+        <v>529</v>
+      </c>
       <c r="C181" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
-      <c r="G181" s="3"/>
-      <c r="H181" s="3"/>
-      <c r="I181" s="3"/>
-      <c r="J181" s="3"/>
-      <c r="K181" s="3"/>
-      <c r="L181" s="3"/>
+        <v>530</v>
+      </c>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+      <c r="L181" s="4"/>
       <c r="M181" s="3"/>
       <c r="N181" s="3"/>
       <c r="O181" s="3"/>
@@ -6923,13 +6929,13 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
@@ -6952,41 +6958,44 @@
       <c r="W182" s="3"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="A183" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="B183" s="2" t="s">
+      <c r="A183" s="6" t="s">
         <v>534</v>
       </c>
+      <c r="B183" s="6" t="s">
+        <v>535</v>
+      </c>
       <c r="C183" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="H183" s="4"/>
-      <c r="I183" s="4"/>
-      <c r="J183" s="4"/>
-      <c r="K183" s="4"/>
-      <c r="L183" s="4"/>
-      <c r="M183" s="4"/>
-      <c r="N183" s="4"/>
-      <c r="O183" s="4"/>
-      <c r="P183" s="4"/>
-      <c r="Q183" s="4"/>
-      <c r="R183" s="4"/>
-      <c r="S183" s="4"/>
-      <c r="T183" s="4"/>
-      <c r="U183" s="4"/>
-      <c r="V183" s="4"/>
-      <c r="W183" s="4"/>
+        <v>536</v>
+      </c>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="3"/>
+      <c r="K183" s="3"/>
+      <c r="L183" s="3"/>
+      <c r="M183" s="3"/>
+      <c r="N183" s="3"/>
+      <c r="O183" s="3"/>
+      <c r="P183" s="3"/>
+      <c r="Q183" s="3"/>
+      <c r="R183" s="3"/>
+      <c r="S183" s="3"/>
+      <c r="T183" s="3"/>
+      <c r="U183" s="3"/>
+      <c r="V183" s="3"/>
+      <c r="W183" s="3"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
@@ -7006,68 +7015,68 @@
       <c r="W184" s="4"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="A185" s="1" t="s">
-        <v>539</v>
+      <c r="A185" s="2" t="s">
+        <v>540</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="C185" s="5" t="s">
         <v>541</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>542</v>
       </c>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
       <c r="J185" s="4"/>
       <c r="K185" s="4"/>
       <c r="L185" s="4"/>
-      <c r="M185" s="3"/>
-      <c r="N185" s="3"/>
-      <c r="O185" s="3"/>
-      <c r="P185" s="3"/>
-      <c r="Q185" s="3"/>
-      <c r="R185" s="3"/>
-      <c r="S185" s="3"/>
-      <c r="T185" s="3"/>
-      <c r="U185" s="3"/>
-      <c r="V185" s="3"/>
-      <c r="W185" s="3"/>
+      <c r="M185" s="4"/>
+      <c r="N185" s="4"/>
+      <c r="O185" s="4"/>
+      <c r="P185" s="4"/>
+      <c r="Q185" s="4"/>
+      <c r="R185" s="4"/>
+      <c r="S185" s="4"/>
+      <c r="T185" s="4"/>
+      <c r="U185" s="4"/>
+      <c r="V185" s="4"/>
+      <c r="W185" s="4"/>
     </row>
     <row r="186" ht="14.25" customHeight="1">
-      <c r="A186" s="2" t="s">
-        <v>542</v>
+      <c r="A186" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
       <c r="J186" s="4"/>
       <c r="K186" s="4"/>
       <c r="L186" s="4"/>
-      <c r="M186" s="4"/>
-      <c r="N186" s="4"/>
-      <c r="O186" s="4"/>
-      <c r="P186" s="4"/>
-      <c r="Q186" s="4"/>
-      <c r="R186" s="4"/>
-      <c r="S186" s="4"/>
-      <c r="T186" s="4"/>
-      <c r="U186" s="4"/>
-      <c r="V186" s="4"/>
-      <c r="W186" s="4"/>
+      <c r="M186" s="3"/>
+      <c r="N186" s="3"/>
+      <c r="O186" s="3"/>
+      <c r="P186" s="3"/>
+      <c r="Q186" s="3"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="3"/>
+      <c r="T186" s="3"/>
+      <c r="U186" s="3"/>
+      <c r="V186" s="3"/>
+      <c r="W186" s="3"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
@@ -7087,41 +7096,41 @@
       <c r="W187" s="4"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="1" t="s">
-        <v>548</v>
+      <c r="A188" s="2" t="s">
+        <v>549</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
       <c r="J188" s="4"/>
       <c r="K188" s="4"/>
       <c r="L188" s="4"/>
-      <c r="M188" s="3"/>
-      <c r="N188" s="3"/>
-      <c r="O188" s="3"/>
-      <c r="P188" s="3"/>
-      <c r="Q188" s="3"/>
-      <c r="R188" s="3"/>
-      <c r="S188" s="3"/>
-      <c r="T188" s="3"/>
-      <c r="U188" s="3"/>
-      <c r="V188" s="3"/>
-      <c r="W188" s="3"/>
+      <c r="M188" s="4"/>
+      <c r="N188" s="4"/>
+      <c r="O188" s="4"/>
+      <c r="P188" s="4"/>
+      <c r="Q188" s="4"/>
+      <c r="R188" s="4"/>
+      <c r="S188" s="4"/>
+      <c r="T188" s="4"/>
+      <c r="U188" s="4"/>
+      <c r="V188" s="4"/>
+      <c r="W188" s="4"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" s="2" t="s">
-        <v>551</v>
+      <c r="A189" s="1" t="s">
+        <v>552</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
@@ -7142,71 +7151,73 @@
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
       <c r="J190" s="4"/>
       <c r="K190" s="4"/>
       <c r="L190" s="4"/>
-      <c r="M190" s="4"/>
-      <c r="N190" s="4"/>
-      <c r="O190" s="4"/>
-      <c r="P190" s="4"/>
-      <c r="Q190" s="4"/>
-      <c r="R190" s="4"/>
-      <c r="S190" s="4"/>
-      <c r="T190" s="4"/>
-      <c r="U190" s="4"/>
-      <c r="V190" s="4"/>
-      <c r="W190" s="4"/>
+      <c r="M190" s="3"/>
+      <c r="N190" s="3"/>
+      <c r="O190" s="3"/>
+      <c r="P190" s="3"/>
+      <c r="Q190" s="3"/>
+      <c r="R190" s="3"/>
+      <c r="S190" s="3"/>
+      <c r="T190" s="3"/>
+      <c r="U190" s="3"/>
+      <c r="V190" s="3"/>
+      <c r="W190" s="3"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
       <c r="J191" s="4"/>
       <c r="K191" s="4"/>
       <c r="L191" s="4"/>
-      <c r="M191" s="3"/>
-      <c r="N191" s="3"/>
-      <c r="O191" s="3"/>
-      <c r="P191" s="3"/>
-      <c r="Q191" s="3"/>
-      <c r="R191" s="3"/>
-      <c r="S191" s="3"/>
-      <c r="T191" s="3"/>
-      <c r="U191" s="3"/>
-      <c r="V191" s="3"/>
-      <c r="W191" s="3"/>
+      <c r="M191" s="4"/>
+      <c r="N191" s="4"/>
+      <c r="O191" s="4"/>
+      <c r="P191" s="4"/>
+      <c r="Q191" s="4"/>
+      <c r="R191" s="4"/>
+      <c r="S191" s="4"/>
+      <c r="T191" s="4"/>
+      <c r="U191" s="4"/>
+      <c r="V191" s="4"/>
+      <c r="W191" s="4"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" s="4"/>
-      <c r="B192" s="4"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
-      <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
-      <c r="I192" s="3"/>
-      <c r="J192" s="3"/>
-      <c r="K192" s="3"/>
-      <c r="L192" s="3"/>
+      <c r="A192" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C192" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="H192" s="4"/>
+      <c r="I192" s="4"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+      <c r="L192" s="4"/>
       <c r="M192" s="3"/>
       <c r="N192" s="3"/>
       <c r="O192" s="3"/>

</xml_diff>

<commit_message>
Updated assets with fixes. Updated UI and tutorial text. Minor UI changes.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="571">
   <si>
     <t>Key</t>
   </si>
@@ -266,7 +266,7 @@
     <t>Chosen Management Styles</t>
   </si>
   <si>
-    <t>Stili di gestione selezionati</t>
+    <t>Stili di gestione del conflitto</t>
   </si>
   <si>
     <t>COLLABORATING</t>
@@ -406,29 +406,25 @@
     <t>CONFLICT_MANAGEMENT_HEADER</t>
   </si>
   <si>
-    <t>Conflict Management Styles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stili di gestione del conflitto </t>
+    <t>Assertiveness and Cooperation</t>
+  </si>
+  <si>
+    <t>Assertività e cooperatività</t>
   </si>
   <si>
     <t>CONFLICT_MANAGEMENT_TEXT</t>
   </si>
   <si>
-    <t>The following is a representation of the different styles of conflict management according to the Thomas-Kilmann model.
-The model proposed by Thomas-Kilmann on conflict management is built around two main dimensions:
-1. Assertiveness or affirmation: the extent to which the individual tries to meet their needs.
-2. Cooperativity: the extent to which the individual strives to meet the needs of others.
-These dimensions are used to define five styles of conflict management represented below. If you are curious to find out more you can read a description of each by clicking on the images.
-We suggest starting with the style that best represents you with the highest percentage.</t>
-  </si>
-  <si>
-    <t>Di seguito ti viene mostrata una rappresentazione dei diversi stili di gestione del conflitto secondo il modello di Thomas-Kilmann.
-Il modello proposto da Thomas-Kilmann sulla gestione del conflitto si costruisce attorno a due dimensioni principali:
-1. Assertività o affermazione: la misura in cui l’individuo cerca di soddisfare le proprie esigenze.
-2. Cooperatività: la misura in cui l’individuo si adopera per soddisfare le esigenze altrui.
-Tali dimensioni sono utilizzate per definire 5 stili di gestione del conflitto qui di seguito rappresentate. Se sei curioso di scoprire qualcosa in più puoi leggere le descrizioni cliccando sulle immagini.
-Ti suggeriamo di partire dallo stile che più ti rappresenta con la percentuale più alta e dal suo opposto, con la percentuale più bassa.</t>
+    <t>The model proposed by Thomas-Kilmann on conflict management is built around two main dimensions:
+Assertiveness or affirmation: the extent to which the individual tries to satisfy his/her needs,
+Cooperative: the extent to which the individual strives to meet the needs of others.
+These dimensions are used to define the 5 styles of conflict management. If you are curious to find out more, you can read descriptions on each by clicking on the images. We suggest starting with the style that most represents you the most (with the highest percentage) and the least (with the lowest percentage).</t>
+  </si>
+  <si>
+    <t>Il modello proposto da Thomas-Kilmann sulla gestione del conflitto si costruisce attorno a due dimensioni principali:
+Assertività o affermazione: la misura in cui l’individuo cerca di soddisfare le proprie esigenze,
+Cooperatività: la misura in cui l’individuo si adopera per soddisfare le esigenze altrui.
+Tali dimensioni sono utilizzate per definire i 5 stili di gestione del conflitto. Se sei curioso di scoprire qualcosa in più puoi leggere le descrizioni cliccando sulle immagini. Parti dallo stile che più ti rappresenta (con la percentuale più alta) e dal suo opposto (con la percentuale più bassa).</t>
   </si>
   <si>
     <t>CONFLICT_QUESTIONNAIRE</t>
@@ -553,19 +549,19 @@
     <t>FINAL_RESULT_HEADER</t>
   </si>
   <si>
-    <t>Final Result</t>
-  </si>
-  <si>
-    <t>Risultati finali</t>
+    <t>Prevailing Leadership Style</t>
+  </si>
+  <si>
+    <t>Stile di leadership prevalente</t>
   </si>
   <si>
     <t>FINAL_RESULT_TEXT</t>
   </si>
   <si>
-    <t>In this game we found that your prevailing style is:</t>
-  </si>
-  <si>
-    <t>Nel gioco è emerso che il tuo stile prevalente è:</t>
+    <t>Your prevailing leadership style is</t>
+  </si>
+  <si>
+    <t>Il tuo stile di leadership prevalente è</t>
   </si>
   <si>
     <t>FIRE</t>
@@ -625,12 +621,12 @@
     <t>GRAPH_INTRO</t>
   </si>
   <si>
-    <t>For management styles that were selected frequently or rarely, some questions of reflection are provided that may be useful for further thinking.
-The next page also provides more information on each management style.</t>
-  </si>
-  <si>
-    <t>Per gli stili in cui ti sei collocato nella fascia al di sotto di molto basso e al di sopra di molto alto ti compariranno alcune domande di riflessione che potranno esserti utili agli approfondimenti successivi. 
-Se non ti compare nessuna domanda vai allo step successivo per scoprire di più sulla tua modalità di gestione del conflitto.</t>
+    <t>Below, you will find the various conflict management styles according to Thomas-Kilmann's model. The percentages indicate how much you've adopted each of these styles during the game.
+In order to be able to interpret your profile, we point you to the style with the highest percentage (which represents you the most) and the lowest percentage (which represents you less). Next to these two styles, you will see some reflection questions that may be helpful.</t>
+  </si>
+  <si>
+    <t>Di seguito ti vengono presentati i diversi stili di gestione del conflitto secondo il modello di Thomas-Kilmann. Le percentuali indicano quanto hai adottato ognuno di questi stili durante il gioco. 
+Per poter interpretare il tuo profilo ti indichiamo di soffermarti sullo stile con la percentuale più alta (che ti rappresenta di più) e su quello con la percentuale più bassa (che ti rappresenta di meno). In corrispondenza di questi due stili ti compariranno alcune domande di riflessione che potranno esserti utili in termini di approfondimento.</t>
   </si>
   <si>
     <t>GREEN_PLACEMENT</t>
@@ -777,16 +773,18 @@
     <t>LEADERSHIP_STYLES_TEXT</t>
   </si>
   <si>
-    <t>The conflict management styles can be matched with three leadership styles. The two main dimensions are:
-1. Watching out for yourself, focusing on your own needs and interests;
-2. Watching out for others, focusing on the needs and interests of others.
-The combination of these results in three leadership styles is represented below. If you are curious to find out more you can read a description of each by clicking on the images.</t>
-  </si>
-  <si>
-    <t>Agli stili di gestione del conflitto sono stati abbinati tre stili di gestione della leadership. Le due dimensioni principali sono:
-1. Attenzione per sé: focalizzazione sui propri bisogni e interessi;
-2. Attenzione per l’altro: focalizzazione sui bisogni e interessi altrui.
-La combinazione di queste si traduce in 3 stili di leadership qui di seguito rappresentate. Se sei curioso di scoprire qualcosa in più puoi leggere le descrizioni cliccando sulle immagini.</t>
+    <t>In the game, whilst managing conflicts you were in the leader role.
+Thomas-Kilmann's conflict management model styles have been combined with three leadership styles. The two main dimensions are:
+Being careful about yourself: focusing on your own needs and interests;
+Attention to others: focusing on the needs and interests of others.
+The combination of these results in 3 leadership styles is shown below with your percentages. If you are curious to find out more about your style, you can read descriptions of each by clicking on their images.</t>
+  </si>
+  <si>
+    <t>Nel gioco oltre che gestire i conflitti hai agito il ruolo di leader. 
+Agli stili di gestione del conflitto del modello di Thomas-Kilmann sono stati abbinati tre stili di gestione della leadership.  Le due dimensioni principali sono:
+Attenzione per sé: focalizzazione sui propri bisogni e interessi;
+Attenzione per l’altro: focalizzazione sui bisogni e interessi altrui.
+La combinazione di queste si traduce in 3 stili di leadership qui di seguito rappresentati con le tue percentuali. Se sei curioso di scoprire qualcosa in più sul tuo stile puoi leggere le descrizioni cliccando sulle immagini.</t>
   </si>
   <si>
     <t>LOAD_GAME</t>
@@ -966,7 +964,7 @@
     <t>Stows sails below deck and helps with sail changes. Crew positioned here will need to be physically fit, agile and able to deal with being in this hot, dark and wet position.</t>
   </si>
   <si>
-    <t>Ripiega le vele sottocoperta e aiuta nel cambio della vela. Chi e occupa questa posizione deve essere fisicamente prestante, agile, in grado di sopportare il caldo, il buio e l'umidità.</t>
+    <t>Ripiega le vele sottocoperta e aiuta nel cambio della vela. Chi occupa questa posizione deve essere fisicamente prestante, agile, in grado di sopportare il caldo, il buio e l'umidità.</t>
   </si>
   <si>
     <t>MOOD_FEEDBACK</t>
@@ -1114,7 +1112,7 @@
     <t>This line-up was lacking in perception</t>
   </si>
   <si>
-    <t>Questa formazione è stata carente in percezione</t>
+    <t>Questa formazione era carente in percezione</t>
   </si>
   <si>
     <t>PITMAN</t>
@@ -1141,7 +1139,7 @@
     <t>1st</t>
   </si>
   <si>
-    <t>Primo</t>
+    <t>primo</t>
   </si>
   <si>
     <t>POSITION_10</t>
@@ -1150,7 +1148,7 @@
     <t>10th</t>
   </si>
   <si>
-    <t>Decimo</t>
+    <t>decimo</t>
   </si>
   <si>
     <t>POSITION_2</t>
@@ -1159,7 +1157,7 @@
     <t>2nd</t>
   </si>
   <si>
-    <t>Secondo</t>
+    <t>secondo</t>
   </si>
   <si>
     <t>POSITION_3</t>
@@ -1168,7 +1166,7 @@
     <t>3rd</t>
   </si>
   <si>
-    <t>Terzo</t>
+    <t>terzo</t>
   </si>
   <si>
     <t>POSITION_4</t>
@@ -1177,7 +1175,7 @@
     <t>4th</t>
   </si>
   <si>
-    <t>Quarto</t>
+    <t>quarto</t>
   </si>
   <si>
     <t>POSITION_5</t>
@@ -1186,7 +1184,7 @@
     <t>5th</t>
   </si>
   <si>
-    <t>Quinto</t>
+    <t>quinto</t>
   </si>
   <si>
     <t>POSITION_6</t>
@@ -1195,7 +1193,7 @@
     <t>6th</t>
   </si>
   <si>
-    <t>Sesto</t>
+    <t>sesto</t>
   </si>
   <si>
     <t>POSITION_7</t>
@@ -1204,7 +1202,7 @@
     <t>7th</t>
   </si>
   <si>
-    <t>Settimo</t>
+    <t>settimo</t>
   </si>
   <si>
     <t>POSITION_8</t>
@@ -1213,7 +1211,7 @@
     <t>8th</t>
   </si>
   <si>
-    <t>Ottavo</t>
+    <t>ottavo</t>
   </si>
   <si>
     <t>POSITION_9</t>
@@ -1222,7 +1220,7 @@
     <t>9th</t>
   </si>
   <si>
-    <t>Nono</t>
+    <t>nono</t>
   </si>
   <si>
     <t>POSITION_NAME</t>
@@ -1249,7 +1247,7 @@
     <t>Previous Members</t>
   </si>
   <si>
-    <t>Membri precedenti</t>
+    <t>Chi ha già ricoperto questo ruolo</t>
   </si>
   <si>
     <t>PROMOTION_ADDED</t>
@@ -1323,7 +1321,7 @@
     <t>This line-up was lacking in quickness</t>
   </si>
   <si>
-    <t xml:space="preserve">Questa formazione è stata carente in velocità </t>
+    <t xml:space="preserve">Questa formazione era carente in velocità </t>
   </si>
   <si>
     <t>RACE_BUTTON_PRACTICE</t>
@@ -1352,7 +1350,7 @@
   </si>
   <si>
     <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.
-Sei sicuro di voler gareggiare con questa formazione?</t>
+Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
   </si>
   <si>
     <t>RACE_CONFIRM_NO_ALLOWANCE</t>
@@ -1361,7 +1359,7 @@
     <t>Are you sure you want to race with this line-up now?</t>
   </si>
   <si>
-    <t>Sei sicuro di voler gareggiare con questa formazione?</t>
+    <t>Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
   </si>
   <si>
     <t>RACE_POSITION</t>
@@ -1389,19 +1387,12 @@
 Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
   </si>
   <si>
-    <t>Hai {0} tempo di conversazione rimanente! Se non lo usi prima della gara andrà perduto.
-Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
-  </si>
-  <si>
     <t>RACE_SKIP_CONFIRM_NO_ALLOWANCE</t>
   </si>
   <si>
     <t>Are you sure you want to skip the remaining practice sessions and race with this line-up now?</t>
   </si>
   <si>
-    <t>Sei sicuro di voler saltare le sessioni di prova rimanenti e gareggiare con questa formazione?</t>
-  </si>
-  <si>
     <t>RANDOMISE</t>
   </si>
   <si>
@@ -1519,7 +1510,7 @@
     <t>The race is over and the results are in...</t>
   </si>
   <si>
-    <t>La gara è finita e i risultati sono stati salvati</t>
+    <t>La gara è finita</t>
   </si>
   <si>
     <t>ROLE</t>
@@ -1837,6 +1828,15 @@
   </si>
   <si>
     <t>Tu</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Medio</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1884,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1909,6 +1909,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1919,6 +1920,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2417,7 +2425,7 @@
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
         <v>50</v>
       </c>
       <c r="H17" s="4"/>
@@ -2546,7 +2554,7 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2579,7 +2587,7 @@
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="8" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="4"/>
@@ -2606,7 +2614,7 @@
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="10" t="s">
         <v>71</v>
       </c>
       <c r="H24" s="3"/>
@@ -2984,7 +2992,7 @@
       <c r="B37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="10" t="s">
         <v>110</v>
       </c>
       <c r="H37" s="3"/>
@@ -3011,7 +3019,7 @@
       <c r="B38" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E38" s="3"/>
@@ -3434,7 +3442,7 @@
       <c r="B53" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="10" t="s">
         <v>155</v>
       </c>
       <c r="H53" s="3"/>
@@ -3461,7 +3469,7 @@
       <c r="B54" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="10" t="s">
         <v>158</v>
       </c>
       <c r="E54" s="3"/>
@@ -4122,7 +4130,7 @@
       <c r="B78" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="10" t="s">
         <v>227</v>
       </c>
       <c r="E78" s="3"/>
@@ -4395,7 +4403,7 @@
       <c r="A88" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="11" t="s">
         <v>256</v>
       </c>
       <c r="C88" s="5" t="s">
@@ -4506,7 +4514,7 @@
       <c r="B92" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="10" t="s">
         <v>269</v>
       </c>
       <c r="H92" s="4"/>
@@ -4560,7 +4568,7 @@
       <c r="B94" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="10" t="s">
         <v>275</v>
       </c>
       <c r="H94" s="4"/>
@@ -4587,7 +4595,7 @@
       <c r="B95" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="12" t="s">
         <v>278</v>
       </c>
       <c r="H95" s="4"/>
@@ -4668,7 +4676,7 @@
       <c r="B98" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="13" t="s">
         <v>287</v>
       </c>
       <c r="H98" s="4"/>
@@ -4695,7 +4703,7 @@
       <c r="B99" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="10" t="s">
         <v>290</v>
       </c>
       <c r="H99" s="3"/>
@@ -5073,7 +5081,7 @@
       <c r="B113" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C113" s="10" t="s">
+      <c r="C113" s="11" t="s">
         <v>330</v>
       </c>
       <c r="H113" s="4"/>
@@ -5100,7 +5108,7 @@
       <c r="B114" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C114" s="10" t="s">
+      <c r="C114" s="11" t="s">
         <v>333</v>
       </c>
       <c r="H114" s="4"/>
@@ -5127,7 +5135,7 @@
       <c r="B115" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="C115" s="14" t="s">
         <v>336</v>
       </c>
       <c r="H115" s="4"/>
@@ -5535,7 +5543,7 @@
       <c r="B130" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C130" s="15" t="s">
         <v>381</v>
       </c>
       <c r="H130" s="4"/>
@@ -5673,7 +5681,7 @@
       <c r="B135" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C135" s="12" t="s">
+      <c r="C135" s="16" t="s">
         <v>396</v>
       </c>
       <c r="E135" s="3"/>
@@ -5757,7 +5765,7 @@
       <c r="B138" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C138" s="14" t="s">
         <v>405</v>
       </c>
       <c r="H138" s="4"/>
@@ -5838,7 +5846,7 @@
       <c r="B141" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C141" s="9" t="s">
+      <c r="C141" s="10" t="s">
         <v>414</v>
       </c>
       <c r="H141" s="4"/>
@@ -5865,7 +5873,7 @@
       <c r="B142" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C142" s="10" t="s">
         <v>417</v>
       </c>
       <c r="H142" s="4"/>
@@ -5946,8 +5954,8 @@
       <c r="B145" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="C145" s="9" t="s">
-        <v>426</v>
+      <c r="C145" s="10" t="s">
+        <v>414</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -5968,13 +5976,13 @@
     </row>
     <row r="146" ht="14.25" customHeight="1">
       <c r="A146" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>428</v>
-      </c>
       <c r="C146" s="5" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -5995,13 +6003,13 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C147" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>432</v>
       </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -6022,13 +6030,13 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C148" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>435</v>
       </c>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -6049,13 +6057,13 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C149" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>438</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -6076,13 +6084,13 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C150" s="5" t="s">
         <v>439</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>441</v>
       </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -6103,13 +6111,13 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -6130,13 +6138,13 @@
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -6157,13 +6165,13 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C153" s="5" t="s">
         <v>446</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>448</v>
       </c>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -6184,13 +6192,13 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C154" s="5" t="s">
         <v>449</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>451</v>
       </c>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -6211,13 +6219,13 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C155" s="5" t="s">
         <v>452</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>454</v>
       </c>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -6238,13 +6246,13 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="C156" s="5" t="s">
         <v>455</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>457</v>
       </c>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -6265,13 +6273,13 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C157" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="C157" s="5" t="s">
-        <v>460</v>
       </c>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -6292,13 +6300,13 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C158" s="5" t="s">
         <v>461</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>463</v>
       </c>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -6319,13 +6327,13 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C159" s="5" t="s">
         <v>464</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>466</v>
       </c>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
@@ -6346,13 +6354,13 @@
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C160" s="10" t="s">
         <v>467</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>469</v>
       </c>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -6373,13 +6381,13 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C161" s="5" t="s">
         <v>470</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>472</v>
       </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -6400,13 +6408,13 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>473</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>475</v>
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -6427,13 +6435,13 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>476</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>478</v>
       </c>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -6454,13 +6462,13 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C164" s="5" t="s">
         <v>479</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>481</v>
       </c>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
@@ -6481,13 +6489,13 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C165" s="5" t="s">
         <v>482</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>484</v>
       </c>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
@@ -6508,13 +6516,13 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C166" s="5" t="s">
         <v>485</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -6535,13 +6543,13 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
@@ -6562,13 +6570,13 @@
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C168" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C168" s="5" t="s">
-        <v>492</v>
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
@@ -6589,13 +6597,13 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>493</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>495</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6616,13 +6624,13 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="C170" s="5" t="s">
         <v>496</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>498</v>
       </c>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
@@ -6646,13 +6654,13 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -6673,13 +6681,13 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="C172" s="5" t="s">
         <v>501</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>503</v>
       </c>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
@@ -6700,13 +6708,13 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C173" s="5" t="s">
         <v>504</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="C173" s="5" t="s">
-        <v>506</v>
       </c>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
@@ -6727,13 +6735,13 @@
     </row>
     <row r="174" ht="14.25" customHeight="1">
       <c r="A174" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C174" s="5" t="s">
         <v>507</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>509</v>
       </c>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
@@ -6754,13 +6762,13 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C175" s="5" t="s">
         <v>510</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>512</v>
       </c>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
@@ -6781,13 +6789,13 @@
     </row>
     <row r="176" ht="14.25" customHeight="1">
       <c r="A176" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C176" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="C176" s="5" t="s">
-        <v>515</v>
       </c>
       <c r="H176" s="3"/>
       <c r="I176" s="3"/>
@@ -6808,13 +6816,13 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="C177" s="5" t="s">
         <v>516</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="C177" s="5" t="s">
-        <v>518</v>
       </c>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
@@ -6838,13 +6846,13 @@
     </row>
     <row r="178" ht="14.25" customHeight="1">
       <c r="A178" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C178" s="10" t="s">
         <v>519</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="C178" s="9" t="s">
-        <v>521</v>
       </c>
       <c r="H178" s="3"/>
       <c r="I178" s="3"/>
@@ -6865,13 +6873,13 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C179" s="5" t="s">
         <v>522</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="C179" s="5" t="s">
-        <v>524</v>
       </c>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -6895,13 +6903,13 @@
     </row>
     <row r="180" ht="14.25" customHeight="1">
       <c r="A180" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C180" s="5" t="s">
         <v>525</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="C180" s="5" t="s">
-        <v>527</v>
       </c>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
@@ -6922,13 +6930,13 @@
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C181" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="C181" s="5" t="s">
-        <v>530</v>
       </c>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
@@ -6949,13 +6957,13 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C182" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>533</v>
       </c>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
@@ -6980,13 +6988,13 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C183" s="5" t="s">
         <v>534</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="C183" s="5" t="s">
-        <v>536</v>
       </c>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
@@ -7007,13 +7015,13 @@
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C184" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>539</v>
       </c>
       <c r="E184" s="3"/>
       <c r="F184" s="3"/>
@@ -7037,13 +7045,13 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="6" t="s">
+        <v>538</v>
+      </c>
+      <c r="B185" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C185" s="5" t="s">
         <v>540</v>
-      </c>
-      <c r="B185" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>542</v>
       </c>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
@@ -7067,13 +7075,13 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C186" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="C186" s="5" t="s">
-        <v>545</v>
       </c>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
@@ -7094,13 +7102,13 @@
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C187" s="10" t="s">
         <v>546</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="C187" s="9" t="s">
-        <v>548</v>
       </c>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
@@ -7121,13 +7129,13 @@
     </row>
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C188" s="5" t="s">
         <v>549</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C188" s="5" t="s">
-        <v>551</v>
       </c>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
@@ -7148,13 +7156,13 @@
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C189" s="5" t="s">
         <v>552</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C189" s="5" t="s">
-        <v>554</v>
       </c>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
@@ -7175,13 +7183,13 @@
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C190" s="5" t="s">
         <v>555</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="C190" s="5" t="s">
-        <v>557</v>
       </c>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
@@ -7202,13 +7210,13 @@
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C191" s="5" t="s">
         <v>558</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C191" s="5" t="s">
-        <v>560</v>
       </c>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
@@ -7229,13 +7237,13 @@
     </row>
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C192" s="5" t="s">
         <v>561</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>563</v>
       </c>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
@@ -7256,13 +7264,13 @@
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C193" s="5" t="s">
         <v>564</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="C193" s="5" t="s">
-        <v>566</v>
       </c>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
@@ -7283,13 +7291,13 @@
     </row>
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C194" s="5" t="s">
         <v>567</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="C194" s="5" t="s">
-        <v>569</v>
       </c>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
@@ -7309,9 +7317,15 @@
       <c r="W194" s="3"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="A195" s="4"/>
-      <c r="B195" s="4"/>
-      <c r="C195" s="3"/>
+      <c r="A195" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>570</v>
+      </c>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
       <c r="F195" s="3"/>
@@ -27458,56 +27472,6 @@
       <c r="V1000" s="3"/>
       <c r="W1000" s="3"/>
     </row>
-    <row r="1001" ht="14.25" customHeight="1">
-      <c r="A1001" s="4"/>
-      <c r="B1001" s="4"/>
-      <c r="C1001" s="3"/>
-      <c r="D1001" s="3"/>
-      <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="3"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="3"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="3"/>
-      <c r="O1001" s="3"/>
-      <c r="P1001" s="3"/>
-      <c r="Q1001" s="3"/>
-      <c r="R1001" s="3"/>
-      <c r="S1001" s="3"/>
-      <c r="T1001" s="3"/>
-      <c r="U1001" s="3"/>
-      <c r="V1001" s="3"/>
-      <c r="W1001" s="3"/>
-    </row>
-    <row r="1002" ht="14.25" customHeight="1">
-      <c r="A1002" s="4"/>
-      <c r="B1002" s="4"/>
-      <c r="C1002" s="3"/>
-      <c r="D1002" s="3"/>
-      <c r="E1002" s="3"/>
-      <c r="F1002" s="3"/>
-      <c r="G1002" s="3"/>
-      <c r="H1002" s="3"/>
-      <c r="I1002" s="3"/>
-      <c r="J1002" s="3"/>
-      <c r="K1002" s="3"/>
-      <c r="L1002" s="3"/>
-      <c r="M1002" s="3"/>
-      <c r="N1002" s="3"/>
-      <c r="O1002" s="3"/>
-      <c r="P1002" s="3"/>
-      <c r="Q1002" s="3"/>
-      <c r="R1002" s="3"/>
-      <c r="S1002" s="3"/>
-      <c r="T1002" s="3"/>
-      <c r="U1002" s="3"/>
-      <c r="V1002" s="3"/>
-      <c r="W1002" s="3"/>
-    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Cup result pop-up that leads into questionnaire. Minor localization fix.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -16,7 +16,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C113">
+    <comment authorId="0" ref="C116">
       <text>
         <t xml:space="preserve">?????Avere una visione d'insieme, attenzione, percezione sensoriale
 	-Ellis Spice</t>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="578">
   <si>
     <t>Key</t>
   </si>
@@ -483,6 +483,16 @@
     <t>Avresti potuto scegliere una formazione più efficace in cui le persone vanno più d'accordo tra di loro</t>
   </si>
   <si>
+    <t>CUP_RESULT_OUTRO</t>
+  </si>
+  <si>
+    <t>That was the final race and you've now completed the cup.
+Click the button below to fill out a questionnaire and receive your final feedback.</t>
+  </si>
+  <si>
+    <t>XXXX</t>
+  </si>
+  <si>
     <t>ENGLISH</t>
   </si>
   <si>
@@ -886,6 +896,15 @@
     <t xml:space="preserve">Avresti potuto scegliere una formazione più efficace in cui le persone vanno più d'accordo con te </t>
   </si>
   <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
     <t>MEETING_EARLY_EXIT</t>
   </si>
   <si>
@@ -922,6 +941,15 @@
     <t>Volevi vedermi?</t>
   </si>
   <si>
+    <t>MEETING_INTRO_NEGATIVE</t>
+  </si>
+  <si>
+    <t>What do you want?</t>
+  </si>
+  <si>
+    <t>Cosa vuoi?</t>
+  </si>
+  <si>
     <t>MEETING_INTRO_POSITIVE</t>
   </si>
   <si>
@@ -929,15 +957,6 @@
   </si>
   <si>
     <t>Che cosa vuoi chiedere?</t>
-  </si>
-  <si>
-    <t>MEETING_INTRO_NEGATIVE</t>
-  </si>
-  <si>
-    <t>What do you want?</t>
-  </si>
-  <si>
-    <t>Cosa vuoi?</t>
   </si>
   <si>
     <t>MENU_QUIT_CONFIRM</t>
@@ -1079,6 +1098,12 @@
     <t>Ok</t>
   </si>
   <si>
+    <t>OVERALL_RESULT</t>
+  </si>
+  <si>
+    <t>Final Cup Position</t>
+  </si>
+  <si>
     <t>OVERWRITE</t>
   </si>
   <si>
@@ -1139,7 +1164,7 @@
     <t>1st</t>
   </si>
   <si>
-    <t>primo</t>
+    <t>Primo</t>
   </si>
   <si>
     <t>POSITION_10</t>
@@ -1148,7 +1173,7 @@
     <t>10th</t>
   </si>
   <si>
-    <t>decimo</t>
+    <t>Decimo</t>
   </si>
   <si>
     <t>POSITION_2</t>
@@ -1157,7 +1182,7 @@
     <t>2nd</t>
   </si>
   <si>
-    <t>secondo</t>
+    <t>Secondo</t>
   </si>
   <si>
     <t>POSITION_3</t>
@@ -1166,7 +1191,7 @@
     <t>3rd</t>
   </si>
   <si>
-    <t>terzo</t>
+    <t>Terzo</t>
   </si>
   <si>
     <t>POSITION_4</t>
@@ -1175,7 +1200,7 @@
     <t>4th</t>
   </si>
   <si>
-    <t>quarto</t>
+    <t>Quarto</t>
   </si>
   <si>
     <t>POSITION_5</t>
@@ -1184,7 +1209,7 @@
     <t>5th</t>
   </si>
   <si>
-    <t>quinto</t>
+    <t>Quinto</t>
   </si>
   <si>
     <t>POSITION_6</t>
@@ -1193,7 +1218,7 @@
     <t>6th</t>
   </si>
   <si>
-    <t>sesto</t>
+    <t>Sesto</t>
   </si>
   <si>
     <t>POSITION_7</t>
@@ -1202,7 +1227,7 @@
     <t>7th</t>
   </si>
   <si>
-    <t>settimo</t>
+    <t>Settimo</t>
   </si>
   <si>
     <t>POSITION_8</t>
@@ -1211,7 +1236,7 @@
     <t>8th</t>
   </si>
   <si>
-    <t>ottavo</t>
+    <t>Ottavo</t>
   </si>
   <si>
     <t>POSITION_9</t>
@@ -1220,7 +1245,7 @@
     <t>9th</t>
   </si>
   <si>
-    <t>nono</t>
+    <t>Nono</t>
   </si>
   <si>
     <t>POSITION_NAME</t>
@@ -1371,13 +1396,19 @@
     <t>Posizione:</t>
   </si>
   <si>
-    <t>RACE_RESULT_POSTION</t>
+    <t>RACE_RESULT_POSITION</t>
   </si>
   <si>
     <t>{0} finished {1}!</t>
   </si>
   <si>
     <t>{0} si classifica {1}!</t>
+  </si>
+  <si>
+    <t>RACE_RESULTS</t>
+  </si>
+  <si>
+    <t>Race Results</t>
   </si>
   <si>
     <t>RACE_SKIP_CONFIRM_ALLOWANCE_REMAINING</t>
@@ -1828,15 +1859,6 @@
   </si>
   <si>
     <t>Tu</t>
-  </si>
-  <si>
-    <t>MED</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Medio</t>
   </si>
 </sst>
 </file>
@@ -1925,10 +1947,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3214,20 +3236,24 @@
       <c r="W44" s="3"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
+      <c r="C45" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
@@ -3242,13 +3268,13 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
@@ -3269,10 +3295,10 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>138</v>
@@ -3282,134 +3308,134 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
+        <v>144</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="2" t="s">
         <v>145</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="6" t="s">
         <v>148</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
-      <c r="V51" s="4"/>
-      <c r="W51" s="4"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>150</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3418,22 +3444,22 @@
       <c r="C52" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1" t="s">
@@ -3442,7 +3468,7 @@
       <c r="B53" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="5" t="s">
         <v>155</v>
       </c>
       <c r="H53" s="3"/>
@@ -3463,18 +3489,15 @@
       <c r="W53" s="3"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -3493,31 +3516,34 @@
       <c r="W54" s="3"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="4"/>
-      <c r="P55" s="4"/>
-      <c r="Q55" s="4"/>
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="2" t="s">
@@ -3534,17 +3560,17 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-      <c r="V56" s="3"/>
-      <c r="W56" s="3"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="2" t="s">
@@ -3642,64 +3668,64 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
-      <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
-      <c r="U60" s="4"/>
-      <c r="V60" s="4"/>
-      <c r="W60" s="4"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
@@ -3720,7 +3746,7 @@
         <v>184</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -3741,10 +3767,10 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>187</v>
@@ -3835,20 +3861,20 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
-      <c r="U67" s="4"/>
-      <c r="V67" s="4"/>
-      <c r="W67" s="4"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -3857,36 +3883,33 @@
       <c r="C68" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-      <c r="Q68" s="3"/>
-      <c r="R68" s="3"/>
-      <c r="S68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="4"/>
+      <c r="U68" s="4"/>
+      <c r="V68" s="4"/>
+      <c r="W68" s="4"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
@@ -3905,20 +3928,23 @@
       <c r="W69" s="3"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="6" t="s">
         <v>204</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
@@ -3966,7 +3992,7 @@
         <v>210</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
@@ -3986,20 +4012,20 @@
       <c r="W72" s="3"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="1" t="s">
-        <v>211</v>
+      <c r="A73" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
@@ -4014,17 +4040,14 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B74" s="6" t="s">
         <v>214</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -4043,20 +4066,23 @@
       <c r="W74" s="3"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="6" t="s">
         <v>217</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
@@ -4097,7 +4123,7 @@
       <c r="W76" s="3"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -4106,11 +4132,11 @@
       <c r="C77" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
@@ -4124,18 +4150,15 @@
       <c r="W77" s="3"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
@@ -4154,31 +4177,34 @@
       <c r="W78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="4"/>
-      <c r="R79" s="4"/>
-      <c r="S79" s="4"/>
-      <c r="T79" s="4"/>
-      <c r="U79" s="4"/>
-      <c r="V79" s="4"/>
-      <c r="W79" s="4"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="2" t="s">
@@ -4195,17 +4221,17 @@
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
-      <c r="P80" s="3"/>
-      <c r="Q80" s="3"/>
-      <c r="R80" s="3"/>
-      <c r="S80" s="3"/>
-      <c r="T80" s="3"/>
-      <c r="U80" s="3"/>
-      <c r="V80" s="3"/>
-      <c r="W80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4"/>
+      <c r="V80" s="4"/>
+      <c r="W80" s="4"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="2" t="s">
@@ -4235,23 +4261,20 @@
       <c r="W81" s="3"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
@@ -4265,31 +4288,34 @@
       <c r="W82" s="3"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="6" t="s">
         <v>241</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-      <c r="R83" s="4"/>
-      <c r="S83" s="4"/>
-      <c r="T83" s="4"/>
-      <c r="U83" s="4"/>
-      <c r="V83" s="4"/>
-      <c r="W83" s="4"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="2" t="s">
@@ -4400,37 +4426,37 @@
       <c r="W87" s="4"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="2" t="s">
         <v>256</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="3"/>
-      <c r="P88" s="3"/>
-      <c r="Q88" s="3"/>
-      <c r="R88" s="3"/>
-      <c r="S88" s="3"/>
-      <c r="T88" s="3"/>
-      <c r="U88" s="3"/>
-      <c r="V88" s="3"/>
-      <c r="W88" s="3"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4"/>
+      <c r="U88" s="4"/>
+      <c r="V88" s="4"/>
+      <c r="W88" s="4"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="11" t="s">
         <v>259</v>
       </c>
       <c r="C89" s="5" t="s">
@@ -4454,7 +4480,7 @@
       <c r="W89" s="3"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>261</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -4463,11 +4489,11 @@
       <c r="C90" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
@@ -4481,20 +4507,24 @@
       <c r="W90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
@@ -4511,10 +4541,10 @@
       <c r="A92" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" s="5" t="s">
         <v>269</v>
       </c>
       <c r="H92" s="4"/>
@@ -4522,17 +4552,17 @@
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
-      <c r="Q92" s="4"/>
-      <c r="R92" s="4"/>
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
-      <c r="U92" s="4"/>
-      <c r="V92" s="4"/>
-      <c r="W92" s="4"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="2" t="s">
@@ -4565,7 +4595,7 @@
       <c r="A94" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>274</v>
       </c>
       <c r="C94" s="10" t="s">
@@ -4576,17 +4606,17 @@
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-      <c r="Q94" s="3"/>
-      <c r="R94" s="3"/>
-      <c r="S94" s="3"/>
-      <c r="T94" s="3"/>
-      <c r="U94" s="3"/>
-      <c r="V94" s="3"/>
-      <c r="W94" s="3"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+      <c r="U94" s="4"/>
+      <c r="V94" s="4"/>
+      <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="2" t="s">
@@ -4595,7 +4625,7 @@
       <c r="B95" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="C95" s="5" t="s">
         <v>278</v>
       </c>
       <c r="H95" s="4"/>
@@ -4622,7 +4652,7 @@
       <c r="B96" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="12" t="s">
         <v>281</v>
       </c>
       <c r="H96" s="4"/>
@@ -4649,7 +4679,7 @@
       <c r="B97" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="10" t="s">
         <v>284</v>
       </c>
       <c r="H97" s="4"/>
@@ -4697,20 +4727,20 @@
       <c r="W98" s="3"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C99" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="4"/>
+      <c r="L99" s="4"/>
       <c r="M99" s="3"/>
       <c r="N99" s="3"/>
       <c r="O99" s="3"/>
@@ -4730,7 +4760,7 @@
       <c r="B100" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="14" t="s">
         <v>293</v>
       </c>
       <c r="H100" s="4"/>
@@ -4751,20 +4781,20 @@
       <c r="W100" s="3"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>294</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
-      <c r="K101" s="4"/>
-      <c r="L101" s="4"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
       <c r="M101" s="3"/>
       <c r="N101" s="3"/>
       <c r="O101" s="3"/>
@@ -4792,17 +4822,17 @@
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="4"/>
-      <c r="R102" s="4"/>
-      <c r="S102" s="4"/>
-      <c r="T102" s="4"/>
-      <c r="U102" s="4"/>
-      <c r="V102" s="4"/>
-      <c r="W102" s="4"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="3"/>
+      <c r="T102" s="3"/>
+      <c r="U102" s="3"/>
+      <c r="V102" s="3"/>
+      <c r="W102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="2" t="s">
@@ -4846,17 +4876,17 @@
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-      <c r="M104" s="3"/>
-      <c r="N104" s="3"/>
-      <c r="O104" s="3"/>
-      <c r="P104" s="3"/>
-      <c r="Q104" s="3"/>
-      <c r="R104" s="3"/>
-      <c r="S104" s="3"/>
-      <c r="T104" s="3"/>
-      <c r="U104" s="3"/>
-      <c r="V104" s="3"/>
-      <c r="W104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+      <c r="U104" s="4"/>
+      <c r="V104" s="4"/>
+      <c r="W104" s="4"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="2" t="s">
@@ -4873,17 +4903,17 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="4"/>
-      <c r="N105" s="4"/>
-      <c r="O105" s="4"/>
-      <c r="P105" s="4"/>
-      <c r="Q105" s="4"/>
-      <c r="R105" s="4"/>
-      <c r="S105" s="4"/>
-      <c r="T105" s="4"/>
-      <c r="U105" s="4"/>
-      <c r="V105" s="4"/>
-      <c r="W105" s="4"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="3"/>
+      <c r="T105" s="3"/>
+      <c r="U105" s="3"/>
+      <c r="V105" s="3"/>
+      <c r="W105" s="3"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="2" t="s">
@@ -4927,20 +4957,20 @@
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
-      <c r="O107" s="3"/>
-      <c r="P107" s="3"/>
-      <c r="Q107" s="3"/>
-      <c r="R107" s="3"/>
-      <c r="S107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
+      <c r="S107" s="4"/>
+      <c r="T107" s="4"/>
+      <c r="U107" s="4"/>
+      <c r="V107" s="4"/>
+      <c r="W107" s="4"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="2" t="s">
         <v>315</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -4949,11 +4979,11 @@
       <c r="C108" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="4"/>
+      <c r="L108" s="4"/>
       <c r="M108" s="3"/>
       <c r="N108" s="3"/>
       <c r="O108" s="3"/>
@@ -4974,40 +5004,40 @@
         <v>319</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
-      <c r="M109" s="4"/>
-      <c r="N109" s="4"/>
-      <c r="O109" s="4"/>
-      <c r="P109" s="4"/>
-      <c r="Q109" s="4"/>
-      <c r="R109" s="4"/>
-      <c r="S109" s="4"/>
-      <c r="T109" s="4"/>
-      <c r="U109" s="4"/>
-      <c r="V109" s="4"/>
-      <c r="W109" s="4"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3"/>
+      <c r="T109" s="3"/>
+      <c r="U109" s="3"/>
+      <c r="V109" s="3"/>
+      <c r="W109" s="3"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" s="2" t="s">
-        <v>320</v>
+      <c r="A110" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-      <c r="J110" s="4"/>
-      <c r="K110" s="4"/>
-      <c r="L110" s="4"/>
+        <v>323</v>
+      </c>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
       <c r="M110" s="3"/>
       <c r="N110" s="3"/>
       <c r="O110" s="3"/>
@@ -5022,13 +5052,13 @@
     </row>
     <row r="111" ht="14.25" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -5049,13 +5079,13 @@
     </row>
     <row r="112" ht="14.25" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -5076,12 +5106,12 @@
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="5" t="s">
         <v>330</v>
       </c>
       <c r="H113" s="4"/>
@@ -5102,41 +5132,45 @@
       <c r="W113" s="4"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="3"/>
+      <c r="T114" s="3"/>
+      <c r="U114" s="3"/>
+      <c r="V114" s="3"/>
+      <c r="W114" s="3"/>
+    </row>
+    <row r="115" ht="14.25" customHeight="1">
+      <c r="A115" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
-      <c r="J114" s="4"/>
-      <c r="K114" s="4"/>
-      <c r="L114" s="4"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="4"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
-      <c r="Q114" s="4"/>
-      <c r="R114" s="4"/>
-      <c r="S114" s="4"/>
-      <c r="T114" s="4"/>
-      <c r="U114" s="4"/>
-      <c r="V114" s="4"/>
-      <c r="W114" s="4"/>
-    </row>
-    <row r="115" ht="14.25" customHeight="1">
-      <c r="A115" s="1" t="s">
+      <c r="B115" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="5" t="s">
         <v>335</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>336</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -5157,67 +5191,67 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="11" t="s">
         <v>338</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>339</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
       <c r="L116" s="4"/>
-      <c r="M116" s="3"/>
-      <c r="N116" s="3"/>
-      <c r="O116" s="3"/>
-      <c r="P116" s="3"/>
-      <c r="Q116" s="3"/>
-      <c r="R116" s="3"/>
-      <c r="S116" s="3"/>
-      <c r="T116" s="3"/>
-      <c r="U116" s="3"/>
-      <c r="V116" s="3"/>
-      <c r="W116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="4"/>
+      <c r="S116" s="4"/>
+      <c r="T116" s="4"/>
+      <c r="U116" s="4"/>
+      <c r="V116" s="4"/>
+      <c r="W116" s="4"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="11" t="s">
         <v>341</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>342</v>
       </c>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
-      <c r="M117" s="3"/>
-      <c r="N117" s="3"/>
-      <c r="O117" s="3"/>
-      <c r="P117" s="3"/>
-      <c r="Q117" s="3"/>
-      <c r="R117" s="3"/>
-      <c r="S117" s="3"/>
-      <c r="T117" s="3"/>
-      <c r="U117" s="3"/>
-      <c r="V117" s="3"/>
-      <c r="W117" s="3"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="4"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+      <c r="U117" s="4"/>
+      <c r="V117" s="4"/>
+      <c r="W117" s="4"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="15" t="s">
         <v>344</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>345</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -5238,13 +5272,13 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="5" t="s">
         <v>347</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>348</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -5265,13 +5299,13 @@
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="C120" s="5" t="s">
-        <v>351</v>
       </c>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
@@ -5292,13 +5326,13 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="10" t="s">
         <v>353</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>354</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -5319,13 +5353,13 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="10" t="s">
         <v>356</v>
-      </c>
-      <c r="C122" s="5" t="s">
-        <v>357</v>
       </c>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
@@ -5346,13 +5380,13 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>360</v>
       </c>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -5373,13 +5407,13 @@
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>363</v>
       </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -5400,13 +5434,13 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="10" t="s">
         <v>365</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>366</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -5427,13 +5461,13 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="10" t="s">
         <v>368</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>369</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -5454,13 +5488,13 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="10" t="s">
         <v>371</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>372</v>
       </c>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -5481,49 +5515,46 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="C128" s="5" t="s">
-        <v>375</v>
       </c>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
-      <c r="M128" s="4"/>
-      <c r="N128" s="4"/>
-      <c r="O128" s="4"/>
-      <c r="P128" s="4"/>
-      <c r="Q128" s="4"/>
-      <c r="R128" s="4"/>
-      <c r="S128" s="4"/>
-      <c r="T128" s="4"/>
-      <c r="U128" s="4"/>
-      <c r="V128" s="4"/>
-      <c r="W128" s="4"/>
+      <c r="M128" s="3"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="3"/>
+      <c r="P128" s="3"/>
+      <c r="Q128" s="3"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="3"/>
+      <c r="T128" s="3"/>
+      <c r="U128" s="3"/>
+      <c r="V128" s="3"/>
+      <c r="W128" s="3"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B129" s="6" t="s">
+      <c r="C129" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="C129" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
-      <c r="H129" s="3"/>
-      <c r="I129" s="3"/>
-      <c r="J129" s="3"/>
-      <c r="K129" s="3"/>
-      <c r="L129" s="3"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="4"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
       <c r="M129" s="3"/>
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
@@ -5538,73 +5569,76 @@
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="C130" s="10" t="s">
         <v>380</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>381</v>
       </c>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
       <c r="L130" s="4"/>
-      <c r="M130" s="4"/>
-      <c r="N130" s="4"/>
-      <c r="O130" s="4"/>
-      <c r="P130" s="4"/>
-      <c r="Q130" s="4"/>
-      <c r="R130" s="4"/>
-      <c r="S130" s="4"/>
-      <c r="T130" s="4"/>
-      <c r="U130" s="4"/>
-      <c r="V130" s="4"/>
-      <c r="W130" s="4"/>
+      <c r="M130" s="3"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="3"/>
+      <c r="P130" s="3"/>
+      <c r="Q130" s="3"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="3"/>
+      <c r="T130" s="3"/>
+      <c r="U130" s="3"/>
+      <c r="V130" s="3"/>
+      <c r="W130" s="3"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="C131" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>384</v>
       </c>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
       <c r="L131" s="4"/>
-      <c r="M131" s="3"/>
-      <c r="N131" s="3"/>
-      <c r="O131" s="3"/>
-      <c r="P131" s="3"/>
-      <c r="Q131" s="3"/>
-      <c r="R131" s="3"/>
-      <c r="S131" s="3"/>
-      <c r="T131" s="3"/>
-      <c r="U131" s="3"/>
-      <c r="V131" s="3"/>
-      <c r="W131" s="3"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="4"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+      <c r="U131" s="4"/>
+      <c r="V131" s="4"/>
+      <c r="W131" s="4"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B132" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="C132" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="4"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
       <c r="M132" s="3"/>
       <c r="N132" s="3"/>
       <c r="O132" s="3"/>
@@ -5619,49 +5653,46 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>390</v>
       </c>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
       <c r="L133" s="4"/>
-      <c r="M133" s="3"/>
-      <c r="N133" s="3"/>
-      <c r="O133" s="3"/>
-      <c r="P133" s="3"/>
-      <c r="Q133" s="3"/>
-      <c r="R133" s="3"/>
-      <c r="S133" s="3"/>
-      <c r="T133" s="3"/>
-      <c r="U133" s="3"/>
-      <c r="V133" s="3"/>
-      <c r="W133" s="3"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="4"/>
+      <c r="S133" s="4"/>
+      <c r="T133" s="4"/>
+      <c r="U133" s="4"/>
+      <c r="V133" s="4"/>
+      <c r="W133" s="4"/>
     </row>
     <row r="134" ht="14.25" customHeight="1">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B134" s="6" t="s">
+      <c r="C134" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="E134" s="3"/>
-      <c r="F134" s="3"/>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="3"/>
-      <c r="K134" s="3"/>
-      <c r="L134" s="3"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="4"/>
       <c r="M134" s="3"/>
       <c r="N134" s="3"/>
       <c r="O134" s="3"/>
@@ -5675,23 +5706,20 @@
       <c r="W134" s="3"/>
     </row>
     <row r="135" ht="14.25" customHeight="1">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="C135" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="C135" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="E135" s="3"/>
-      <c r="F135" s="3"/>
-      <c r="G135" s="3"/>
-      <c r="H135" s="3"/>
-      <c r="I135" s="3"/>
-      <c r="J135" s="3"/>
-      <c r="K135" s="3"/>
-      <c r="L135" s="3"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
       <c r="M135" s="3"/>
       <c r="N135" s="3"/>
       <c r="O135" s="3"/>
@@ -5706,73 +5734,79 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="C136" s="5" t="s">
-        <v>399</v>
       </c>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
       <c r="K136" s="4"/>
       <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
-      <c r="N136" s="4"/>
-      <c r="O136" s="4"/>
-      <c r="P136" s="4"/>
-      <c r="Q136" s="4"/>
-      <c r="R136" s="4"/>
-      <c r="S136" s="4"/>
-      <c r="T136" s="4"/>
-      <c r="U136" s="4"/>
-      <c r="V136" s="4"/>
-      <c r="W136" s="4"/>
+      <c r="M136" s="3"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="3"/>
+      <c r="P136" s="3"/>
+      <c r="Q136" s="3"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="3"/>
+      <c r="T136" s="3"/>
+      <c r="U136" s="3"/>
+      <c r="V136" s="3"/>
+      <c r="W136" s="3"/>
     </row>
     <row r="137" ht="14.25" customHeight="1">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="B137" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3"/>
+      <c r="N137" s="3"/>
+      <c r="O137" s="3"/>
+      <c r="P137" s="3"/>
+      <c r="Q137" s="3"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="3"/>
+      <c r="T137" s="3"/>
+      <c r="U137" s="3"/>
+      <c r="V137" s="3"/>
+      <c r="W137" s="3"/>
+    </row>
+    <row r="138" ht="14.25" customHeight="1">
+      <c r="A138" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="H137" s="4"/>
-      <c r="I137" s="4"/>
-      <c r="J137" s="4"/>
-      <c r="K137" s="4"/>
-      <c r="L137" s="4"/>
-      <c r="M137" s="4"/>
-      <c r="N137" s="4"/>
-      <c r="O137" s="4"/>
-      <c r="P137" s="4"/>
-      <c r="Q137" s="4"/>
-      <c r="R137" s="4"/>
-      <c r="S137" s="4"/>
-      <c r="T137" s="4"/>
-      <c r="U137" s="4"/>
-      <c r="V137" s="4"/>
-      <c r="W137" s="4"/>
-    </row>
-    <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" s="1" t="s">
+      <c r="B138" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="C138" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="C138" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="H138" s="4"/>
-      <c r="I138" s="4"/>
-      <c r="J138" s="4"/>
-      <c r="K138" s="4"/>
-      <c r="L138" s="4"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
       <c r="M138" s="3"/>
       <c r="N138" s="3"/>
       <c r="O138" s="3"/>
@@ -5787,67 +5821,67 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>408</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
       <c r="K139" s="4"/>
       <c r="L139" s="4"/>
-      <c r="M139" s="3"/>
-      <c r="N139" s="3"/>
-      <c r="O139" s="3"/>
-      <c r="P139" s="3"/>
-      <c r="Q139" s="3"/>
-      <c r="R139" s="3"/>
-      <c r="S139" s="3"/>
-      <c r="T139" s="3"/>
-      <c r="U139" s="3"/>
-      <c r="V139" s="3"/>
-      <c r="W139" s="3"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="4"/>
+      <c r="S139" s="4"/>
+      <c r="T139" s="4"/>
+      <c r="U139" s="4"/>
+      <c r="V139" s="4"/>
+      <c r="W139" s="4"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="C140" s="5" t="s">
         <v>410</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>411</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4"/>
-      <c r="M140" s="3"/>
-      <c r="N140" s="3"/>
-      <c r="O140" s="3"/>
-      <c r="P140" s="3"/>
-      <c r="Q140" s="3"/>
-      <c r="R140" s="3"/>
-      <c r="S140" s="3"/>
-      <c r="T140" s="3"/>
-      <c r="U140" s="3"/>
-      <c r="V140" s="3"/>
-      <c r="W140" s="3"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="4"/>
+      <c r="S140" s="4"/>
+      <c r="T140" s="4"/>
+      <c r="U140" s="4"/>
+      <c r="V140" s="4"/>
+      <c r="W140" s="4"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="15" t="s">
         <v>413</v>
-      </c>
-      <c r="C141" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -5868,13 +5902,13 @@
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="C142" s="10" t="s">
-        <v>417</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -5895,13 +5929,13 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="5" t="s">
         <v>419</v>
-      </c>
-      <c r="C143" s="5" t="s">
-        <v>420</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -5922,13 +5956,13 @@
     </row>
     <row r="144" ht="14.25" customHeight="1">
       <c r="A144" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="10" t="s">
         <v>422</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>423</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -5949,13 +5983,13 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="10" t="s">
         <v>425</v>
-      </c>
-      <c r="C145" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -5982,7 +6016,7 @@
         <v>427</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -6003,46 +6037,50 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
       <c r="K147" s="4"/>
       <c r="L147" s="4"/>
-      <c r="M147" s="4"/>
-      <c r="N147" s="4"/>
-      <c r="O147" s="4"/>
-      <c r="P147" s="4"/>
-      <c r="Q147" s="4"/>
-      <c r="R147" s="4"/>
-      <c r="S147" s="4"/>
-      <c r="T147" s="4"/>
-      <c r="U147" s="4"/>
-      <c r="V147" s="4"/>
-      <c r="W147" s="4"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
+      <c r="O147" s="3"/>
+      <c r="P147" s="3"/>
+      <c r="Q147" s="3"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="3"/>
+      <c r="T147" s="3"/>
+      <c r="U147" s="3"/>
+      <c r="V147" s="3"/>
+      <c r="W147" s="3"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B148" s="2" t="s">
+      <c r="A148" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="B148" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
-      <c r="J148" s="4"/>
-      <c r="K148" s="4"/>
-      <c r="L148" s="4"/>
+      <c r="C148" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
       <c r="M148" s="3"/>
       <c r="N148" s="3"/>
       <c r="O148" s="3"/>
@@ -6062,8 +6100,8 @@
       <c r="B149" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C149" s="5" t="s">
-        <v>436</v>
+      <c r="C149" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -6084,13 +6122,13 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>438</v>
-      </c>
       <c r="C150" s="5" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -6111,40 +6149,40 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C151" s="5" t="s">
         <v>440</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>441</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
       <c r="K151" s="4"/>
       <c r="L151" s="4"/>
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
-      <c r="O151" s="3"/>
-      <c r="P151" s="3"/>
-      <c r="Q151" s="3"/>
-      <c r="R151" s="3"/>
-      <c r="S151" s="3"/>
-      <c r="T151" s="3"/>
-      <c r="U151" s="3"/>
-      <c r="V151" s="3"/>
-      <c r="W151" s="3"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="4"/>
+      <c r="S151" s="4"/>
+      <c r="T151" s="4"/>
+      <c r="U151" s="4"/>
+      <c r="V151" s="4"/>
+      <c r="W151" s="4"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>439</v>
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -6205,17 +6243,17 @@
       <c r="J154" s="4"/>
       <c r="K154" s="4"/>
       <c r="L154" s="4"/>
-      <c r="M154" s="4"/>
-      <c r="N154" s="4"/>
-      <c r="O154" s="4"/>
-      <c r="P154" s="4"/>
-      <c r="Q154" s="4"/>
-      <c r="R154" s="4"/>
-      <c r="S154" s="4"/>
-      <c r="T154" s="4"/>
-      <c r="U154" s="4"/>
-      <c r="V154" s="4"/>
-      <c r="W154" s="4"/>
+      <c r="M154" s="3"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="3"/>
+      <c r="P154" s="3"/>
+      <c r="Q154" s="3"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="3"/>
+      <c r="T154" s="3"/>
+      <c r="U154" s="3"/>
+      <c r="V154" s="3"/>
+      <c r="W154" s="3"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
@@ -6225,7 +6263,7 @@
         <v>451</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -6246,13 +6284,13 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B156" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="C156" s="5" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -6273,13 +6311,13 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C157" s="5" t="s">
         <v>456</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="C157" s="5" t="s">
-        <v>458</v>
       </c>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -6300,13 +6338,13 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C158" s="5" t="s">
         <v>459</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>461</v>
       </c>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -6327,94 +6365,94 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C159" s="5" t="s">
         <v>462</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>464</v>
       </c>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
       <c r="K159" s="4"/>
       <c r="L159" s="4"/>
-      <c r="M159" s="4"/>
-      <c r="N159" s="4"/>
-      <c r="O159" s="4"/>
-      <c r="P159" s="4"/>
-      <c r="Q159" s="4"/>
-      <c r="R159" s="4"/>
-      <c r="S159" s="4"/>
-      <c r="T159" s="4"/>
-      <c r="U159" s="4"/>
-      <c r="V159" s="4"/>
-      <c r="W159" s="4"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
+      <c r="O159" s="3"/>
+      <c r="P159" s="3"/>
+      <c r="Q159" s="3"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="3"/>
+      <c r="T159" s="3"/>
+      <c r="U159" s="3"/>
+      <c r="V159" s="3"/>
+      <c r="W159" s="3"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C160" s="5" t="s">
         <v>465</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C160" s="10" t="s">
-        <v>467</v>
       </c>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
       <c r="L160" s="4"/>
-      <c r="M160" s="4"/>
-      <c r="N160" s="4"/>
-      <c r="O160" s="4"/>
-      <c r="P160" s="4"/>
-      <c r="Q160" s="4"/>
-      <c r="R160" s="4"/>
-      <c r="S160" s="4"/>
-      <c r="T160" s="4"/>
-      <c r="U160" s="4"/>
-      <c r="V160" s="4"/>
-      <c r="W160" s="4"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="3"/>
+      <c r="T160" s="3"/>
+      <c r="U160" s="3"/>
+      <c r="V160" s="3"/>
+      <c r="W160" s="3"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="C161" s="5" t="s">
         <v>468</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>470</v>
       </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
       <c r="J161" s="4"/>
       <c r="K161" s="4"/>
       <c r="L161" s="4"/>
-      <c r="M161" s="4"/>
-      <c r="N161" s="4"/>
-      <c r="O161" s="4"/>
-      <c r="P161" s="4"/>
-      <c r="Q161" s="4"/>
-      <c r="R161" s="4"/>
-      <c r="S161" s="4"/>
-      <c r="T161" s="4"/>
-      <c r="U161" s="4"/>
-      <c r="V161" s="4"/>
-      <c r="W161" s="4"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
+      <c r="O161" s="3"/>
+      <c r="P161" s="3"/>
+      <c r="Q161" s="3"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="3"/>
+      <c r="T161" s="3"/>
+      <c r="U161" s="3"/>
+      <c r="V161" s="3"/>
+      <c r="W161" s="3"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C162" s="5" t="s">
         <v>471</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>473</v>
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -6435,13 +6473,13 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>474</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>476</v>
       </c>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -6462,67 +6500,67 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C164" s="10" t="s">
         <v>477</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>479</v>
       </c>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
       <c r="J164" s="4"/>
       <c r="K164" s="4"/>
       <c r="L164" s="4"/>
-      <c r="M164" s="3"/>
-      <c r="N164" s="3"/>
-      <c r="O164" s="3"/>
-      <c r="P164" s="3"/>
-      <c r="Q164" s="3"/>
-      <c r="R164" s="3"/>
-      <c r="S164" s="3"/>
-      <c r="T164" s="3"/>
-      <c r="U164" s="3"/>
-      <c r="V164" s="3"/>
-      <c r="W164" s="3"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="4"/>
+      <c r="S164" s="4"/>
+      <c r="T164" s="4"/>
+      <c r="U164" s="4"/>
+      <c r="V164" s="4"/>
+      <c r="W164" s="4"/>
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C165" s="5" t="s">
         <v>480</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>482</v>
       </c>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
       <c r="K165" s="4"/>
       <c r="L165" s="4"/>
-      <c r="M165" s="3"/>
-      <c r="N165" s="3"/>
-      <c r="O165" s="3"/>
-      <c r="P165" s="3"/>
-      <c r="Q165" s="3"/>
-      <c r="R165" s="3"/>
-      <c r="S165" s="3"/>
-      <c r="T165" s="3"/>
-      <c r="U165" s="3"/>
-      <c r="V165" s="3"/>
-      <c r="W165" s="3"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="4"/>
+      <c r="S165" s="4"/>
+      <c r="T165" s="4"/>
+      <c r="U165" s="4"/>
+      <c r="V165" s="4"/>
+      <c r="W165" s="4"/>
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C166" s="5" t="s">
         <v>483</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>485</v>
       </c>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -6543,40 +6581,40 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C167" s="5" t="s">
         <v>486</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C167" s="5" t="s">
-        <v>487</v>
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
-      <c r="M167" s="3"/>
-      <c r="N167" s="3"/>
-      <c r="O167" s="3"/>
-      <c r="P167" s="3"/>
-      <c r="Q167" s="3"/>
-      <c r="R167" s="3"/>
-      <c r="S167" s="3"/>
-      <c r="T167" s="3"/>
-      <c r="U167" s="3"/>
-      <c r="V167" s="3"/>
-      <c r="W167" s="3"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="4"/>
+      <c r="S167" s="4"/>
+      <c r="T167" s="4"/>
+      <c r="U167" s="4"/>
+      <c r="V167" s="4"/>
+      <c r="W167" s="4"/>
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="C168" s="5" t="s">
         <v>489</v>
-      </c>
-      <c r="C168" s="5" t="s">
-        <v>490</v>
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
@@ -6597,13 +6635,13 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>493</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6623,44 +6661,41 @@
       <c r="W169" s="3"/>
     </row>
     <row r="170" ht="14.25" customHeight="1">
-      <c r="A170" s="6" t="s">
+      <c r="A170" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B170" s="6" t="s">
+      <c r="C170" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="C170" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
-      <c r="I170" s="3"/>
-      <c r="J170" s="3"/>
-      <c r="K170" s="3"/>
-      <c r="L170" s="3"/>
-      <c r="M170" s="3"/>
-      <c r="N170" s="3"/>
-      <c r="O170" s="3"/>
-      <c r="P170" s="3"/>
-      <c r="Q170" s="3"/>
-      <c r="R170" s="3"/>
-      <c r="S170" s="3"/>
-      <c r="T170" s="3"/>
-      <c r="U170" s="3"/>
-      <c r="V170" s="3"/>
-      <c r="W170" s="3"/>
+      <c r="H170" s="4"/>
+      <c r="I170" s="4"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="4"/>
+      <c r="L170" s="4"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
+      <c r="R170" s="4"/>
+      <c r="S170" s="4"/>
+      <c r="T170" s="4"/>
+      <c r="U170" s="4"/>
+      <c r="V170" s="4"/>
+      <c r="W170" s="4"/>
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B171" s="2" t="s">
-        <v>498</v>
-      </c>
       <c r="C171" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -6681,241 +6716,238 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="C172" s="5" t="s">
         <v>500</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>501</v>
       </c>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
       <c r="K172" s="4"/>
       <c r="L172" s="4"/>
-      <c r="M172" s="4"/>
-      <c r="N172" s="4"/>
-      <c r="O172" s="4"/>
-      <c r="P172" s="4"/>
-      <c r="Q172" s="4"/>
-      <c r="R172" s="4"/>
-      <c r="S172" s="4"/>
-      <c r="T172" s="4"/>
-      <c r="U172" s="4"/>
-      <c r="V172" s="4"/>
-      <c r="W172" s="4"/>
+      <c r="M172" s="3"/>
+      <c r="N172" s="3"/>
+      <c r="O172" s="3"/>
+      <c r="P172" s="3"/>
+      <c r="Q172" s="3"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="3"/>
+      <c r="T172" s="3"/>
+      <c r="U172" s="3"/>
+      <c r="V172" s="3"/>
+      <c r="W172" s="3"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="5" t="s">
         <v>503</v>
-      </c>
-      <c r="C173" s="5" t="s">
-        <v>504</v>
       </c>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
       <c r="K173" s="4"/>
       <c r="L173" s="4"/>
-      <c r="M173" s="4"/>
-      <c r="N173" s="4"/>
-      <c r="O173" s="4"/>
-      <c r="P173" s="4"/>
-      <c r="Q173" s="4"/>
-      <c r="R173" s="4"/>
-      <c r="S173" s="4"/>
-      <c r="T173" s="4"/>
-      <c r="U173" s="4"/>
-      <c r="V173" s="4"/>
-      <c r="W173" s="4"/>
+      <c r="M173" s="3"/>
+      <c r="N173" s="3"/>
+      <c r="O173" s="3"/>
+      <c r="P173" s="3"/>
+      <c r="Q173" s="3"/>
+      <c r="R173" s="3"/>
+      <c r="S173" s="3"/>
+      <c r="T173" s="3"/>
+      <c r="U173" s="3"/>
+      <c r="V173" s="3"/>
+      <c r="W173" s="3"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B174" s="6" t="s">
         <v>505</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="C174" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="C174" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="H174" s="4"/>
-      <c r="I174" s="4"/>
-      <c r="J174" s="4"/>
-      <c r="K174" s="4"/>
-      <c r="L174" s="4"/>
-      <c r="M174" s="4"/>
-      <c r="N174" s="4"/>
-      <c r="O174" s="4"/>
-      <c r="P174" s="4"/>
-      <c r="Q174" s="4"/>
-      <c r="R174" s="4"/>
-      <c r="S174" s="4"/>
-      <c r="T174" s="4"/>
-      <c r="U174" s="4"/>
-      <c r="V174" s="4"/>
-      <c r="W174" s="4"/>
+      <c r="E174" s="3"/>
+      <c r="F174" s="3"/>
+      <c r="G174" s="3"/>
+      <c r="H174" s="3"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="3"/>
+      <c r="K174" s="3"/>
+      <c r="L174" s="3"/>
+      <c r="M174" s="3"/>
+      <c r="N174" s="3"/>
+      <c r="O174" s="3"/>
+      <c r="P174" s="3"/>
+      <c r="Q174" s="3"/>
+      <c r="R174" s="3"/>
+      <c r="S174" s="3"/>
+      <c r="T174" s="3"/>
+      <c r="U174" s="3"/>
+      <c r="V174" s="3"/>
+      <c r="W174" s="3"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>509</v>
-      </c>
       <c r="C175" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
       <c r="J175" s="4"/>
       <c r="K175" s="4"/>
       <c r="L175" s="4"/>
-      <c r="M175" s="4"/>
-      <c r="N175" s="4"/>
-      <c r="O175" s="4"/>
-      <c r="P175" s="4"/>
-      <c r="Q175" s="4"/>
-      <c r="R175" s="4"/>
-      <c r="S175" s="4"/>
-      <c r="T175" s="4"/>
-      <c r="U175" s="4"/>
-      <c r="V175" s="4"/>
-      <c r="W175" s="4"/>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
+      <c r="O175" s="3"/>
+      <c r="P175" s="3"/>
+      <c r="Q175" s="3"/>
+      <c r="R175" s="3"/>
+      <c r="S175" s="3"/>
+      <c r="T175" s="3"/>
+      <c r="U175" s="3"/>
+      <c r="V175" s="3"/>
+      <c r="W175" s="3"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" s="1" t="s">
+      <c r="A176" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C176" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="H176" s="4"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="4"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="4"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+      <c r="U176" s="4"/>
+      <c r="V176" s="4"/>
+      <c r="W176" s="4"/>
+    </row>
+    <row r="177" ht="14.25" customHeight="1">
+      <c r="A177" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="C176" s="5" t="s">
+      <c r="B177" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="H176" s="3"/>
-      <c r="I176" s="3"/>
-      <c r="J176" s="3"/>
-      <c r="K176" s="3"/>
-      <c r="L176" s="3"/>
-      <c r="M176" s="3"/>
-      <c r="N176" s="3"/>
-      <c r="O176" s="3"/>
-      <c r="P176" s="3"/>
-      <c r="Q176" s="3"/>
-      <c r="R176" s="3"/>
-      <c r="S176" s="3"/>
-      <c r="T176" s="3"/>
-      <c r="U176" s="3"/>
-      <c r="V176" s="3"/>
-      <c r="W176" s="3"/>
-    </row>
-    <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" s="1" t="s">
+      <c r="C177" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="B177" s="6" t="s">
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="4"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="4"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+      <c r="U177" s="4"/>
+      <c r="V177" s="4"/>
+      <c r="W177" s="4"/>
+    </row>
+    <row r="178" ht="14.25" customHeight="1">
+      <c r="A178" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="C177" s="5" t="s">
+      <c r="B178" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E177" s="3"/>
-      <c r="F177" s="3"/>
-      <c r="G177" s="3"/>
-      <c r="H177" s="3"/>
-      <c r="I177" s="3"/>
-      <c r="J177" s="3"/>
-      <c r="K177" s="3"/>
-      <c r="L177" s="3"/>
-      <c r="M177" s="3"/>
-      <c r="N177" s="3"/>
-      <c r="O177" s="3"/>
-      <c r="P177" s="3"/>
-      <c r="Q177" s="3"/>
-      <c r="R177" s="3"/>
-      <c r="S177" s="3"/>
-      <c r="T177" s="3"/>
-      <c r="U177" s="3"/>
-      <c r="V177" s="3"/>
-      <c r="W177" s="3"/>
-    </row>
-    <row r="178" ht="14.25" customHeight="1">
-      <c r="A178" s="1" t="s">
+      <c r="C178" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="4"/>
+      <c r="M178" s="4"/>
+      <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
+      <c r="P178" s="4"/>
+      <c r="Q178" s="4"/>
+      <c r="R178" s="4"/>
+      <c r="S178" s="4"/>
+      <c r="T178" s="4"/>
+      <c r="U178" s="4"/>
+      <c r="V178" s="4"/>
+      <c r="W178" s="4"/>
+    </row>
+    <row r="179" ht="14.25" customHeight="1">
+      <c r="A179" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="C178" s="10" t="s">
+      <c r="B179" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="H178" s="3"/>
-      <c r="I178" s="3"/>
-      <c r="J178" s="3"/>
-      <c r="K178" s="3"/>
-      <c r="L178" s="3"/>
-      <c r="M178" s="3"/>
-      <c r="N178" s="3"/>
-      <c r="O178" s="3"/>
-      <c r="P178" s="3"/>
-      <c r="Q178" s="3"/>
-      <c r="R178" s="3"/>
-      <c r="S178" s="3"/>
-      <c r="T178" s="3"/>
-      <c r="U178" s="3"/>
-      <c r="V178" s="3"/>
-      <c r="W178" s="3"/>
-    </row>
-    <row r="179" ht="14.25" customHeight="1">
-      <c r="A179" s="1" t="s">
+      <c r="C179" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="H179" s="4"/>
+      <c r="I179" s="4"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="4"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="4"/>
+      <c r="S179" s="4"/>
+      <c r="T179" s="4"/>
+      <c r="U179" s="4"/>
+      <c r="V179" s="4"/>
+      <c r="W179" s="4"/>
+    </row>
+    <row r="180" ht="14.25" customHeight="1">
+      <c r="A180" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C179" s="5" t="s">
+      <c r="B180" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
-      <c r="G179" s="3"/>
-      <c r="H179" s="3"/>
-      <c r="I179" s="3"/>
-      <c r="J179" s="3"/>
-      <c r="K179" s="3"/>
-      <c r="L179" s="3"/>
-      <c r="M179" s="3"/>
-      <c r="N179" s="3"/>
-      <c r="O179" s="3"/>
-      <c r="P179" s="3"/>
-      <c r="Q179" s="3"/>
-      <c r="R179" s="3"/>
-      <c r="S179" s="3"/>
-      <c r="T179" s="3"/>
-      <c r="U179" s="3"/>
-      <c r="V179" s="3"/>
-      <c r="W179" s="3"/>
-    </row>
-    <row r="180" ht="14.25" customHeight="1">
-      <c r="A180" s="2" t="s">
+      <c r="C180" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="B180" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="C180" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="H180" s="4"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="4"/>
-      <c r="K180" s="4"/>
-      <c r="L180" s="4"/>
+      <c r="H180" s="3"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="3"/>
+      <c r="K180" s="3"/>
+      <c r="L180" s="3"/>
       <c r="M180" s="3"/>
       <c r="N180" s="3"/>
       <c r="O180" s="3"/>
@@ -6929,20 +6961,23 @@
       <c r="W180" s="3"/>
     </row>
     <row r="181" ht="14.25" customHeight="1">
-      <c r="A181" s="2" t="s">
+      <c r="A181" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B181" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="C181" s="5" t="s">
         <v>526</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="C181" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="H181" s="4"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="4"/>
-      <c r="K181" s="4"/>
-      <c r="L181" s="4"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="3"/>
+      <c r="K181" s="3"/>
+      <c r="L181" s="3"/>
       <c r="M181" s="3"/>
       <c r="N181" s="3"/>
       <c r="O181" s="3"/>
@@ -6956,19 +6991,15 @@
       <c r="W181" s="3"/>
     </row>
     <row r="182" ht="14.25" customHeight="1">
-      <c r="A182" s="2" t="s">
+      <c r="A182" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C182" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="B182" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="D182" s="3"/>
-      <c r="E182" s="3"/>
-      <c r="F182" s="3"/>
-      <c r="G182" s="3"/>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
@@ -6987,20 +7018,23 @@
       <c r="W182" s="3"/>
     </row>
     <row r="183" ht="14.25" customHeight="1">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="C183" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="C183" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="H183" s="4"/>
-      <c r="I183" s="4"/>
-      <c r="J183" s="4"/>
-      <c r="K183" s="4"/>
-      <c r="L183" s="4"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="3"/>
+      <c r="K183" s="3"/>
+      <c r="L183" s="3"/>
       <c r="M183" s="3"/>
       <c r="N183" s="3"/>
       <c r="O183" s="3"/>
@@ -7014,23 +7048,20 @@
       <c r="W183" s="3"/>
     </row>
     <row r="184" ht="14.25" customHeight="1">
-      <c r="A184" s="6" t="s">
+      <c r="A184" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C184" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="B184" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="C184" s="5" t="s">
-        <v>537</v>
-      </c>
-      <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
-      <c r="G184" s="3"/>
-      <c r="H184" s="3"/>
-      <c r="I184" s="3"/>
-      <c r="J184" s="3"/>
-      <c r="K184" s="3"/>
-      <c r="L184" s="3"/>
+      <c r="H184" s="4"/>
+      <c r="I184" s="4"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="4"/>
+      <c r="L184" s="4"/>
       <c r="M184" s="3"/>
       <c r="N184" s="3"/>
       <c r="O184" s="3"/>
@@ -7044,23 +7075,20 @@
       <c r="W184" s="3"/>
     </row>
     <row r="185" ht="14.25" customHeight="1">
-      <c r="A185" s="6" t="s">
+      <c r="A185" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C185" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B185" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
-      <c r="G185" s="3"/>
-      <c r="H185" s="3"/>
-      <c r="I185" s="3"/>
-      <c r="J185" s="3"/>
-      <c r="K185" s="3"/>
-      <c r="L185" s="3"/>
+      <c r="H185" s="4"/>
+      <c r="I185" s="4"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="4"/>
+      <c r="L185" s="4"/>
       <c r="M185" s="3"/>
       <c r="N185" s="3"/>
       <c r="O185" s="3"/>
@@ -7075,73 +7103,80 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="C186" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="H186" s="4"/>
-      <c r="I186" s="4"/>
-      <c r="J186" s="4"/>
-      <c r="K186" s="4"/>
-      <c r="L186" s="4"/>
-      <c r="M186" s="4"/>
-      <c r="N186" s="4"/>
-      <c r="O186" s="4"/>
-      <c r="P186" s="4"/>
-      <c r="Q186" s="4"/>
-      <c r="R186" s="4"/>
-      <c r="S186" s="4"/>
-      <c r="T186" s="4"/>
-      <c r="U186" s="4"/>
-      <c r="V186" s="4"/>
-      <c r="W186" s="4"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="3"/>
+      <c r="K186" s="3"/>
+      <c r="L186" s="3"/>
+      <c r="M186" s="3"/>
+      <c r="N186" s="3"/>
+      <c r="O186" s="3"/>
+      <c r="P186" s="3"/>
+      <c r="Q186" s="3"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="3"/>
+      <c r="T186" s="3"/>
+      <c r="U186" s="3"/>
+      <c r="V186" s="3"/>
+      <c r="W186" s="3"/>
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C187" s="5" t="s">
         <v>544</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C187" s="10" t="s">
-        <v>546</v>
       </c>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
       <c r="J187" s="4"/>
       <c r="K187" s="4"/>
       <c r="L187" s="4"/>
-      <c r="M187" s="4"/>
-      <c r="N187" s="4"/>
-      <c r="O187" s="4"/>
-      <c r="P187" s="4"/>
-      <c r="Q187" s="4"/>
-      <c r="R187" s="4"/>
-      <c r="S187" s="4"/>
-      <c r="T187" s="4"/>
-      <c r="U187" s="4"/>
-      <c r="V187" s="4"/>
-      <c r="W187" s="4"/>
+      <c r="M187" s="3"/>
+      <c r="N187" s="3"/>
+      <c r="O187" s="3"/>
+      <c r="P187" s="3"/>
+      <c r="Q187" s="3"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="3"/>
+      <c r="T187" s="3"/>
+      <c r="U187" s="3"/>
+      <c r="V187" s="3"/>
+      <c r="W187" s="3"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" s="1" t="s">
+      <c r="A188" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C188" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C188" s="5" t="s">
-        <v>549</v>
-      </c>
-      <c r="H188" s="4"/>
-      <c r="I188" s="4"/>
-      <c r="J188" s="4"/>
-      <c r="K188" s="4"/>
-      <c r="L188" s="4"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="3"/>
+      <c r="K188" s="3"/>
+      <c r="L188" s="3"/>
       <c r="M188" s="3"/>
       <c r="N188" s="3"/>
       <c r="O188" s="3"/>
@@ -7155,41 +7190,44 @@
       <c r="W188" s="3"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" s="2" t="s">
+      <c r="A189" s="6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C189" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C189" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="H189" s="4"/>
-      <c r="I189" s="4"/>
-      <c r="J189" s="4"/>
-      <c r="K189" s="4"/>
-      <c r="L189" s="4"/>
-      <c r="M189" s="4"/>
-      <c r="N189" s="4"/>
-      <c r="O189" s="4"/>
-      <c r="P189" s="4"/>
-      <c r="Q189" s="4"/>
-      <c r="R189" s="4"/>
-      <c r="S189" s="4"/>
-      <c r="T189" s="4"/>
-      <c r="U189" s="4"/>
-      <c r="V189" s="4"/>
-      <c r="W189" s="4"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="3"/>
+      <c r="K189" s="3"/>
+      <c r="L189" s="3"/>
+      <c r="M189" s="3"/>
+      <c r="N189" s="3"/>
+      <c r="O189" s="3"/>
+      <c r="P189" s="3"/>
+      <c r="Q189" s="3"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="3"/>
+      <c r="T189" s="3"/>
+      <c r="U189" s="3"/>
+      <c r="V189" s="3"/>
+      <c r="W189" s="3"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C190" s="5" t="s">
         <v>553</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="C190" s="5" t="s">
-        <v>555</v>
       </c>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
@@ -7209,41 +7247,41 @@
       <c r="W190" s="4"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="A191" s="1" t="s">
+      <c r="A191" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C191" s="10" t="s">
         <v>556</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="C191" s="5" t="s">
-        <v>558</v>
       </c>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
       <c r="J191" s="4"/>
       <c r="K191" s="4"/>
       <c r="L191" s="4"/>
-      <c r="M191" s="3"/>
-      <c r="N191" s="3"/>
-      <c r="O191" s="3"/>
-      <c r="P191" s="3"/>
-      <c r="Q191" s="3"/>
-      <c r="R191" s="3"/>
-      <c r="S191" s="3"/>
-      <c r="T191" s="3"/>
-      <c r="U191" s="3"/>
-      <c r="V191" s="3"/>
-      <c r="W191" s="3"/>
+      <c r="M191" s="4"/>
+      <c r="N191" s="4"/>
+      <c r="O191" s="4"/>
+      <c r="P191" s="4"/>
+      <c r="Q191" s="4"/>
+      <c r="R191" s="4"/>
+      <c r="S191" s="4"/>
+      <c r="T191" s="4"/>
+      <c r="U191" s="4"/>
+      <c r="V191" s="4"/>
+      <c r="W191" s="4"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C192" s="5" t="s">
         <v>559</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="C192" s="5" t="s">
-        <v>561</v>
       </c>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
@@ -7264,13 +7302,13 @@
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C193" s="5" t="s">
         <v>562</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="C193" s="5" t="s">
-        <v>564</v>
       </c>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
@@ -7291,50 +7329,46 @@
     </row>
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C194" s="5" t="s">
         <v>565</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C194" s="5" t="s">
-        <v>567</v>
       </c>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
       <c r="J194" s="4"/>
       <c r="K194" s="4"/>
       <c r="L194" s="4"/>
-      <c r="M194" s="3"/>
-      <c r="N194" s="3"/>
-      <c r="O194" s="3"/>
-      <c r="P194" s="3"/>
-      <c r="Q194" s="3"/>
-      <c r="R194" s="3"/>
-      <c r="S194" s="3"/>
-      <c r="T194" s="3"/>
-      <c r="U194" s="3"/>
-      <c r="V194" s="3"/>
-      <c r="W194" s="3"/>
+      <c r="M194" s="4"/>
+      <c r="N194" s="4"/>
+      <c r="O194" s="4"/>
+      <c r="P194" s="4"/>
+      <c r="Q194" s="4"/>
+      <c r="R194" s="4"/>
+      <c r="S194" s="4"/>
+      <c r="T194" s="4"/>
+      <c r="U194" s="4"/>
+      <c r="V194" s="4"/>
+      <c r="W194" s="4"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="A195" s="6" t="s">
+      <c r="A195" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C195" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="B195" s="6" t="s">
-        <v>569</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="D195" s="3"/>
-      <c r="E195" s="3"/>
-      <c r="F195" s="3"/>
-      <c r="G195" s="3"/>
-      <c r="H195" s="3"/>
-      <c r="I195" s="3"/>
-      <c r="J195" s="3"/>
-      <c r="K195" s="3"/>
-      <c r="L195" s="3"/>
+      <c r="H195" s="4"/>
+      <c r="I195" s="4"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+      <c r="L195" s="4"/>
       <c r="M195" s="3"/>
       <c r="N195" s="3"/>
       <c r="O195" s="3"/>
@@ -7348,18 +7382,20 @@
       <c r="W195" s="3"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="A196" s="4"/>
-      <c r="B196" s="4"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
-      <c r="E196" s="3"/>
-      <c r="F196" s="3"/>
-      <c r="G196" s="3"/>
-      <c r="H196" s="3"/>
-      <c r="I196" s="3"/>
-      <c r="J196" s="3"/>
-      <c r="K196" s="3"/>
-      <c r="L196" s="3"/>
+      <c r="A196" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="H196" s="4"/>
+      <c r="I196" s="4"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="4"/>
+      <c r="L196" s="4"/>
       <c r="M196" s="3"/>
       <c r="N196" s="3"/>
       <c r="O196" s="3"/>
@@ -7373,43 +7409,47 @@
       <c r="W196" s="3"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="A197" s="4"/>
-      <c r="B197" s="4"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
-      <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
-      <c r="I197" s="3"/>
-      <c r="J197" s="3"/>
-      <c r="K197" s="3"/>
-      <c r="L197" s="3"/>
-      <c r="M197" s="3"/>
-      <c r="N197" s="3"/>
-      <c r="O197" s="3"/>
-      <c r="P197" s="3"/>
-      <c r="Q197" s="3"/>
-      <c r="R197" s="3"/>
-      <c r="S197" s="3"/>
-      <c r="T197" s="3"/>
-      <c r="U197" s="3"/>
-      <c r="V197" s="3"/>
-      <c r="W197" s="3"/>
+      <c r="A197" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="H197" s="4"/>
+      <c r="I197" s="4"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="4"/>
+      <c r="L197" s="4"/>
+      <c r="M197" s="4"/>
+      <c r="N197" s="4"/>
+      <c r="O197" s="4"/>
+      <c r="P197" s="4"/>
+      <c r="Q197" s="4"/>
+      <c r="R197" s="4"/>
+      <c r="S197" s="4"/>
+      <c r="T197" s="4"/>
+      <c r="U197" s="4"/>
+      <c r="V197" s="4"/>
+      <c r="W197" s="4"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="A198" s="4"/>
-      <c r="B198" s="4"/>
-      <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
-      <c r="E198" s="3"/>
-      <c r="F198" s="3"/>
-      <c r="G198" s="3"/>
-      <c r="H198" s="3"/>
-      <c r="I198" s="3"/>
-      <c r="J198" s="3"/>
-      <c r="K198" s="3"/>
-      <c r="L198" s="3"/>
+      <c r="A198" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="H198" s="4"/>
+      <c r="I198" s="4"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="4"/>
+      <c r="L198" s="4"/>
       <c r="M198" s="3"/>
       <c r="N198" s="3"/>
       <c r="O198" s="3"/>

</xml_diff>

<commit_message>
Achievement and leaderboard names in Italian.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="607">
   <si>
     <t>Key</t>
   </si>
@@ -490,7 +490,8 @@
 Click the button below to fill out a questionnaire and receive your final feedback.</t>
   </si>
   <si>
-    <t>XXXX</t>
+    <t>Questa era la gara finale e ora hai completato il campionato.
+Clicca il pulsante qui sotto per compilare un questionario e ricevere il feedback finale.</t>
   </si>
   <si>
     <t>ENGLISH</t>
@@ -1104,6 +1105,9 @@
     <t>Final Cup Position</t>
   </si>
   <si>
+    <t>Posizione Finale in classifica</t>
+  </si>
+  <si>
     <t>OVERWRITE</t>
   </si>
   <si>
@@ -1409,6 +1413,9 @@
   </si>
   <si>
     <t>Race Results</t>
+  </si>
+  <si>
+    <t>Risultati della gara</t>
   </si>
   <si>
     <t>RACE_SKIP_CONFIRM_ALLOWANCE_REMAINING</t>
@@ -1859,6 +1866,87 @@
   </si>
   <si>
     <t>Tu</t>
+  </si>
+  <si>
+    <t>QUESTIONS_ASKED</t>
+  </si>
+  <si>
+    <t>Questions Asked</t>
+  </si>
+  <si>
+    <t>Domande sottoposte</t>
+  </si>
+  <si>
+    <t>FASTEST_TIME</t>
+  </si>
+  <si>
+    <t>Fastest Time</t>
+  </si>
+  <si>
+    <t>Miglior tempo</t>
+  </si>
+  <si>
+    <t>TUTORIAL_COMPLETE</t>
+  </si>
+  <si>
+    <t>Tutorial Complete!</t>
+  </si>
+  <si>
+    <t>Tutorial completato!</t>
+  </si>
+  <si>
+    <t>RACE_WINNER</t>
+  </si>
+  <si>
+    <t>Race Winner</t>
+  </si>
+  <si>
+    <t>Vincitore della gara</t>
+  </si>
+  <si>
+    <t>UNHAPPY_BUT_VICTORIOUS</t>
+  </si>
+  <si>
+    <t>Unhappy But Victorious</t>
+  </si>
+  <si>
+    <t>Infelice ma vittorioso</t>
+  </si>
+  <si>
+    <t>FIVE_HOURS_LATER</t>
+  </si>
+  <si>
+    <t>Five Hours Later...</t>
+  </si>
+  <si>
+    <t>Cinque ore dopo</t>
+  </si>
+  <si>
+    <t>NIGHT_AND_DAY_AND_SO_ON</t>
+  </si>
+  <si>
+    <t>Night And Day And So On</t>
+  </si>
+  <si>
+    <t>Notte e giorno e così via</t>
+  </si>
+  <si>
+    <t>POSITIVE_OUTLOOK</t>
+  </si>
+  <si>
+    <t>Positive Outlook</t>
+  </si>
+  <si>
+    <t>Atteggiamento positivo</t>
+  </si>
+  <si>
+    <t>NO_WASTED_TIME</t>
+  </si>
+  <si>
+    <t>No Wasted Time</t>
+  </si>
+  <si>
+    <t>Non perdere tempo</t>
   </si>
 </sst>
 </file>
@@ -5139,7 +5227,7 @@
         <v>332</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>134</v>
+        <v>333</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -5164,13 +5252,13 @@
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -5191,13 +5279,13 @@
     </row>
     <row r="116" ht="14.25" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
@@ -5218,13 +5306,13 @@
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -5245,13 +5333,13 @@
     </row>
     <row r="118" ht="14.25" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -5272,13 +5360,13 @@
     </row>
     <row r="119" ht="14.25" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -5299,13 +5387,13 @@
     </row>
     <row r="120" ht="14.25" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
@@ -5326,13 +5414,13 @@
     </row>
     <row r="121" ht="14.25" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -5353,13 +5441,13 @@
     </row>
     <row r="122" ht="14.25" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
@@ -5380,13 +5468,13 @@
     </row>
     <row r="123" ht="14.25" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -5407,13 +5495,13 @@
     </row>
     <row r="124" ht="14.25" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -5434,13 +5522,13 @@
     </row>
     <row r="125" ht="14.25" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C125" s="10" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -5461,13 +5549,13 @@
     </row>
     <row r="126" ht="14.25" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -5488,13 +5576,13 @@
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -5515,13 +5603,13 @@
     </row>
     <row r="128" ht="14.25" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
@@ -5542,13 +5630,13 @@
     </row>
     <row r="129" ht="14.25" customHeight="1">
       <c r="A129" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -5569,13 +5657,13 @@
     </row>
     <row r="130" ht="14.25" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
@@ -5596,13 +5684,13 @@
     </row>
     <row r="131" ht="14.25" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
@@ -5623,13 +5711,13 @@
     </row>
     <row r="132" ht="14.25" customHeight="1">
       <c r="A132" s="6" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
@@ -5653,13 +5741,13 @@
     </row>
     <row r="133" ht="14.25" customHeight="1">
       <c r="A133" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
@@ -5680,13 +5768,13 @@
     </row>
     <row r="134" ht="14.25" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
@@ -5707,13 +5795,13 @@
     </row>
     <row r="135" ht="14.25" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -5734,13 +5822,13 @@
     </row>
     <row r="136" ht="14.25" customHeight="1">
       <c r="A136" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -5761,13 +5849,13 @@
     </row>
     <row r="137" ht="14.25" customHeight="1">
       <c r="A137" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E137" s="3"/>
       <c r="F137" s="3"/>
@@ -5791,13 +5879,13 @@
     </row>
     <row r="138" ht="14.25" customHeight="1">
       <c r="A138" s="6" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C138" s="16" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
@@ -5821,13 +5909,13 @@
     </row>
     <row r="139" ht="14.25" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -5848,13 +5936,13 @@
     </row>
     <row r="140" ht="14.25" customHeight="1">
       <c r="A140" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -5875,13 +5963,13 @@
     </row>
     <row r="141" ht="14.25" customHeight="1">
       <c r="A141" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -5902,13 +5990,13 @@
     </row>
     <row r="142" ht="14.25" customHeight="1">
       <c r="A142" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -5929,13 +6017,13 @@
     </row>
     <row r="143" ht="14.25" customHeight="1">
       <c r="A143" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -5956,13 +6044,13 @@
     </row>
     <row r="144" ht="14.25" customHeight="1">
       <c r="A144" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -5983,13 +6071,13 @@
     </row>
     <row r="145" ht="14.25" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -6010,13 +6098,13 @@
     </row>
     <row r="146" ht="14.25" customHeight="1">
       <c r="A146" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -6037,13 +6125,13 @@
     </row>
     <row r="147" ht="14.25" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -6064,13 +6152,13 @@
     </row>
     <row r="148" ht="14.25" customHeight="1">
       <c r="A148" s="6" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>134</v>
+        <v>435</v>
       </c>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
@@ -6095,13 +6183,13 @@
     </row>
     <row r="149" ht="14.25" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -6122,13 +6210,13 @@
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="A150" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -6149,13 +6237,13 @@
     </row>
     <row r="151" ht="14.25" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -6176,13 +6264,13 @@
     </row>
     <row r="152" ht="14.25" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -6203,13 +6291,13 @@
     </row>
     <row r="153" ht="14.25" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -6230,13 +6318,13 @@
     </row>
     <row r="154" ht="14.25" customHeight="1">
       <c r="A154" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -6257,13 +6345,13 @@
     </row>
     <row r="155" ht="14.25" customHeight="1">
       <c r="A155" s="2" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -6284,13 +6372,13 @@
     </row>
     <row r="156" ht="14.25" customHeight="1">
       <c r="A156" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -6311,13 +6399,13 @@
     </row>
     <row r="157" ht="14.25" customHeight="1">
       <c r="A157" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -6338,13 +6426,13 @@
     </row>
     <row r="158" ht="14.25" customHeight="1">
       <c r="A158" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -6365,13 +6453,13 @@
     </row>
     <row r="159" ht="14.25" customHeight="1">
       <c r="A159" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
@@ -6392,13 +6480,13 @@
     </row>
     <row r="160" ht="14.25" customHeight="1">
       <c r="A160" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -6419,13 +6507,13 @@
     </row>
     <row r="161" ht="14.25" customHeight="1">
       <c r="A161" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -6446,13 +6534,13 @@
     </row>
     <row r="162" ht="14.25" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -6473,13 +6561,13 @@
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -6500,13 +6588,13 @@
     </row>
     <row r="164" ht="14.25" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C164" s="10" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
@@ -6527,13 +6615,13 @@
     </row>
     <row r="165" ht="14.25" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
@@ -6554,13 +6642,13 @@
     </row>
     <row r="166" ht="14.25" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -6581,13 +6669,13 @@
     </row>
     <row r="167" ht="14.25" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
@@ -6608,13 +6696,13 @@
     </row>
     <row r="168" ht="14.25" customHeight="1">
       <c r="A168" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
@@ -6635,13 +6723,13 @@
     </row>
     <row r="169" ht="14.25" customHeight="1">
       <c r="A169" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -6662,13 +6750,13 @@
     </row>
     <row r="170" ht="14.25" customHeight="1">
       <c r="A170" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
@@ -6689,13 +6777,13 @@
     </row>
     <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -6716,13 +6804,13 @@
     </row>
     <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
@@ -6743,13 +6831,13 @@
     </row>
     <row r="173" ht="14.25" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
@@ -6770,13 +6858,13 @@
     </row>
     <row r="174" ht="14.25" customHeight="1">
       <c r="A174" s="6" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
@@ -6800,13 +6888,13 @@
     </row>
     <row r="175" ht="14.25" customHeight="1">
       <c r="A175" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
@@ -6827,13 +6915,13 @@
     </row>
     <row r="176" ht="14.25" customHeight="1">
       <c r="A176" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
@@ -6854,13 +6942,13 @@
     </row>
     <row r="177" ht="14.25" customHeight="1">
       <c r="A177" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
@@ -6881,13 +6969,13 @@
     </row>
     <row r="178" ht="14.25" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
@@ -6908,13 +6996,13 @@
     </row>
     <row r="179" ht="14.25" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
@@ -6935,13 +7023,13 @@
     </row>
     <row r="180" ht="14.25" customHeight="1">
       <c r="A180" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="H180" s="3"/>
       <c r="I180" s="3"/>
@@ -6962,13 +7050,13 @@
     </row>
     <row r="181" ht="14.25" customHeight="1">
       <c r="A181" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E181" s="3"/>
       <c r="F181" s="3"/>
@@ -6992,13 +7080,13 @@
     </row>
     <row r="182" ht="14.25" customHeight="1">
       <c r="A182" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="H182" s="3"/>
       <c r="I182" s="3"/>
@@ -7019,13 +7107,13 @@
     </row>
     <row r="183" ht="14.25" customHeight="1">
       <c r="A183" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B183" s="6" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
@@ -7049,13 +7137,13 @@
     </row>
     <row r="184" ht="14.25" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
@@ -7076,13 +7164,13 @@
     </row>
     <row r="185" ht="14.25" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
@@ -7103,13 +7191,13 @@
     </row>
     <row r="186" ht="14.25" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
@@ -7134,13 +7222,13 @@
     </row>
     <row r="187" ht="14.25" customHeight="1">
       <c r="A187" s="2" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
@@ -7161,13 +7249,13 @@
     </row>
     <row r="188" ht="14.25" customHeight="1">
       <c r="A188" s="6" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
@@ -7191,13 +7279,13 @@
     </row>
     <row r="189" ht="14.25" customHeight="1">
       <c r="A189" s="6" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B189" s="6" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E189" s="3"/>
       <c r="F189" s="3"/>
@@ -7221,13 +7309,13 @@
     </row>
     <row r="190" ht="14.25" customHeight="1">
       <c r="A190" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
@@ -7248,13 +7336,13 @@
     </row>
     <row r="191" ht="14.25" customHeight="1">
       <c r="A191" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
@@ -7275,13 +7363,13 @@
     </row>
     <row r="192" ht="14.25" customHeight="1">
       <c r="A192" s="1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
@@ -7302,13 +7390,13 @@
     </row>
     <row r="193" ht="14.25" customHeight="1">
       <c r="A193" s="2" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
@@ -7329,13 +7417,13 @@
     </row>
     <row r="194" ht="14.25" customHeight="1">
       <c r="A194" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
@@ -7356,13 +7444,13 @@
     </row>
     <row r="195" ht="14.25" customHeight="1">
       <c r="A195" s="1" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
@@ -7383,13 +7471,13 @@
     </row>
     <row r="196" ht="14.25" customHeight="1">
       <c r="A196" s="2" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="H196" s="4"/>
       <c r="I196" s="4"/>
@@ -7410,13 +7498,13 @@
     </row>
     <row r="197" ht="14.25" customHeight="1">
       <c r="A197" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="H197" s="4"/>
       <c r="I197" s="4"/>
@@ -7437,13 +7525,13 @@
     </row>
     <row r="198" ht="14.25" customHeight="1">
       <c r="A198" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="H198" s="4"/>
       <c r="I198" s="4"/>
@@ -7463,9 +7551,15 @@
       <c r="W198" s="3"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="A199" s="4"/>
-      <c r="B199" s="4"/>
-      <c r="C199" s="3"/>
+      <c r="A199" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>582</v>
+      </c>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
       <c r="F199" s="3"/>
@@ -7488,9 +7582,15 @@
       <c r="W199" s="3"/>
     </row>
     <row r="200" ht="14.25" customHeight="1">
-      <c r="A200" s="4"/>
-      <c r="B200" s="4"/>
-      <c r="C200" s="3"/>
+      <c r="A200" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>584</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>585</v>
+      </c>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
@@ -7513,9 +7613,15 @@
       <c r="W200" s="3"/>
     </row>
     <row r="201" ht="14.25" customHeight="1">
-      <c r="A201" s="4"/>
-      <c r="B201" s="4"/>
-      <c r="C201" s="3"/>
+      <c r="A201" s="6" t="s">
+        <v>586</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>588</v>
+      </c>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
@@ -7538,9 +7644,15 @@
       <c r="W201" s="3"/>
     </row>
     <row r="202" ht="14.25" customHeight="1">
-      <c r="A202" s="4"/>
-      <c r="B202" s="4"/>
-      <c r="C202" s="3"/>
+      <c r="A202" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>591</v>
+      </c>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
@@ -7563,9 +7675,15 @@
       <c r="W202" s="3"/>
     </row>
     <row r="203" ht="14.25" customHeight="1">
-      <c r="A203" s="4"/>
-      <c r="B203" s="4"/>
-      <c r="C203" s="3"/>
+      <c r="A203" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>594</v>
+      </c>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
       <c r="F203" s="3"/>
@@ -7588,9 +7706,15 @@
       <c r="W203" s="3"/>
     </row>
     <row r="204" ht="14.25" customHeight="1">
-      <c r="A204" s="4"/>
-      <c r="B204" s="4"/>
-      <c r="C204" s="3"/>
+      <c r="A204" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>597</v>
+      </c>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
       <c r="F204" s="3"/>
@@ -7613,9 +7737,15 @@
       <c r="W204" s="3"/>
     </row>
     <row r="205" ht="14.25" customHeight="1">
-      <c r="A205" s="4"/>
-      <c r="B205" s="4"/>
-      <c r="C205" s="3"/>
+      <c r="A205" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>600</v>
+      </c>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
       <c r="F205" s="3"/>
@@ -7638,9 +7768,15 @@
       <c r="W205" s="3"/>
     </row>
     <row r="206" ht="14.25" customHeight="1">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
-      <c r="C206" s="3"/>
+      <c r="A206" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>603</v>
+      </c>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
       <c r="F206" s="3"/>
@@ -7663,9 +7799,15 @@
       <c r="W206" s="3"/>
     </row>
     <row r="207" ht="14.25" customHeight="1">
-      <c r="A207" s="4"/>
-      <c r="B207" s="4"/>
-      <c r="C207" s="3"/>
+      <c r="A207" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>606</v>
+      </c>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
       <c r="F207" s="3"/>
@@ -7690,7 +7832,7 @@
     <row r="208" ht="14.25" customHeight="1">
       <c r="A208" s="4"/>
       <c r="B208" s="4"/>
-      <c r="C208" s="3"/>
+      <c r="C208" s="5"/>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
       <c r="F208" s="3"/>
@@ -7715,7 +7857,6 @@
     <row r="209" ht="14.25" customHeight="1">
       <c r="A209" s="4"/>
       <c r="B209" s="4"/>
-      <c r="C209" s="3"/>
       <c r="D209" s="3"/>
       <c r="E209" s="3"/>
       <c r="F209" s="3"/>
@@ -7740,7 +7881,6 @@
     <row r="210" ht="14.25" customHeight="1">
       <c r="A210" s="4"/>
       <c r="B210" s="4"/>
-      <c r="C210" s="3"/>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
@@ -7790,7 +7930,6 @@
     <row r="212" ht="14.25" customHeight="1">
       <c r="A212" s="4"/>
       <c r="B212" s="4"/>
-      <c r="C212" s="3"/>
       <c r="D212" s="3"/>
       <c r="E212" s="3"/>
       <c r="F212" s="3"/>

</xml_diff>

<commit_message>
Tutorial and localization update
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="652">
   <si>
     <t>Key</t>
   </si>
@@ -2012,13 +2012,13 @@
     <t>IMPACT_MANAGER_OPINION_MUCH_BETTER</t>
   </si>
   <si>
+    <t>{0} now likes working under you a lot more.</t>
+  </si>
+  <si>
+    <t>IMPACT_MANAGER_OPINION_MUCH_WORSE</t>
+  </si>
+  <si>
     <t>{0} now dislikes working under you a lot more.</t>
-  </si>
-  <si>
-    <t>IMPACT_MANAGER_OPINION_MUCH_WORSE</t>
-  </si>
-  <si>
-    <t>{0} now likes working under you a lot more.</t>
   </si>
   <si>
     <t>IMPACT_REVEAL_TWO_SKILLS</t>
@@ -2071,6 +2071,18 @@
   </si>
   <si>
     <t>As a result of that conversation...</t>
+  </si>
+  <si>
+    <t>RESTART</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>Continue</t>
   </si>
 </sst>
 </file>
@@ -8545,8 +8557,15 @@
       <c r="W226" s="3"/>
     </row>
     <row r="227" ht="14.25" customHeight="1">
-      <c r="B227" s="4"/>
-      <c r="C227" s="3"/>
+      <c r="A227" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="C227" s="10" t="s">
+        <v>609</v>
+      </c>
       <c r="D227" s="3"/>
       <c r="E227" s="3"/>
       <c r="F227" s="3"/>
@@ -8569,8 +8588,15 @@
       <c r="W227" s="3"/>
     </row>
     <row r="228" ht="14.25" customHeight="1">
-      <c r="B228" s="4"/>
-      <c r="C228" s="3"/>
+      <c r="A228" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="C228" s="10" t="s">
+        <v>609</v>
+      </c>
       <c r="D228" s="3"/>
       <c r="E228" s="3"/>
       <c r="F228" s="3"/>

</xml_diff>

<commit_message>
Feedback video bug fixing, latest text for learning pills, episodes and UI
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="656">
   <si>
     <t>Key</t>
   </si>
@@ -57,7 +57,8 @@
   <si>
     <t>La persona tralascia i propri interessi per soddisfare quelli altrui. Questa modalità implica un aspetto di autosacrificio. L’individuo che esercita questo stile può risultare generoso o altruista, obbediente alle richieste altrui anche quando non è d’accordo, oppure si arrende al punto di vista dell’altro. 
 Uso appropriato:
-quando l’altra parte è l’esperto o ha una soluzione migliore. Può essere efficace anche nel preservare relazioni future con l’altra parte.</t>
+quando l’altra parte è l’esperto o ha una soluzione migliore. Può essere efficace anche nel preservare relazioni future con l’altra parte.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>ACCOMMODATING_QUESTIONS_HIGH</t>
@@ -156,7 +157,8 @@
 Quando il problema non è molto importante, quando ci sono altri problemi più importanti da affrontare o quando non si ha nessuna possibilità di vincere;
 Può essere efficace anche quando il problema sarebbe molto costoso da affrontare (il costo è molto più alto dei vantaggi) o quando il clima è emotivamente carico tanto da richiedere un certo spazio;
 Quando altri sono in grado di risolvere il conflitto in modo più efficace. 
-A volte i problemi si risolvono da soli, ma la speranza non è una strategia, e soprattutto l’evitamento non è una buona strategia nel lungo periodo.</t>
+A volte i problemi si risolvono da soli, ma la speranza non è una strategia, e soprattutto l’evitamento non è una buona strategia nel lungo periodo.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>AVOIDING_QUESTIONS_HIGH</t>
@@ -287,10 +289,11 @@
 In complex situations when you need to find a new and innovative solution. This may involve a redefinition of the problem bringing out everyone's ideas. It requires a high level of confidence, a lot of time and effort to convince all and synthesize ideas.</t>
   </si>
   <si>
-    <t xml:space="preserve">L’individuo cerca di cooperare con l’altro per trovare una soluzione che possa soddisfare i bisogni di entrambe le parti. Implica l’approfondimento del problema al fine di identificare le questioni sottostanti percepite dalle parti in gioco e trovare un’ alternativa in grado di soddisfare i bisogni di entrambe.
+    <t>L’individuo cerca di cooperare con l’altro per trovare una soluzione che possa soddisfare i bisogni di entrambe le parti. Implica l’approfondimento del problema al fine di identificare le questioni sottostanti percepite dalle parti in gioco e trovare un’ alternativa in grado di soddisfare i bisogni di entrambe.
 La collaborazione tra due individui può assumere la forma di esplorazione del disaccordo in un tentativo d’imparare l’uno dall’altro, di risoluzione di una condizione specifica altrimenti suscettibile di causare una competizione per le risorse, oppure di confronto e ricerca di una soluzione creativa di un problema interpersonale. 
 Uso appropriato:
-In situazioni complesse quando è necessario trovare una soluzione nuova o innovativa. Questo può implicare una ridefinizione del problema facendo emergere le idee di tutti. Richiede alto livello di fiducia, molto tempo e sforzo per convincere tutti e sintetizzare le idee. </t>
+In situazioni complesse quando è necessario trovare una soluzione nuova o innovativa. Questo può implicare una ridefinizione del problema facendo emergere le idee di tutti. Richiede alto livello di fiducia, molto tempo e sforzo per convincere tutti e sintetizzare le idee. 
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>COLLABORATING_QUESTIONS_HIGH</t>
@@ -332,9 +335,10 @@
 In emergency situations when you need to take a decisive decision quickly and other people are aware of this and thus approve the adoption of this style.</t>
   </si>
   <si>
-    <t xml:space="preserve">La persona è orientata a perseguire i propri interessi a spese dell’altro usando qualsiasi forma di potere per ottenere ciò che desidera: difendere i propri diritti, difendere una posizione che si ritiene corretta o semplicemente mettere in atto il tentativo di vincere o prevalere sull’altro. 
+    <t>La persona è orientata a perseguire i propri interessi a spese dell’altro usando qualsiasi forma di potere per ottenere ciò che desidera: difendere i propri diritti, difendere una posizione che si ritiene corretta o semplicemente mettere in atto il tentativo di vincere o prevalere sull’altro. 
 Uso appropriato:
-In situazioni di emergenza, quando è necessario prendere una decisione decisiva in tempi rapidi e le altre persone sono consapevoli di questo, approvando l’adozione di questo stile. </t>
+In situazioni di emergenza, quando è necessario prendere una decisione decisiva in tempi rapidi e le altre persone sono consapevoli di questo, approvando l’adozione di questo stile. 
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>COMPETING_QUESTIONS_HIGH</t>
@@ -378,7 +382,8 @@
   <si>
     <t>La persona cerca di giungere a un compromesso, l’obiettivo è quello di trovare un espediente, una soluzione reciprocamente accettabile che soddisfi parzialmente i bisogni di entrambe le parti. La ricerca di un compromesso rappresenta una via di mezzo tra la competizione e l’accomodamento, nel senso che si rinuncia un po’ di più rispetto a quando si compete, ma meno rispetto a quando si adotta un comportamento accomodante. Parimenti, il problema viene affrontato in modo più diretto rispetto all’elusione, ma non si arriva ad approfondirlo come con la collaborazione. Il compromesso può significare trovare un accordo a metà strada, fare delle concessioni reciproche oppure cercare una soluzione che rappresenti una via di mezzo. 
 Uso appropriato:
-Quando serve una soluzione temporanea o quando entrambe le parti hanno obiettivi parimenti importanti. La trappola è cadere nel compromesso come facile via di uscita quando in realtà la collaborazione produrrebbe una soluzione migliore.</t>
+Quando serve una soluzione temporanea o quando entrambe le parti hanno obiettivi parimenti importanti. La trappola è cadere nel compromesso come facile via di uscita quando in realtà la collaborazione produrrebbe una soluzione migliore.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>COMPROMISING_QUESTIONS_HIGH</t>
@@ -654,8 +659,11 @@
 In order to be able to interpret your profile, we point you to the style with the highest percentage (which represents you the most) and the lowest percentage (which represents you less). Next to these two styles, you will see some reflection questions that may be helpful.</t>
   </si>
   <si>
-    <t>Di seguito ti vengono presentati i diversi stili di gestione del conflitto secondo il modello di Thomas-Kilmann. Le percentuali indicano quanto hai adottato ognuno di questi stili durante il gioco. 
-Per poter interpretare il tuo profilo ti indichiamo di soffermarti sullo stile con la percentuale più alta (che ti rappresenta di più) e su quello con la percentuale più bassa (che ti rappresenta di meno). In corrispondenza di questi due stili ti compariranno alcune domande di riflessione che potranno esserti utili in termini di approfondimento.</t>
+    <t>Durante il gioco ti sei trovato a gestire delle situazioni di conflitto.
+Nel grafico vengono riportate le percentuali che indicano a quali stili di gestione del conflitto le tue scelte fanno riferimento (il modello che abbiamo adottato è quello di Thomas-Kilmann).
+Come punto di partenza inizia a scoprire qual è lo stile con la percentuale più alta, quello che corrisponde alla frequenza maggiore delle tue scelte.
+Cerca di scoprire se ti rappresenta, in quali situazioni è più adeguato e in quali casi è sconsigliato.
+Se ti interessa, hai anche la possibilità di scoprire gli altri stili, e individuare in quali situazioni potrebbe essere vantaggioso adottarli.</t>
   </si>
   <si>
     <t>GREEN_PLACEMENT</t>
@@ -769,7 +777,8 @@
     <t>Questo stile si caratterizza per:
 Uno scambio contenuto con il gruppo e una relativa attenzione alla crescita dei singoli;
 La rinuncia alla responsabilità, il rinviare la decisione, il non restituire feedback;
-L’operare il minimo sforzo per soddisfare i bisogni dei collaboratori.</t>
+L’operare il minimo sforzo per soddisfare i bisogni dei collaboratori.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>LANGUAGE</t>
@@ -1584,7 +1593,7 @@
     <t>Are you sure you want to use the same crew line-up as the previous race?</t>
   </si>
   <si>
-    <t>Sei sicuro di voler utilizzare la stessa formazione anche per la prossima gara?</t>
+    <t>Sei sicuro di voler utilizzare la stessa squadra della gara precedente?</t>
   </si>
   <si>
     <t>REQUIRED</t>
@@ -1764,7 +1773,8 @@
     <t>Questo stile si basa sulla negoziazione e lo scambio tra il leader e il gruppo, in funzione del raggiungimento degli obiettivi.
 Le principali caratteristiche sono:
 La propensione a riconoscere i ruoli e chiarire le richieste dei compiti;
-La capacità di riconoscere e rinforzare i comportamenti e i risultati adeguati.</t>
+La capacità di riconoscere e rinforzare i comportamenti e i risultati adeguati.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>TRANSFORMATIONAL</t>
@@ -1792,7 +1802,8 @@
 È proteso all’ascolto ed è interessato a emozioni, valori, morale, qualità individuali. 
 Presta attenzione alla crescita e ai bisogni degli altri, stimolandoli ad essere creativi e innovativi. 
 È un modello di riferimento e dà il buon esempio.
-Ha la capacità di adattarsi alle situazioni e ai contesti.</t>
+Ha la capacità di adattarsi alle situazioni e ai contesti.
+Guarda il video per vedere questo stile in azione.</t>
   </si>
   <si>
     <t>TRIMMER</t>
@@ -2083,6 +2094,18 @@
   </si>
   <si>
     <t>Continue</t>
+  </si>
+  <si>
+    <t>VIDEO</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>Close</t>
   </si>
 </sst>
 </file>
@@ -2154,6 +2177,9 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2161,9 +2187,6 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -2204,7 +2227,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="49.14"/>
     <col customWidth="1" min="2" max="2" width="73.86"/>
-    <col customWidth="1" min="3" max="3" width="66.14"/>
+    <col customWidth="1" min="3" max="3" width="71.0"/>
     <col customWidth="1" min="4" max="4" width="29.71"/>
     <col customWidth="1" min="5" max="23" width="8.71"/>
   </cols>
@@ -2271,7 +2294,7 @@
       <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3"/>
@@ -2295,7 +2318,7 @@
       <c r="W3" s="3"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2325,7 +2348,7 @@
       <c r="W4" s="3"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2529,7 +2552,7 @@
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="3"/>
@@ -2553,7 +2576,7 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2583,7 +2606,7 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -2673,7 +2696,7 @@
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>50</v>
       </c>
       <c r="H17" s="4"/>
@@ -2802,7 +2825,7 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2835,7 +2858,7 @@
       <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>68</v>
       </c>
       <c r="H23" s="4"/>
@@ -2862,7 +2885,7 @@
       <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
       <c r="H24" s="3"/>
@@ -2916,7 +2939,7 @@
       <c r="B26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E26" s="3"/>
@@ -2940,7 +2963,7 @@
       <c r="W26" s="3"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -2970,7 +2993,7 @@
       <c r="W27" s="3"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -3033,7 +3056,7 @@
       <c r="B30" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="7" t="s">
         <v>89</v>
       </c>
       <c r="E30" s="3"/>
@@ -3057,7 +3080,7 @@
       <c r="W30" s="3"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -3087,7 +3110,7 @@
       <c r="W31" s="3"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -3150,7 +3173,7 @@
       <c r="B34" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E34" s="3"/>
@@ -3174,7 +3197,7 @@
       <c r="W34" s="3"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>102</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -3204,7 +3227,7 @@
       <c r="W35" s="3"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>105</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -3240,7 +3263,7 @@
       <c r="B37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="7" t="s">
         <v>110</v>
       </c>
       <c r="H37" s="3"/>
@@ -3267,7 +3290,7 @@
       <c r="B38" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="7" t="s">
         <v>113</v>
       </c>
       <c r="E38" s="3"/>
@@ -3752,7 +3775,7 @@
       <c r="B55" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="7" t="s">
         <v>161</v>
       </c>
       <c r="H55" s="3"/>
@@ -3779,7 +3802,7 @@
       <c r="B56" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="7" t="s">
         <v>164</v>
       </c>
       <c r="E56" s="3"/>
@@ -4360,7 +4383,7 @@
       <c r="B77" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="7" t="s">
         <v>224</v>
       </c>
       <c r="E77" s="3"/>
@@ -4471,7 +4494,7 @@
       <c r="B81" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="7" t="s">
         <v>236</v>
       </c>
       <c r="E81" s="3"/>
@@ -4886,7 +4909,7 @@
       <c r="B96" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="7" t="s">
         <v>281</v>
       </c>
       <c r="H96" s="4"/>
@@ -4967,7 +4990,7 @@
       <c r="B99" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C99" s="7" t="s">
         <v>290</v>
       </c>
       <c r="H99" s="4"/>
@@ -5075,7 +5098,7 @@
       <c r="B103" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C103" s="10" t="s">
+      <c r="C103" s="7" t="s">
         <v>302</v>
       </c>
       <c r="H103" s="3"/>
@@ -5681,7 +5704,7 @@
       <c r="B125" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C125" s="10" t="s">
+      <c r="C125" s="7" t="s">
         <v>366</v>
       </c>
       <c r="H125" s="4"/>
@@ -5708,7 +5731,7 @@
       <c r="B126" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C126" s="10" t="s">
+      <c r="C126" s="7" t="s">
         <v>369</v>
       </c>
       <c r="H126" s="4"/>
@@ -5735,7 +5758,7 @@
       <c r="B127" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C127" s="10" t="s">
+      <c r="C127" s="7" t="s">
         <v>372</v>
       </c>
       <c r="H127" s="4"/>
@@ -5762,7 +5785,7 @@
       <c r="B128" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C128" s="7" t="s">
         <v>375</v>
       </c>
       <c r="H128" s="4"/>
@@ -5789,7 +5812,7 @@
       <c r="B129" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C129" s="10" t="s">
+      <c r="C129" s="7" t="s">
         <v>378</v>
       </c>
       <c r="H129" s="4"/>
@@ -5816,7 +5839,7 @@
       <c r="B130" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C130" s="10" t="s">
+      <c r="C130" s="7" t="s">
         <v>381</v>
       </c>
       <c r="H130" s="4"/>
@@ -5843,7 +5866,7 @@
       <c r="B131" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C131" s="10" t="s">
+      <c r="C131" s="7" t="s">
         <v>384</v>
       </c>
       <c r="H131" s="4"/>
@@ -5870,7 +5893,7 @@
       <c r="B132" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C132" s="10" t="s">
+      <c r="C132" s="7" t="s">
         <v>387</v>
       </c>
       <c r="H132" s="4"/>
@@ -5897,7 +5920,7 @@
       <c r="B133" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="C133" s="10" t="s">
+      <c r="C133" s="7" t="s">
         <v>390</v>
       </c>
       <c r="H133" s="4"/>
@@ -5924,7 +5947,7 @@
       <c r="B134" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C134" s="10" t="s">
+      <c r="C134" s="7" t="s">
         <v>393</v>
       </c>
       <c r="H134" s="4"/>
@@ -6373,7 +6396,7 @@
       <c r="B150" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C150" s="10" t="s">
+      <c r="C150" s="7" t="s">
         <v>441</v>
       </c>
       <c r="H150" s="4"/>
@@ -6400,7 +6423,7 @@
       <c r="B151" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C151" s="10" t="s">
+      <c r="C151" s="7" t="s">
         <v>444</v>
       </c>
       <c r="H151" s="4"/>
@@ -6512,7 +6535,7 @@
       <c r="B155" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C155" s="10" t="s">
+      <c r="C155" s="7" t="s">
         <v>441</v>
       </c>
       <c r="H155" s="4"/>
@@ -6867,7 +6890,7 @@
       <c r="B168" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C168" s="7" t="s">
         <v>491</v>
       </c>
       <c r="H168" s="4"/>
@@ -6948,7 +6971,7 @@
       <c r="B171" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="C171" s="10" t="s">
+      <c r="C171" s="7" t="s">
         <v>500</v>
       </c>
       <c r="H171" s="4"/>
@@ -7410,7 +7433,7 @@
       <c r="B188" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="C188" s="5" t="s">
+      <c r="C188" s="7" t="s">
         <v>549</v>
       </c>
       <c r="E188" s="3"/>
@@ -7440,7 +7463,7 @@
       <c r="B189" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C189" s="10" t="s">
+      <c r="C189" s="7" t="s">
         <v>552</v>
       </c>
       <c r="H189" s="3"/>
@@ -7467,7 +7490,7 @@
       <c r="B190" s="6" t="s">
         <v>554</v>
       </c>
-      <c r="C190" s="5" t="s">
+      <c r="C190" s="7" t="s">
         <v>555</v>
       </c>
       <c r="E190" s="3"/>
@@ -7758,7 +7781,7 @@
       <c r="B200" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="C200" s="10" t="s">
+      <c r="C200" s="7" t="s">
         <v>585</v>
       </c>
       <c r="H200" s="4"/>
@@ -7974,7 +7997,7 @@
       <c r="B208" s="6" t="s">
         <v>608</v>
       </c>
-      <c r="C208" s="10" t="s">
+      <c r="C208" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D208" s="3"/>
@@ -8002,10 +8025,10 @@
       <c r="A209" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="B209" s="10" t="s">
+      <c r="B209" s="7" t="s">
         <v>611</v>
       </c>
-      <c r="C209" s="10" t="s">
+      <c r="C209" s="7" t="s">
         <v>612</v>
       </c>
       <c r="D209" s="3"/>
@@ -8033,10 +8056,10 @@
       <c r="A210" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="B210" s="9" t="s">
+      <c r="B210" s="10" t="s">
         <v>614</v>
       </c>
-      <c r="C210" s="9" t="s">
+      <c r="C210" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D210" s="3"/>
@@ -8064,10 +8087,10 @@
       <c r="A211" s="6" t="s">
         <v>615</v>
       </c>
-      <c r="B211" s="9" t="s">
+      <c r="B211" s="10" t="s">
         <v>616</v>
       </c>
-      <c r="C211" s="9" t="s">
+      <c r="C211" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D211" s="3"/>
@@ -8095,10 +8118,10 @@
       <c r="A212" s="6" t="s">
         <v>617</v>
       </c>
-      <c r="B212" s="9" t="s">
+      <c r="B212" s="10" t="s">
         <v>618</v>
       </c>
-      <c r="C212" s="9" t="s">
+      <c r="C212" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D212" s="3"/>
@@ -8126,10 +8149,10 @@
       <c r="A213" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="B213" s="9" t="s">
+      <c r="B213" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="C213" s="9" t="s">
+      <c r="C213" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D213" s="3"/>
@@ -8157,10 +8180,10 @@
       <c r="A214" s="6" t="s">
         <v>621</v>
       </c>
-      <c r="B214" s="10" t="s">
+      <c r="B214" s="7" t="s">
         <v>622</v>
       </c>
-      <c r="C214" s="10" t="s">
+      <c r="C214" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D214" s="3"/>
@@ -8188,10 +8211,10 @@
       <c r="A215" s="6" t="s">
         <v>623</v>
       </c>
-      <c r="B215" s="9" t="s">
+      <c r="B215" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="C215" s="9" t="s">
+      <c r="C215" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D215" s="3"/>
@@ -8219,10 +8242,10 @@
       <c r="A216" s="6" t="s">
         <v>625</v>
       </c>
-      <c r="B216" s="10" t="s">
+      <c r="B216" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="C216" s="10" t="s">
+      <c r="C216" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D216" s="3"/>
@@ -8250,10 +8273,10 @@
       <c r="A217" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="B217" s="9" t="s">
+      <c r="B217" s="10" t="s">
         <v>628</v>
       </c>
-      <c r="C217" s="9" t="s">
+      <c r="C217" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D217" s="3"/>
@@ -8281,10 +8304,10 @@
       <c r="A218" s="6" t="s">
         <v>629</v>
       </c>
-      <c r="B218" s="9" t="s">
+      <c r="B218" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="C218" s="9" t="s">
+      <c r="C218" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D218" s="3"/>
@@ -8312,10 +8335,10 @@
       <c r="A219" s="6" t="s">
         <v>631</v>
       </c>
-      <c r="B219" s="9" t="s">
+      <c r="B219" s="10" t="s">
         <v>632</v>
       </c>
-      <c r="C219" s="9" t="s">
+      <c r="C219" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D219" s="3"/>
@@ -8343,10 +8366,10 @@
       <c r="A220" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="B220" s="9" t="s">
+      <c r="B220" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="C220" s="9" t="s">
+      <c r="C220" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D220" s="3"/>
@@ -8374,10 +8397,10 @@
       <c r="A221" s="6" t="s">
         <v>635</v>
       </c>
-      <c r="B221" s="9" t="s">
+      <c r="B221" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="C221" s="9" t="s">
+      <c r="C221" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D221" s="3"/>
@@ -8405,10 +8428,10 @@
       <c r="A222" s="6" t="s">
         <v>637</v>
       </c>
-      <c r="B222" s="9" t="s">
+      <c r="B222" s="10" t="s">
         <v>638</v>
       </c>
-      <c r="C222" s="9" t="s">
+      <c r="C222" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D222" s="3"/>
@@ -8436,10 +8459,10 @@
       <c r="A223" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="B223" s="9" t="s">
+      <c r="B223" s="10" t="s">
         <v>640</v>
       </c>
-      <c r="C223" s="9" t="s">
+      <c r="C223" s="10" t="s">
         <v>612</v>
       </c>
       <c r="D223" s="3"/>
@@ -8467,10 +8490,10 @@
       <c r="A224" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B224" s="10" t="s">
+      <c r="B224" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="C224" s="10" t="s">
+      <c r="C224" s="7" t="s">
         <v>643</v>
       </c>
       <c r="D224" s="3"/>
@@ -8498,10 +8521,10 @@
       <c r="A225" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B225" s="10" t="s">
+      <c r="B225" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="C225" s="10" t="s">
+      <c r="C225" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D225" s="3"/>
@@ -8532,7 +8555,7 @@
       <c r="B226" s="6" t="s">
         <v>647</v>
       </c>
-      <c r="C226" s="10" t="s">
+      <c r="C226" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D226" s="3"/>
@@ -8563,7 +8586,7 @@
       <c r="B227" s="6" t="s">
         <v>649</v>
       </c>
-      <c r="C227" s="10" t="s">
+      <c r="C227" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D227" s="3"/>
@@ -8594,7 +8617,7 @@
       <c r="B228" s="6" t="s">
         <v>651</v>
       </c>
-      <c r="C228" s="10" t="s">
+      <c r="C228" s="7" t="s">
         <v>609</v>
       </c>
       <c r="D228" s="3"/>
@@ -8619,9 +8642,15 @@
       <c r="W228" s="3"/>
     </row>
     <row r="229" ht="14.25" customHeight="1">
-      <c r="A229" s="4"/>
-      <c r="B229" s="4"/>
-      <c r="C229" s="3"/>
+      <c r="A229" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>653</v>
+      </c>
       <c r="D229" s="3"/>
       <c r="E229" s="3"/>
       <c r="F229" s="3"/>
@@ -8644,9 +8673,15 @@
       <c r="W229" s="3"/>
     </row>
     <row r="230" ht="14.25" customHeight="1">
-      <c r="A230" s="4"/>
-      <c r="B230" s="4"/>
-      <c r="C230" s="3"/>
+      <c r="A230" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>609</v>
+      </c>
       <c r="D230" s="3"/>
       <c r="E230" s="3"/>
       <c r="F230" s="3"/>

</xml_diff>

<commit_message>
Minor logic code changes. Transform extensions added in an attempt to heavily tidy code.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Resources/Localization/Sports Team Manager Localization.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="670">
   <si>
     <t>Key</t>
   </si>
@@ -909,7 +909,7 @@
     <t>MANAGER_OPINION</t>
   </si>
   <si>
-    <t>Manager Opinion</t>
+    <t>Opinion of you</t>
   </si>
   <si>
     <t>Opinione del coach</t>
@@ -2230,14 +2230,14 @@
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
@@ -4809,7 +4809,7 @@
       <c r="A91" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="7" t="s">
         <v>265</v>
       </c>
       <c r="C91" s="5" t="s">
@@ -5005,7 +5005,7 @@
       <c r="B98" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C98" s="12" t="s">
+      <c r="C98" s="11" t="s">
         <v>287</v>
       </c>
       <c r="H98" s="4"/>
@@ -5113,7 +5113,7 @@
       <c r="B102" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="12" t="s">
         <v>299</v>
       </c>
       <c r="H102" s="4"/>
@@ -5611,7 +5611,7 @@
       <c r="B120" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="13" t="s">
         <v>351</v>
       </c>
       <c r="H120" s="4"/>
@@ -5638,7 +5638,7 @@
       <c r="B121" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C121" s="11" t="s">
+      <c r="C121" s="13" t="s">
         <v>354</v>
       </c>
       <c r="H121" s="4"/>
@@ -6104,7 +6104,7 @@
       <c r="B138" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C138" s="13" t="s">
+      <c r="C138" s="12" t="s">
         <v>405</v>
       </c>
       <c r="H138" s="4"/>
@@ -8963,15 +8963,9 @@
       <c r="W237" s="3"/>
     </row>
     <row r="238" ht="14.25" customHeight="1">
-      <c r="A238" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>609</v>
-      </c>
+      <c r="A238" s="4"/>
+      <c r="B238" s="4"/>
+      <c r="C238" s="3"/>
       <c r="D238" s="3"/>
       <c r="E238" s="3"/>
       <c r="F238" s="3"/>
@@ -28018,31 +28012,6 @@
       <c r="V999" s="3"/>
       <c r="W999" s="3"/>
     </row>
-    <row r="1000" ht="14.25" customHeight="1">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="4"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="3"/>
-      <c r="J1000" s="3"/>
-      <c r="K1000" s="3"/>
-      <c r="L1000" s="3"/>
-      <c r="M1000" s="3"/>
-      <c r="N1000" s="3"/>
-      <c r="O1000" s="3"/>
-      <c r="P1000" s="3"/>
-      <c r="Q1000" s="3"/>
-      <c r="R1000" s="3"/>
-      <c r="S1000" s="3"/>
-      <c r="T1000" s="3"/>
-      <c r="U1000" s="3"/>
-      <c r="V1000" s="3"/>
-      <c r="W1000" s="3"/>
-    </row>
   </sheetData>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>